<commit_message>
add some CV doc
</commit_message>
<xml_diff>
--- a/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
+++ b/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
@@ -4,13 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="2014_Thang6" sheetId="1" r:id="rId1"/>
     <sheet name="2014_Thang7" sheetId="5" r:id="rId2"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="2014_Thang8" sheetId="6" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -464,8 +463,232 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SONY Y2</author>
+    <author>HinhND</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thuybt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- Lập đầu tuần (hàng tuần)
+- Các công việc được chia theo nhóm công việc/khách hàng/dự án cụ thể
+- Chi tiết các bước thực hiện cho 1 công việc cụ thể
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thuybt:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Các tuần không thực hiện có thể Hide đi và chỉ đẻ các tuần đang tác nghiệp
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thuybt:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>- Thực hiện khi lập BC hàng tuần
+- Ghi chú đề xuất (nếu có)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+Kết quả thực tế đạt được có thể là tài liệu, source code, bản thiết kế, cuộc họp, kế hoạch,...</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Kết quả cần đưa vào khi thực hiện lập kế hoạch
+-Các đầu việc cần được chia nhỏ đủ để hoàn thành trong vòng 1 tuần
+-Kết quả cần cụ thể, đo lường được là tài liệu, sourcecode
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Thời gian thực hiện công việc đủ trong 1 tuần</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Đánh giá kết quả thực hiện so với kế hoạch
+-Đạt bao nhiêu % 
+-Kết luận đạt hay không đạt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Nếu không đạt kế hoạch thì nguyên nhân do đâu?
+-Đề xuất cách thực hiện, giải pháp nâng cao chất lượng</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="143">
   <si>
     <t>TT</t>
   </si>
@@ -821,6 +1044,81 @@
   </si>
   <si>
     <t>25/07/2014</t>
+  </si>
+  <si>
+    <t>Hiện tại Comverse vẫn đang chưa hỗ trợ để có thể Full Luồng</t>
+  </si>
+  <si>
+    <t>Hướng dẫn nhân viên mới</t>
+  </si>
+  <si>
+    <t>Hướng dẫn Đạo tuân thủ Code Convention, ...</t>
+  </si>
+  <si>
+    <t>04/08/2014</t>
+  </si>
+  <si>
+    <t>Đánh giá công việc</t>
+  </si>
+  <si>
+    <t>Các công việc phát sinh trong quá trình phát triển eOneRate</t>
+  </si>
+  <si>
+    <t>Dựng hệ thống, phát triển trực tiếp trên hệ thống VNP C1</t>
+  </si>
+  <si>
+    <t>30/08/2014</t>
+  </si>
+  <si>
+    <t>Tìm hiểu chức năng WorkFlow trong BigData</t>
+  </si>
+  <si>
+    <t>09/08/2014</t>
+  </si>
+  <si>
+    <t>Tìm hiểu cách Input, output Serialization Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đang tiếp tục tìm hiểu </t>
+  </si>
+  <si>
+    <t>Cover Hadoop Workflow</t>
+  </si>
+  <si>
+    <t>16/08/2014</t>
+  </si>
+  <si>
+    <t>ETL: Data Cleansing</t>
+  </si>
+  <si>
+    <t>Hoàn thành các công việc phát sinh</t>
+  </si>
+  <si>
+    <t>Tuần này chưa qua VNP làm việc</t>
+  </si>
+  <si>
+    <t>Nghiên cứu, cover nội dung Ảo hóa</t>
+  </si>
+  <si>
+    <t>Cover vmWare Sphere, Hypervisor, vMotion</t>
+  </si>
+  <si>
+    <t>Tham gia khóa học Robusta Virtualization Fundamental</t>
+  </si>
+  <si>
+    <t>Đã nắm được 100%</t>
+  </si>
+  <si>
+    <t>VMS Oracle Private Cloud</t>
+  </si>
+  <si>
+    <t>Dựng hệ thống Oracle Private Cloud tại ELCOM</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Cloud</t>
+  </si>
+  <si>
+    <t>Nghiên cứu Oracle Private Cloud</t>
   </si>
 </sst>
 </file>
@@ -1043,7 +1341,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="54">
+  <borders count="55">
     <border>
       <left/>
       <right/>
@@ -1704,11 +2002,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="hair">
+        <color auto="1"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2032,6 +2345,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="33" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="8" borderId="33" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2115,6 +2437,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2204,6 +2529,79 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1134927</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="ELCOM_LOGO_136x60pcs"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="85724" y="28575"/>
+          <a:ext cx="1382578" cy="412377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -2704,10 +3102,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="121"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -2773,163 +3171,163 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="131" t="s">
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132"/>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="146" t="s">
+      <c r="AC6" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="125" t="s">
+      <c r="AD6" s="128" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="140" t="s">
+      <c r="A7" s="126"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="143" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="143" t="s">
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="140" t="s">
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="143" t="s">
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="145"/>
+      <c r="R7" s="146" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="140" t="s">
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="147"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="142"/>
-      <c r="AB7" s="132"/>
-      <c r="AC7" s="147"/>
-      <c r="AD7" s="126"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="144"/>
+      <c r="Z7" s="144"/>
+      <c r="AA7" s="145"/>
+      <c r="AB7" s="135"/>
+      <c r="AC7" s="150"/>
+      <c r="AD7" s="129"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="136" t="s">
+      <c r="A8" s="126"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="134" t="s">
+      <c r="D8" s="140"/>
+      <c r="E8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="136" t="s">
+      <c r="G8" s="142"/>
+      <c r="H8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="137"/>
-      <c r="J8" s="134" t="s">
+      <c r="I8" s="140"/>
+      <c r="J8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="138" t="s">
+      <c r="K8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="139"/>
-      <c r="M8" s="136" t="s">
+      <c r="L8" s="142"/>
+      <c r="M8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="137"/>
-      <c r="O8" s="134" t="s">
+      <c r="N8" s="140"/>
+      <c r="O8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="138" t="s">
+      <c r="P8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="139"/>
-      <c r="R8" s="136" t="s">
+      <c r="Q8" s="142"/>
+      <c r="R8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="137"/>
-      <c r="T8" s="134" t="s">
+      <c r="S8" s="140"/>
+      <c r="T8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="138" t="s">
+      <c r="U8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="139"/>
-      <c r="W8" s="136" t="s">
+      <c r="V8" s="142"/>
+      <c r="W8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="X8" s="137"/>
-      <c r="Y8" s="134" t="s">
+      <c r="X8" s="140"/>
+      <c r="Y8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="138" t="s">
+      <c r="Z8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="139"/>
-      <c r="AB8" s="132"/>
-      <c r="AC8" s="147"/>
-      <c r="AD8" s="126"/>
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="135"/>
+      <c r="AC8" s="150"/>
+      <c r="AD8" s="129"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="127"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="135"/>
+      <c r="E9" s="138"/>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2942,7 +3340,7 @@
       <c r="I9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="135"/>
+      <c r="J9" s="138"/>
       <c r="K9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2955,7 +3353,7 @@
       <c r="N9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="135"/>
+      <c r="O9" s="138"/>
       <c r="P9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2968,7 +3366,7 @@
       <c r="S9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="T9" s="135"/>
+      <c r="T9" s="138"/>
       <c r="U9" s="2" t="s">
         <v>25</v>
       </c>
@@ -2981,16 +3379,16 @@
       <c r="X9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Y9" s="135"/>
+      <c r="Y9" s="138"/>
       <c r="Z9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="133"/>
-      <c r="AC9" s="148"/>
-      <c r="AD9" s="127"/>
+      <c r="AB9" s="136"/>
+      <c r="AC9" s="151"/>
+      <c r="AD9" s="130"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -5263,8 +5661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M15" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView topLeftCell="O33" workbookViewId="0">
+      <selection activeCell="R33" sqref="R33:T37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5402,10 +5800,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="124" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="121"/>
+      <c r="B4" s="124"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -5471,163 +5869,163 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="128" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="131" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="131" t="s">
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132"/>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="134" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="146" t="s">
+      <c r="AC6" s="149" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="125" t="s">
+      <c r="AD6" s="128" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="140" t="s">
+      <c r="A7" s="126"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="143" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="143" t="s">
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="146" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="140" t="s">
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="143" t="s">
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="145"/>
+      <c r="R7" s="146" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="140" t="s">
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="147"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="143" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="142"/>
-      <c r="AB7" s="132"/>
-      <c r="AC7" s="147"/>
-      <c r="AD7" s="126"/>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="144"/>
+      <c r="Z7" s="144"/>
+      <c r="AA7" s="145"/>
+      <c r="AB7" s="135"/>
+      <c r="AC7" s="150"/>
+      <c r="AD7" s="129"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
-      <c r="C8" s="136" t="s">
+      <c r="A8" s="126"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="137"/>
-      <c r="E8" s="134" t="s">
+      <c r="D8" s="140"/>
+      <c r="E8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="139"/>
-      <c r="H8" s="136" t="s">
+      <c r="G8" s="142"/>
+      <c r="H8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="137"/>
-      <c r="J8" s="134" t="s">
+      <c r="I8" s="140"/>
+      <c r="J8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="138" t="s">
+      <c r="K8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="139"/>
-      <c r="M8" s="136" t="s">
+      <c r="L8" s="142"/>
+      <c r="M8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="N8" s="137"/>
-      <c r="O8" s="134" t="s">
+      <c r="N8" s="140"/>
+      <c r="O8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="138" t="s">
+      <c r="P8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="139"/>
-      <c r="R8" s="136" t="s">
+      <c r="Q8" s="142"/>
+      <c r="R8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="S8" s="137"/>
-      <c r="T8" s="134" t="s">
+      <c r="S8" s="140"/>
+      <c r="T8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="138" t="s">
+      <c r="U8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="139"/>
-      <c r="W8" s="136" t="s">
+      <c r="V8" s="142"/>
+      <c r="W8" s="139" t="s">
         <v>6</v>
       </c>
-      <c r="X8" s="137"/>
-      <c r="Y8" s="134" t="s">
+      <c r="X8" s="140"/>
+      <c r="Y8" s="137" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="138" t="s">
+      <c r="Z8" s="141" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="139"/>
-      <c r="AB8" s="132"/>
-      <c r="AC8" s="147"/>
-      <c r="AD8" s="126"/>
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="135"/>
+      <c r="AC8" s="150"/>
+      <c r="AD8" s="129"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="127"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="135"/>
+      <c r="E9" s="138"/>
       <c r="F9" s="2" t="s">
         <v>25</v>
       </c>
@@ -5640,7 +6038,7 @@
       <c r="I9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J9" s="135"/>
+      <c r="J9" s="138"/>
       <c r="K9" s="2" t="s">
         <v>25</v>
       </c>
@@ -5653,7 +6051,7 @@
       <c r="N9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="O9" s="135"/>
+      <c r="O9" s="138"/>
       <c r="P9" s="2" t="s">
         <v>25</v>
       </c>
@@ -5666,7 +6064,7 @@
       <c r="S9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="T9" s="135"/>
+      <c r="T9" s="138"/>
       <c r="U9" s="2" t="s">
         <v>25</v>
       </c>
@@ -5679,16 +6077,16 @@
       <c r="X9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="Y9" s="135"/>
+      <c r="Y9" s="138"/>
       <c r="Z9" s="2" t="s">
         <v>25</v>
       </c>
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="133"/>
-      <c r="AC9" s="148"/>
-      <c r="AD9" s="127"/>
+      <c r="AB9" s="136"/>
+      <c r="AC9" s="151"/>
+      <c r="AD9" s="130"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -5938,7 +6336,9 @@
       <c r="S16" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="T16" s="42"/>
+      <c r="T16" s="42" t="s">
+        <v>118</v>
+      </c>
       <c r="U16" s="42"/>
       <c r="V16" s="38"/>
       <c r="W16" s="43"/>
@@ -6086,7 +6486,7 @@
       <c r="AC20" s="45"/>
       <c r="AD20" s="46"/>
     </row>
-    <row r="21" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
       <c r="B21" s="26"/>
       <c r="C21" s="47"/>
@@ -6110,7 +6510,9 @@
       <c r="S21" s="42" t="s">
         <v>117</v>
       </c>
-      <c r="T21" s="42"/>
+      <c r="T21" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="U21" s="42"/>
       <c r="V21" s="38"/>
       <c r="W21" s="43"/>
@@ -6526,7 +6928,9 @@
       <c r="S33" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="T33" s="42"/>
+      <c r="T33" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="U33" s="51"/>
       <c r="V33" s="108"/>
       <c r="W33" s="43"/>
@@ -6570,7 +6974,9 @@
       <c r="S34" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="T34" s="42"/>
+      <c r="T34" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="U34" s="51"/>
       <c r="V34" s="108"/>
       <c r="W34" s="43"/>
@@ -6648,7 +7054,9 @@
       <c r="S36" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="T36" s="42"/>
+      <c r="T36" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="U36" s="51"/>
       <c r="V36" s="108"/>
       <c r="W36" s="43"/>
@@ -6838,7 +7246,9 @@
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
+      <c r="B42" s="26" t="s">
+        <v>119</v>
+      </c>
       <c r="C42" s="47"/>
       <c r="D42" s="51"/>
       <c r="E42" s="67"/>
@@ -6868,7 +7278,7 @@
       <c r="AC42" s="45"/>
       <c r="AD42" s="46"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
       <c r="B43" s="37"/>
       <c r="C43" s="47"/>
@@ -6882,12 +7292,16 @@
       <c r="K43" s="51"/>
       <c r="L43" s="108"/>
       <c r="M43" s="43"/>
-      <c r="N43" s="42"/>
+      <c r="N43" s="101"/>
       <c r="O43" s="42"/>
       <c r="P43" s="51"/>
       <c r="Q43" s="108"/>
-      <c r="R43" s="43"/>
-      <c r="S43" s="42"/>
+      <c r="R43" s="43" t="s">
+        <v>120</v>
+      </c>
+      <c r="S43" s="101" t="s">
+        <v>121</v>
+      </c>
       <c r="T43" s="42"/>
       <c r="U43" s="51"/>
       <c r="V43" s="108"/>
@@ -7444,25 +7858,2257 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="32.42578125" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="19.140625" customWidth="1"/>
+    <col min="16" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="26.140625" customWidth="1"/>
+    <col min="19" max="19" width="10.140625" customWidth="1"/>
+    <col min="20" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="31.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" customWidth="1"/>
+    <col min="26" max="26" width="29.7109375" customWidth="1"/>
+    <col min="27" max="27" width="17.140625" customWidth="1"/>
+    <col min="28" max="29" width="10.140625" customWidth="1"/>
+    <col min="30" max="30" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+    </row>
+    <row r="2" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+    </row>
+    <row r="3" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
+    </row>
+    <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="124" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="124"/>
+      <c r="C4" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="65"/>
+      <c r="AA5" s="65"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="63"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="125" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="128" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="131" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="132"/>
+      <c r="E6" s="132"/>
+      <c r="F6" s="132"/>
+      <c r="G6" s="132"/>
+      <c r="H6" s="132"/>
+      <c r="I6" s="132"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="132"/>
+      <c r="L6" s="132"/>
+      <c r="M6" s="132"/>
+      <c r="N6" s="132"/>
+      <c r="O6" s="132"/>
+      <c r="P6" s="132"/>
+      <c r="Q6" s="132"/>
+      <c r="R6" s="132"/>
+      <c r="S6" s="132"/>
+      <c r="T6" s="132"/>
+      <c r="U6" s="132"/>
+      <c r="V6" s="132"/>
+      <c r="W6" s="132"/>
+      <c r="X6" s="132"/>
+      <c r="Y6" s="132"/>
+      <c r="Z6" s="132"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="134" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="149" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="128" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="126"/>
+      <c r="B7" s="129"/>
+      <c r="C7" s="143" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="145"/>
+      <c r="H7" s="146" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="147"/>
+      <c r="J7" s="147"/>
+      <c r="K7" s="147"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="143" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="144"/>
+      <c r="O7" s="144"/>
+      <c r="P7" s="144"/>
+      <c r="Q7" s="145"/>
+      <c r="R7" s="146" t="s">
+        <v>72</v>
+      </c>
+      <c r="S7" s="147"/>
+      <c r="T7" s="147"/>
+      <c r="U7" s="147"/>
+      <c r="V7" s="147"/>
+      <c r="W7" s="143" t="s">
+        <v>73</v>
+      </c>
+      <c r="X7" s="144"/>
+      <c r="Y7" s="144"/>
+      <c r="Z7" s="144"/>
+      <c r="AA7" s="145"/>
+      <c r="AB7" s="135"/>
+      <c r="AC7" s="150"/>
+      <c r="AD7" s="129"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="126"/>
+      <c r="B8" s="129"/>
+      <c r="C8" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="140"/>
+      <c r="E8" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="142"/>
+      <c r="H8" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="140"/>
+      <c r="J8" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="142"/>
+      <c r="M8" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="140"/>
+      <c r="O8" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="142"/>
+      <c r="R8" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="140"/>
+      <c r="T8" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="V8" s="142"/>
+      <c r="W8" s="139" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="140"/>
+      <c r="Y8" s="137" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="141" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA8" s="142"/>
+      <c r="AB8" s="135"/>
+      <c r="AC8" s="150"/>
+      <c r="AD8" s="129"/>
+    </row>
+    <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="127"/>
+      <c r="B9" s="130"/>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="138"/>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="138"/>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="138"/>
+      <c r="P9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="138"/>
+      <c r="U9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="138"/>
+      <c r="Z9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB9" s="136"/>
+      <c r="AC9" s="151"/>
+      <c r="AD9" s="130"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="99"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="99"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="104"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="99"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="104"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="102"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="103"/>
+      <c r="AA11" s="102"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="24"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>1</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="35"/>
+    </row>
+    <row r="13" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="36"/>
+      <c r="B13" s="118"/>
+      <c r="C13" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="D13" s="42" t="s">
+        <v>125</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="F13" s="42"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="I13" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="J13" s="42"/>
+      <c r="K13" s="114"/>
+      <c r="L13" s="38"/>
+      <c r="M13" s="43" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="O13" s="101"/>
+      <c r="P13" s="114"/>
+      <c r="Q13" s="38"/>
+      <c r="R13" s="43"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="42"/>
+      <c r="U13" s="42"/>
+      <c r="V13" s="38"/>
+      <c r="W13" s="43"/>
+      <c r="X13" s="42"/>
+      <c r="Y13" s="42"/>
+      <c r="Z13" s="42"/>
+      <c r="AA13" s="38"/>
+      <c r="AB13" s="44"/>
+      <c r="AC13" s="45"/>
+      <c r="AD13" s="46"/>
+    </row>
+    <row r="14" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="36"/>
+      <c r="B14" s="118"/>
+      <c r="C14" s="121" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="43" t="s">
+        <v>125</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>134</v>
+      </c>
+      <c r="F14" s="42"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="I14" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="J14" s="42"/>
+      <c r="K14" s="114"/>
+      <c r="L14" s="38"/>
+      <c r="M14" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="N14" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="O14" s="101"/>
+      <c r="P14" s="114"/>
+      <c r="Q14" s="38"/>
+      <c r="R14" s="43"/>
+      <c r="S14" s="101"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42"/>
+      <c r="V14" s="38"/>
+      <c r="W14" s="43"/>
+      <c r="X14" s="42"/>
+      <c r="Y14" s="42"/>
+      <c r="Z14" s="42"/>
+      <c r="AA14" s="38"/>
+      <c r="AB14" s="44"/>
+      <c r="AC14" s="45"/>
+      <c r="AD14" s="46"/>
+    </row>
+    <row r="15" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36"/>
+      <c r="B15" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C15" s="152"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="42"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="101"/>
+      <c r="J15" s="42"/>
+      <c r="K15" s="114"/>
+      <c r="L15" s="38"/>
+      <c r="M15" s="43"/>
+      <c r="N15" s="101"/>
+      <c r="O15" s="101"/>
+      <c r="P15" s="114"/>
+      <c r="Q15" s="38"/>
+      <c r="R15" s="43"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="42"/>
+      <c r="U15" s="42"/>
+      <c r="V15" s="38"/>
+      <c r="W15" s="43"/>
+      <c r="X15" s="42"/>
+      <c r="Y15" s="42"/>
+      <c r="Z15" s="42"/>
+      <c r="AA15" s="38"/>
+      <c r="AB15" s="44"/>
+      <c r="AC15" s="45"/>
+      <c r="AD15" s="46"/>
+    </row>
+    <row r="16" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="152"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="42"/>
+      <c r="F16" s="42"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="101"/>
+      <c r="J16" s="42"/>
+      <c r="K16" s="114"/>
+      <c r="L16" s="38"/>
+      <c r="M16" s="43" t="s">
+        <v>140</v>
+      </c>
+      <c r="N16" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="O16" s="101"/>
+      <c r="P16" s="114"/>
+      <c r="Q16" s="38"/>
+      <c r="R16" s="43"/>
+      <c r="S16" s="101"/>
+      <c r="T16" s="42"/>
+      <c r="U16" s="42"/>
+      <c r="V16" s="38"/>
+      <c r="W16" s="43"/>
+      <c r="X16" s="42"/>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="42"/>
+      <c r="AA16" s="38"/>
+      <c r="AB16" s="44"/>
+      <c r="AC16" s="45"/>
+      <c r="AD16" s="46"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="47"/>
+      <c r="D17" s="48"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="42"/>
+      <c r="G17" s="38"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="48"/>
+      <c r="J17" s="42"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="38"/>
+      <c r="M17" s="43"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="101"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="38"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="42"/>
+      <c r="T17" s="42"/>
+      <c r="U17" s="42"/>
+      <c r="V17" s="38"/>
+      <c r="W17" s="43"/>
+      <c r="X17" s="42"/>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42"/>
+      <c r="AA17" s="38"/>
+      <c r="AB17" s="44"/>
+      <c r="AC17" s="45"/>
+      <c r="AD17" s="46"/>
+    </row>
+    <row r="18" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="47"/>
+      <c r="D18" s="48"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="42"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="42"/>
+      <c r="L18" s="38"/>
+      <c r="M18" s="43"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="101"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="38"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="42"/>
+      <c r="T18" s="42"/>
+      <c r="U18" s="42"/>
+      <c r="V18" s="38"/>
+      <c r="W18" s="43"/>
+      <c r="X18" s="42"/>
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42"/>
+      <c r="AA18" s="38"/>
+      <c r="AB18" s="44"/>
+      <c r="AC18" s="45"/>
+      <c r="AD18" s="46"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="36"/>
+      <c r="B19" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="47"/>
+      <c r="D19" s="48"/>
+      <c r="E19" s="42"/>
+      <c r="F19" s="42"/>
+      <c r="G19" s="38"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="42"/>
+      <c r="K19" s="42"/>
+      <c r="L19" s="38"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="42"/>
+      <c r="O19" s="101"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="38"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="42"/>
+      <c r="T19" s="42"/>
+      <c r="U19" s="42"/>
+      <c r="V19" s="38"/>
+      <c r="W19" s="43"/>
+      <c r="X19" s="42"/>
+      <c r="Y19" s="42"/>
+      <c r="Z19" s="42"/>
+      <c r="AA19" s="38"/>
+      <c r="AB19" s="44"/>
+      <c r="AC19" s="45"/>
+      <c r="AD19" s="46"/>
+    </row>
+    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A20" s="36"/>
+      <c r="B20" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="E20" s="42"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="48"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
+      <c r="L20" s="38"/>
+      <c r="M20" s="43"/>
+      <c r="N20" s="42"/>
+      <c r="O20" s="101"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="38"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="42"/>
+      <c r="T20" s="42"/>
+      <c r="U20" s="42"/>
+      <c r="V20" s="38"/>
+      <c r="W20" s="43"/>
+      <c r="X20" s="42"/>
+      <c r="Y20" s="42"/>
+      <c r="Z20" s="42"/>
+      <c r="AA20" s="38"/>
+      <c r="AB20" s="44"/>
+      <c r="AC20" s="45"/>
+      <c r="AD20" s="46"/>
+    </row>
+    <row r="21" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C21" s="16"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="106"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="105"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="17"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="106"/>
+      <c r="L21" s="105"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="106"/>
+      <c r="Q21" s="105"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="106"/>
+      <c r="V21" s="105"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="106"/>
+      <c r="AA21" s="105"/>
+      <c r="AB21" s="22"/>
+      <c r="AC21" s="23"/>
+      <c r="AD21" s="24"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="25">
+        <v>1</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="52"/>
+      <c r="D22" s="53"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="108"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="32"/>
+      <c r="K22" s="51"/>
+      <c r="L22" s="108"/>
+      <c r="M22" s="30"/>
+      <c r="N22" s="32"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="108"/>
+      <c r="R22" s="30"/>
+      <c r="S22" s="32"/>
+      <c r="T22" s="32"/>
+      <c r="U22" s="51"/>
+      <c r="V22" s="108"/>
+      <c r="W22" s="30"/>
+      <c r="X22" s="32"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="108"/>
+      <c r="AB22" s="33"/>
+      <c r="AC22" s="34"/>
+      <c r="AD22" s="35"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A23" s="25">
+        <v>2</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C23" s="52"/>
+      <c r="D23" s="53"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="50"/>
+      <c r="G23" s="108"/>
+      <c r="H23" s="52"/>
+      <c r="I23" s="53"/>
+      <c r="J23" s="32"/>
+      <c r="K23" s="51"/>
+      <c r="L23" s="108"/>
+      <c r="M23" s="30"/>
+      <c r="N23" s="32"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="108"/>
+      <c r="R23" s="30"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="32"/>
+      <c r="U23" s="51"/>
+      <c r="V23" s="108"/>
+      <c r="W23" s="30"/>
+      <c r="X23" s="32"/>
+      <c r="Y23" s="32"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="108"/>
+      <c r="AB23" s="33"/>
+      <c r="AC23" s="34"/>
+      <c r="AD23" s="35"/>
+    </row>
+    <row r="24" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="37"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="38"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="38"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="43"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="38"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="38"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="44"/>
+      <c r="AC24" s="45"/>
+      <c r="AD24" s="46"/>
+    </row>
+    <row r="25" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="47"/>
+      <c r="D25" s="51"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="51"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="38"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="42"/>
+      <c r="P25" s="38"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="43"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="38"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="38"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="44"/>
+      <c r="AC25" s="45"/>
+      <c r="AD25" s="46"/>
+    </row>
+    <row r="26" spans="1:30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="36"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="51"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="51"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="43"/>
+      <c r="N26" s="42"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="43"/>
+      <c r="S26" s="42"/>
+      <c r="T26" s="42"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="43"/>
+      <c r="X26" s="42"/>
+      <c r="Y26" s="42"/>
+      <c r="Z26" s="18"/>
+      <c r="AA26" s="18"/>
+      <c r="AB26" s="44"/>
+      <c r="AC26" s="45"/>
+      <c r="AD26" s="46"/>
+    </row>
+    <row r="27" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="25"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="28"/>
+      <c r="G27" s="28"/>
+      <c r="H27" s="70"/>
+      <c r="I27" s="71"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="28"/>
+      <c r="V27" s="28"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="28"/>
+      <c r="AA27" s="28"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="35"/>
+    </row>
+    <row r="28" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+      <c r="W28" s="43"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="44"/>
+      <c r="AC28" s="45"/>
+      <c r="AD28" s="46"/>
+    </row>
+    <row r="29" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="16"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17"/>
+      <c r="F29" s="17"/>
+      <c r="G29" s="105"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="17"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="105"/>
+      <c r="M29" s="20"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="17"/>
+      <c r="Q29" s="105"/>
+      <c r="R29" s="20"/>
+      <c r="S29" s="21"/>
+      <c r="T29" s="21"/>
+      <c r="U29" s="17"/>
+      <c r="V29" s="105"/>
+      <c r="W29" s="20"/>
+      <c r="X29" s="21"/>
+      <c r="Y29" s="21"/>
+      <c r="Z29" s="17"/>
+      <c r="AA29" s="105"/>
+      <c r="AB29" s="22"/>
+      <c r="AC29" s="23"/>
+      <c r="AD29" s="24"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="47"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="67"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="108"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="108"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="108"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="51"/>
+      <c r="V30" s="108"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="108"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="34"/>
+      <c r="AD30" s="35"/>
+    </row>
+    <row r="31" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" s="47"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="67"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="108"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="51"/>
+      <c r="L31" s="108"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="108"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="51"/>
+      <c r="V31" s="108"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="108"/>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="45"/>
+      <c r="AD31" s="46"/>
+    </row>
+    <row r="32" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="36"/>
+      <c r="B32" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C32" s="47"/>
+      <c r="D32" s="51"/>
+      <c r="E32" s="67"/>
+      <c r="F32" s="51"/>
+      <c r="G32" s="111"/>
+      <c r="H32" s="47"/>
+      <c r="I32" s="51"/>
+      <c r="J32" s="42"/>
+      <c r="K32" s="72"/>
+      <c r="L32" s="111"/>
+      <c r="M32" s="47"/>
+      <c r="N32" s="51"/>
+      <c r="O32" s="42"/>
+      <c r="P32" s="72"/>
+      <c r="Q32" s="111"/>
+      <c r="R32" s="47"/>
+      <c r="S32" s="51"/>
+      <c r="T32" s="42"/>
+      <c r="U32" s="72"/>
+      <c r="V32" s="111"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="42"/>
+      <c r="Y32" s="42"/>
+      <c r="Z32" s="72"/>
+      <c r="AA32" s="111"/>
+      <c r="AB32" s="44"/>
+      <c r="AC32" s="45"/>
+      <c r="AD32" s="46"/>
+    </row>
+    <row r="33" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="47" t="s">
+        <v>126</v>
+      </c>
+      <c r="D33" s="122" t="s">
+        <v>127</v>
+      </c>
+      <c r="E33" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="F33" s="51"/>
+      <c r="G33" s="111"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="72"/>
+      <c r="L33" s="111"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="72"/>
+      <c r="Q33" s="111"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="42"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="72"/>
+      <c r="V33" s="111"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="72"/>
+      <c r="AA33" s="111"/>
+      <c r="AB33" s="44"/>
+      <c r="AC33" s="45"/>
+      <c r="AD33" s="46"/>
+    </row>
+    <row r="34" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="36"/>
+      <c r="B34" s="26"/>
+      <c r="C34" s="47" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="123" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="51"/>
+      <c r="G34" s="111"/>
+      <c r="H34" s="47"/>
+      <c r="I34" s="51"/>
+      <c r="J34" s="42"/>
+      <c r="K34" s="72"/>
+      <c r="L34" s="111"/>
+      <c r="M34" s="43"/>
+      <c r="N34" s="42"/>
+      <c r="O34" s="42"/>
+      <c r="P34" s="72"/>
+      <c r="Q34" s="111"/>
+      <c r="R34" s="43"/>
+      <c r="S34" s="42"/>
+      <c r="T34" s="42"/>
+      <c r="U34" s="72"/>
+      <c r="V34" s="111"/>
+      <c r="W34" s="43"/>
+      <c r="X34" s="42"/>
+      <c r="Y34" s="42"/>
+      <c r="Z34" s="72"/>
+      <c r="AA34" s="111"/>
+      <c r="AB34" s="44"/>
+      <c r="AC34" s="45"/>
+      <c r="AD34" s="46"/>
+    </row>
+    <row r="35" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36"/>
+      <c r="B35" s="26"/>
+      <c r="C35" s="47"/>
+      <c r="D35" s="123"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="111"/>
+      <c r="H35" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="I35" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="J35" s="42"/>
+      <c r="K35" s="72"/>
+      <c r="L35" s="111"/>
+      <c r="M35" s="47" t="s">
+        <v>130</v>
+      </c>
+      <c r="N35" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="O35" s="42"/>
+      <c r="P35" s="72"/>
+      <c r="Q35" s="111"/>
+      <c r="R35" s="43"/>
+      <c r="S35" s="42"/>
+      <c r="T35" s="42"/>
+      <c r="U35" s="72"/>
+      <c r="V35" s="111"/>
+      <c r="W35" s="43"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
+      <c r="Z35" s="72"/>
+      <c r="AA35" s="111"/>
+      <c r="AB35" s="44"/>
+      <c r="AC35" s="45"/>
+      <c r="AD35" s="46"/>
+    </row>
+    <row r="36" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="26"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="123"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="111"/>
+      <c r="H36" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="I36" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="J36" s="42"/>
+      <c r="K36" s="72"/>
+      <c r="L36" s="111"/>
+      <c r="M36" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="N36" s="122" t="s">
+        <v>125</v>
+      </c>
+      <c r="O36" s="42"/>
+      <c r="P36" s="72"/>
+      <c r="Q36" s="111"/>
+      <c r="R36" s="43"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="42"/>
+      <c r="U36" s="72"/>
+      <c r="V36" s="111"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="72"/>
+      <c r="AA36" s="111"/>
+      <c r="AB36" s="44"/>
+      <c r="AC36" s="45"/>
+      <c r="AD36" s="46"/>
+    </row>
+    <row r="37" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="123"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="122"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="43"/>
+      <c r="N37" s="101"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="111"/>
+      <c r="R37" s="43"/>
+      <c r="S37" s="42"/>
+      <c r="T37" s="42"/>
+      <c r="U37" s="72"/>
+      <c r="V37" s="111"/>
+      <c r="W37" s="43"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="111"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="45"/>
+      <c r="AD37" s="46"/>
+    </row>
+    <row r="38" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="122"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="43" t="s">
+        <v>142</v>
+      </c>
+      <c r="N38" s="101" t="s">
+        <v>125</v>
+      </c>
+      <c r="O38" s="42"/>
+      <c r="P38" s="72"/>
+      <c r="Q38" s="111"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="42"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="72"/>
+      <c r="V38" s="111"/>
+      <c r="W38" s="43"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="72"/>
+      <c r="AA38" s="111"/>
+      <c r="AB38" s="44"/>
+      <c r="AC38" s="45"/>
+      <c r="AD38" s="46"/>
+    </row>
+    <row r="39" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
+      <c r="B39" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="108"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="108"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="108"/>
+      <c r="W39" s="43"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="108"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="45"/>
+      <c r="AD39" s="46"/>
+    </row>
+    <row r="40" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="36"/>
+      <c r="B40" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="108"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="51"/>
+      <c r="V40" s="108"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="108"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="45"/>
+      <c r="AD40" s="46"/>
+    </row>
+    <row r="41" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
+      <c r="B41" s="26"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="I41" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="J41" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K41" s="51"/>
+      <c r="L41" s="108"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="108"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="51"/>
+      <c r="V41" s="108"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
+      <c r="Z41" s="51"/>
+      <c r="AA41" s="108"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="45"/>
+      <c r="AD41" s="46"/>
+    </row>
+    <row r="42" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="36"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="47"/>
+      <c r="D42" s="51"/>
+      <c r="E42" s="51"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="108"/>
+      <c r="H42" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="I42" s="122" t="s">
+        <v>131</v>
+      </c>
+      <c r="J42" s="42" t="s">
+        <v>138</v>
+      </c>
+      <c r="K42" s="51"/>
+      <c r="L42" s="108"/>
+      <c r="M42" s="43"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="108"/>
+      <c r="R42" s="43"/>
+      <c r="S42" s="42"/>
+      <c r="T42" s="42"/>
+      <c r="U42" s="51"/>
+      <c r="V42" s="108"/>
+      <c r="W42" s="43"/>
+      <c r="X42" s="42"/>
+      <c r="Y42" s="42"/>
+      <c r="Z42" s="51"/>
+      <c r="AA42" s="108"/>
+      <c r="AB42" s="44"/>
+      <c r="AC42" s="45"/>
+      <c r="AD42" s="46"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A43" s="75"/>
+      <c r="B43" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="77"/>
+      <c r="D43" s="76"/>
+      <c r="E43" s="76"/>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="76"/>
+      <c r="I43" s="76"/>
+      <c r="J43" s="76"/>
+      <c r="K43" s="76"/>
+      <c r="L43" s="76"/>
+      <c r="M43" s="76"/>
+      <c r="N43" s="76"/>
+      <c r="O43" s="76"/>
+      <c r="P43" s="76"/>
+      <c r="Q43" s="76"/>
+      <c r="R43" s="76"/>
+      <c r="S43" s="76"/>
+      <c r="T43" s="76"/>
+      <c r="U43" s="76"/>
+      <c r="V43" s="76"/>
+      <c r="W43" s="76"/>
+      <c r="X43" s="76"/>
+      <c r="Y43" s="76"/>
+      <c r="Z43" s="76"/>
+      <c r="AA43" s="76"/>
+      <c r="AB43" s="76"/>
+      <c r="AC43" s="76"/>
+      <c r="AD43" s="78"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="36"/>
+      <c r="B44" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C44" s="47"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="112"/>
+      <c r="F44" s="113"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="113"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="101"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="113"/>
+      <c r="Q44" s="108"/>
+      <c r="R44" s="43"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="113"/>
+      <c r="V44" s="108"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="113"/>
+      <c r="AA44" s="108"/>
+      <c r="AB44" s="44"/>
+      <c r="AC44" s="45"/>
+      <c r="AD44" s="46"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A45" s="36"/>
+      <c r="B45" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="108"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="42"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="108"/>
+      <c r="W45" s="43"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="51"/>
+      <c r="AA45" s="108"/>
+      <c r="AB45" s="44"/>
+      <c r="AC45" s="45"/>
+      <c r="AD45" s="46"/>
+    </row>
+    <row r="46" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="79"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
+      <c r="P46" s="82"/>
+      <c r="Q46" s="88"/>
+      <c r="R46" s="84"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="85"/>
+      <c r="U46" s="82"/>
+      <c r="V46" s="88"/>
+      <c r="W46" s="84"/>
+      <c r="X46" s="85"/>
+      <c r="Y46" s="85"/>
+      <c r="Z46" s="82"/>
+      <c r="AA46" s="88"/>
+      <c r="AB46" s="86"/>
+      <c r="AC46" s="87"/>
+      <c r="AD46" s="88"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A47" s="63"/>
+      <c r="B47" s="64"/>
+      <c r="AB47" s="63"/>
+      <c r="AC47" s="63"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A48" s="63"/>
+      <c r="B48" s="64"/>
+      <c r="AB48" s="63"/>
+      <c r="AC48" s="63"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A49" s="89"/>
+      <c r="B49" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="91"/>
+      <c r="M49" s="91"/>
+      <c r="N49" s="91"/>
+      <c r="O49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="91"/>
+      <c r="T49" s="91"/>
+      <c r="W49" s="89"/>
+      <c r="X49" s="91"/>
+      <c r="Y49" s="91"/>
+      <c r="AB49" s="91"/>
+      <c r="AC49" s="91"/>
+      <c r="AD49" s="91"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A50" s="89"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="91"/>
+      <c r="E50" s="91"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="91"/>
+      <c r="M50" s="91"/>
+      <c r="N50" s="91"/>
+      <c r="O50" s="89"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="91"/>
+      <c r="T50" s="91"/>
+      <c r="W50" s="89"/>
+      <c r="X50" s="91"/>
+      <c r="Y50" s="91"/>
+      <c r="AB50" s="91"/>
+      <c r="AC50" s="91"/>
+      <c r="AD50" s="91"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A51" s="89"/>
+      <c r="B51" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="M51" s="91"/>
+      <c r="N51" s="91"/>
+      <c r="O51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="91"/>
+      <c r="T51" s="91"/>
+      <c r="W51" s="89"/>
+      <c r="X51" s="91"/>
+      <c r="Y51" s="91"/>
+      <c r="AB51" s="91"/>
+      <c r="AC51" s="91"/>
+      <c r="AD51" s="91"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A52" s="89"/>
+      <c r="B52" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="92"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="M52" s="91"/>
+      <c r="N52" s="91"/>
+      <c r="O52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="91"/>
+      <c r="T52" s="91"/>
+      <c r="W52" s="89"/>
+      <c r="X52" s="91"/>
+      <c r="Y52" s="91"/>
+      <c r="AB52" s="91"/>
+      <c r="AC52" s="91"/>
+      <c r="AD52" s="91"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A53" s="63"/>
+      <c r="B53" s="93"/>
+      <c r="C53" s="94"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="94"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="94"/>
+      <c r="J53" s="94"/>
+      <c r="M53" s="94"/>
+      <c r="N53" s="94"/>
+      <c r="O53" s="94"/>
+      <c r="R53" s="94"/>
+      <c r="S53" s="94"/>
+      <c r="T53" s="94"/>
+      <c r="W53" s="94"/>
+      <c r="X53" s="94"/>
+      <c r="Y53" s="94"/>
+      <c r="AB53" s="63"/>
+      <c r="AC53" s="63"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A54" s="63"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="91"/>
+      <c r="L54" s="91"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="94"/>
+      <c r="O54" s="94"/>
+      <c r="P54" s="91"/>
+      <c r="Q54" s="91"/>
+      <c r="R54" s="94"/>
+      <c r="S54" s="94"/>
+      <c r="T54" s="94"/>
+      <c r="U54" s="91"/>
+      <c r="V54" s="91"/>
+      <c r="W54" s="94"/>
+      <c r="X54" s="94"/>
+      <c r="Y54" s="94"/>
+      <c r="Z54" s="91"/>
+      <c r="AA54" s="91"/>
+      <c r="AB54" s="63"/>
+      <c r="AC54" s="63"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A55" s="63"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="91"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="94"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="94"/>
+      <c r="K55" s="91"/>
+      <c r="L55" s="91"/>
+      <c r="M55" s="94"/>
+      <c r="N55" s="94"/>
+      <c r="O55" s="94"/>
+      <c r="P55" s="91"/>
+      <c r="Q55" s="91"/>
+      <c r="R55" s="94"/>
+      <c r="S55" s="94"/>
+      <c r="T55" s="94"/>
+      <c r="U55" s="91"/>
+      <c r="V55" s="91"/>
+      <c r="W55" s="94"/>
+      <c r="X55" s="94"/>
+      <c r="Y55" s="94"/>
+      <c r="Z55" s="91"/>
+      <c r="AA55" s="91"/>
+      <c r="AB55" s="63"/>
+      <c r="AC55" s="63"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A56" s="63"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="91"/>
+      <c r="G56" s="91"/>
+      <c r="H56" s="94"/>
+      <c r="I56" s="94"/>
+      <c r="J56" s="94"/>
+      <c r="K56" s="91"/>
+      <c r="L56" s="91"/>
+      <c r="M56" s="94"/>
+      <c r="N56" s="94"/>
+      <c r="O56" s="94"/>
+      <c r="P56" s="91"/>
+      <c r="Q56" s="91"/>
+      <c r="R56" s="94"/>
+      <c r="S56" s="94"/>
+      <c r="T56" s="94"/>
+      <c r="U56" s="91"/>
+      <c r="V56" s="91"/>
+      <c r="W56" s="94"/>
+      <c r="X56" s="94"/>
+      <c r="Y56" s="94"/>
+      <c r="Z56" s="91"/>
+      <c r="AA56" s="91"/>
+      <c r="AB56" s="63"/>
+      <c r="AC56" s="63"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A57" s="63"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="94"/>
+      <c r="E57" s="94"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
+      <c r="H57" s="94"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="91"/>
+      <c r="M57" s="94"/>
+      <c r="N57" s="94"/>
+      <c r="O57" s="94"/>
+      <c r="P57" s="91"/>
+      <c r="Q57" s="91"/>
+      <c r="R57" s="94"/>
+      <c r="S57" s="94"/>
+      <c r="T57" s="94"/>
+      <c r="U57" s="91"/>
+      <c r="V57" s="91"/>
+      <c r="W57" s="94"/>
+      <c r="X57" s="94"/>
+      <c r="Y57" s="94"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="63"/>
+      <c r="AC57" s="63"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" s="63"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="94"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+      <c r="J58" s="94"/>
+      <c r="K58" s="94"/>
+      <c r="L58" s="94"/>
+      <c r="M58" s="94"/>
+      <c r="N58" s="94"/>
+      <c r="O58" s="94"/>
+      <c r="P58" s="94"/>
+      <c r="Q58" s="94"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="94"/>
+      <c r="T58" s="94"/>
+      <c r="U58" s="94"/>
+      <c r="V58" s="94"/>
+      <c r="W58" s="94"/>
+      <c r="X58" s="94"/>
+      <c r="Y58" s="94"/>
+      <c r="Z58" s="94"/>
+      <c r="AA58" s="94"/>
+      <c r="AB58" s="63"/>
+      <c r="AC58" s="63"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" s="63"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="94"/>
+      <c r="K59" s="94"/>
+      <c r="L59" s="94"/>
+      <c r="M59" s="94"/>
+      <c r="N59" s="94"/>
+      <c r="O59" s="94"/>
+      <c r="P59" s="94"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="94"/>
+      <c r="T59" s="94"/>
+      <c r="U59" s="94"/>
+      <c r="V59" s="94"/>
+      <c r="W59" s="94"/>
+      <c r="X59" s="94"/>
+      <c r="Y59" s="94"/>
+      <c r="Z59" s="94"/>
+      <c r="AA59" s="94"/>
+      <c r="AB59" s="96"/>
+      <c r="AC59" s="96"/>
+      <c r="AD59" s="97"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A60" s="63"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="97"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="94"/>
+      <c r="H60" s="97"/>
+      <c r="I60" s="97"/>
+      <c r="J60" s="97"/>
+      <c r="K60" s="94"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="97"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
+      <c r="P60" s="94"/>
+      <c r="Q60" s="94"/>
+      <c r="R60" s="97"/>
+      <c r="S60" s="97"/>
+      <c r="T60" s="97"/>
+      <c r="U60" s="94"/>
+      <c r="V60" s="94"/>
+      <c r="W60" s="97"/>
+      <c r="X60" s="97"/>
+      <c r="Y60" s="97"/>
+      <c r="Z60" s="94"/>
+      <c r="AA60" s="94"/>
+      <c r="AB60" s="96"/>
+      <c r="AC60" s="96"/>
+      <c r="AD60" s="97"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A61" s="63"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="94"/>
+      <c r="G61" s="94"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="97"/>
+      <c r="K61" s="94"/>
+      <c r="L61" s="94"/>
+      <c r="M61" s="97"/>
+      <c r="N61" s="97"/>
+      <c r="O61" s="97"/>
+      <c r="P61" s="94"/>
+      <c r="Q61" s="94"/>
+      <c r="R61" s="97"/>
+      <c r="S61" s="97"/>
+      <c r="T61" s="97"/>
+      <c r="U61" s="94"/>
+      <c r="V61" s="94"/>
+      <c r="W61" s="97"/>
+      <c r="X61" s="97"/>
+      <c r="Y61" s="97"/>
+      <c r="Z61" s="94"/>
+      <c r="AA61" s="94"/>
+      <c r="AB61" s="96"/>
+      <c r="AC61" s="96"/>
+      <c r="AD61" s="97"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="63"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="97"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="94"/>
+      <c r="G62" s="94"/>
+      <c r="H62" s="97"/>
+      <c r="I62" s="97"/>
+      <c r="J62" s="97"/>
+      <c r="K62" s="94"/>
+      <c r="L62" s="94"/>
+      <c r="M62" s="97"/>
+      <c r="N62" s="97"/>
+      <c r="O62" s="97"/>
+      <c r="P62" s="94"/>
+      <c r="Q62" s="94"/>
+      <c r="R62" s="97"/>
+      <c r="S62" s="97"/>
+      <c r="T62" s="97"/>
+      <c r="U62" s="94"/>
+      <c r="V62" s="94"/>
+      <c r="W62" s="97"/>
+      <c r="X62" s="97"/>
+      <c r="Y62" s="97"/>
+      <c r="Z62" s="94"/>
+      <c r="AA62" s="94"/>
+      <c r="AB62" s="96"/>
+      <c r="AC62" s="96"/>
+      <c r="AD62" s="97"/>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" s="63"/>
+      <c r="B63" s="64"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="94"/>
+      <c r="K63" s="94"/>
+      <c r="L63" s="94"/>
+      <c r="P63" s="94"/>
+      <c r="Q63" s="94"/>
+      <c r="U63" s="94"/>
+      <c r="V63" s="94"/>
+      <c r="Z63" s="94"/>
+      <c r="AA63" s="94"/>
+      <c r="AB63" s="63"/>
+      <c r="AC63" s="63"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F64" s="94"/>
+      <c r="G64" s="94"/>
+      <c r="K64" s="94"/>
+      <c r="L64" s="94"/>
+      <c r="P64" s="94"/>
+      <c r="Q64" s="94"/>
+      <c r="U64" s="94"/>
+      <c r="V64" s="94"/>
+      <c r="Z64" s="94"/>
+      <c r="AA64" s="94"/>
+    </row>
+    <row r="65" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F65" s="97"/>
+      <c r="G65" s="97"/>
+      <c r="K65" s="97"/>
+      <c r="L65" s="97"/>
+      <c r="P65" s="97"/>
+      <c r="Q65" s="97"/>
+      <c r="U65" s="97"/>
+      <c r="V65" s="97"/>
+      <c r="Z65" s="97"/>
+      <c r="AA65" s="97"/>
+    </row>
+    <row r="66" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="97"/>
+      <c r="P66" s="97"/>
+      <c r="Q66" s="97"/>
+      <c r="U66" s="97"/>
+      <c r="V66" s="97"/>
+      <c r="Z66" s="97"/>
+      <c r="AA66" s="97"/>
+    </row>
+    <row r="67" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F67" s="97"/>
+      <c r="G67" s="97"/>
+      <c r="K67" s="97"/>
+      <c r="L67" s="97"/>
+      <c r="P67" s="97"/>
+      <c r="Q67" s="97"/>
+      <c r="U67" s="97"/>
+      <c r="V67" s="97"/>
+      <c r="Z67" s="97"/>
+      <c r="AA67" s="97"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="AD6:AD9"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="AC6:AC9"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change bao cao tuan 4 thang 9
</commit_message>
<xml_diff>
--- a/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
+++ b/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
@@ -913,7 +913,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="175">
   <si>
     <t>TT</t>
   </si>
@@ -1425,6 +1425,21 @@
   </si>
   <si>
     <t>Tìm hiểu hệ thống IBM InfoSphere Stream</t>
+  </si>
+  <si>
+    <t>26/09/2014</t>
+  </si>
+  <si>
+    <t>Pending do Comverse thay đổi flow</t>
+  </si>
+  <si>
+    <t>Chuyển sprint tiếp theo</t>
+  </si>
+  <si>
+    <t>Pending dành thời gian làm C1</t>
+  </si>
+  <si>
+    <t>Hoàn thành 20%</t>
   </si>
 </sst>
 </file>
@@ -2666,6 +2681,81 @@
     <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2673,81 +2763,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3484,10 +3499,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="143"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -3553,94 +3568,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="148"/>
-      <c r="Q6" s="148"/>
-      <c r="R6" s="148"/>
-      <c r="S6" s="148"/>
-      <c r="T6" s="148"/>
-      <c r="U6" s="148"/>
-      <c r="V6" s="148"/>
-      <c r="W6" s="148"/>
-      <c r="X6" s="148"/>
-      <c r="Y6" s="148"/>
-      <c r="Z6" s="148"/>
-      <c r="AA6" s="149"/>
-      <c r="AB6" s="150" t="s">
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="134"/>
+      <c r="Y6" s="134"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="135"/>
+      <c r="AB6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="126" t="s">
+      <c r="AC6" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="129" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="145"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="134" t="s">
+      <c r="A7" s="128"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="137" t="s">
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="134" t="s">
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="137" t="s">
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="134" t="s">
+      <c r="S7" s="149"/>
+      <c r="T7" s="149"/>
+      <c r="U7" s="149"/>
+      <c r="V7" s="149"/>
+      <c r="W7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="135"/>
-      <c r="Y7" s="135"/>
-      <c r="Z7" s="135"/>
-      <c r="AA7" s="136"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="130"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="147"/>
+      <c r="AB7" s="137"/>
+      <c r="AC7" s="152"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="130"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="141" t="s">
         <v>6</v>
       </c>
@@ -3648,10 +3663,10 @@
       <c r="E8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="132" t="s">
+      <c r="F8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="133"/>
+      <c r="G8" s="144"/>
       <c r="H8" s="141" t="s">
         <v>6</v>
       </c>
@@ -3659,10 +3674,10 @@
       <c r="J8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="132" t="s">
+      <c r="K8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="133"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="141" t="s">
         <v>6</v>
       </c>
@@ -3670,10 +3685,10 @@
       <c r="O8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="132" t="s">
+      <c r="P8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="133"/>
+      <c r="Q8" s="144"/>
       <c r="R8" s="141" t="s">
         <v>6</v>
       </c>
@@ -3681,10 +3696,10 @@
       <c r="T8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="132" t="s">
+      <c r="U8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="133"/>
+      <c r="V8" s="144"/>
       <c r="W8" s="141" t="s">
         <v>6</v>
       </c>
@@ -3692,17 +3707,17 @@
       <c r="Y8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="132" t="s">
+      <c r="Z8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="130"/>
+      <c r="AA8" s="144"/>
+      <c r="AB8" s="137"/>
+      <c r="AC8" s="152"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="146"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -3768,9 +3783,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="128"/>
-      <c r="AD9" s="131"/>
+      <c r="AB9" s="138"/>
+      <c r="AC9" s="153"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -6004,6 +6019,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="AC6:AC9"/>
+    <mergeCell ref="AD6:AD9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:AA8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
@@ -6020,17 +6046,6 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="AC6:AC9"/>
-    <mergeCell ref="AD6:AD9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:AA8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6182,10 +6197,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="143"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -6251,94 +6266,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="148"/>
-      <c r="Q6" s="148"/>
-      <c r="R6" s="148"/>
-      <c r="S6" s="148"/>
-      <c r="T6" s="148"/>
-      <c r="U6" s="148"/>
-      <c r="V6" s="148"/>
-      <c r="W6" s="148"/>
-      <c r="X6" s="148"/>
-      <c r="Y6" s="148"/>
-      <c r="Z6" s="148"/>
-      <c r="AA6" s="149"/>
-      <c r="AB6" s="150" t="s">
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="134"/>
+      <c r="Y6" s="134"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="135"/>
+      <c r="AB6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="126" t="s">
+      <c r="AC6" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="129" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="145"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="134" t="s">
+      <c r="A7" s="128"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="137" t="s">
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="134" t="s">
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="137" t="s">
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="134" t="s">
+      <c r="S7" s="149"/>
+      <c r="T7" s="149"/>
+      <c r="U7" s="149"/>
+      <c r="V7" s="149"/>
+      <c r="W7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="135"/>
-      <c r="Y7" s="135"/>
-      <c r="Z7" s="135"/>
-      <c r="AA7" s="136"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="130"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="147"/>
+      <c r="AB7" s="137"/>
+      <c r="AC7" s="152"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="130"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="141" t="s">
         <v>6</v>
       </c>
@@ -6346,10 +6361,10 @@
       <c r="E8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="132" t="s">
+      <c r="F8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="133"/>
+      <c r="G8" s="144"/>
       <c r="H8" s="141" t="s">
         <v>6</v>
       </c>
@@ -6357,10 +6372,10 @@
       <c r="J8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="132" t="s">
+      <c r="K8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="133"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="141" t="s">
         <v>6</v>
       </c>
@@ -6368,10 +6383,10 @@
       <c r="O8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="132" t="s">
+      <c r="P8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="133"/>
+      <c r="Q8" s="144"/>
       <c r="R8" s="141" t="s">
         <v>6</v>
       </c>
@@ -6379,10 +6394,10 @@
       <c r="T8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="132" t="s">
+      <c r="U8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="133"/>
+      <c r="V8" s="144"/>
       <c r="W8" s="141" t="s">
         <v>6</v>
       </c>
@@ -6390,17 +6405,17 @@
       <c r="Y8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="132" t="s">
+      <c r="Z8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="130"/>
+      <c r="AA8" s="144"/>
+      <c r="AB8" s="137"/>
+      <c r="AC8" s="152"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="146"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -6466,9 +6481,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="128"/>
-      <c r="AD9" s="131"/>
+      <c r="AB9" s="138"/>
+      <c r="AC9" s="153"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -8204,17 +8219,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -8231,6 +8235,17 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -8382,10 +8397,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="143"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -8451,94 +8466,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="148"/>
-      <c r="Q6" s="148"/>
-      <c r="R6" s="148"/>
-      <c r="S6" s="148"/>
-      <c r="T6" s="148"/>
-      <c r="U6" s="148"/>
-      <c r="V6" s="148"/>
-      <c r="W6" s="148"/>
-      <c r="X6" s="148"/>
-      <c r="Y6" s="148"/>
-      <c r="Z6" s="148"/>
-      <c r="AA6" s="149"/>
-      <c r="AB6" s="150" t="s">
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="134"/>
+      <c r="Y6" s="134"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="135"/>
+      <c r="AB6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="126" t="s">
+      <c r="AC6" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="129" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="145"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="134" t="s">
+      <c r="A7" s="128"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="137" t="s">
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="134" t="s">
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="137" t="s">
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="134" t="s">
+      <c r="S7" s="149"/>
+      <c r="T7" s="149"/>
+      <c r="U7" s="149"/>
+      <c r="V7" s="149"/>
+      <c r="W7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="135"/>
-      <c r="Y7" s="135"/>
-      <c r="Z7" s="135"/>
-      <c r="AA7" s="136"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="130"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="147"/>
+      <c r="AB7" s="137"/>
+      <c r="AC7" s="152"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="130"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="141" t="s">
         <v>6</v>
       </c>
@@ -8546,10 +8561,10 @@
       <c r="E8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="132" t="s">
+      <c r="F8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="133"/>
+      <c r="G8" s="144"/>
       <c r="H8" s="141" t="s">
         <v>6</v>
       </c>
@@ -8557,10 +8572,10 @@
       <c r="J8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="132" t="s">
+      <c r="K8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="133"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="141" t="s">
         <v>6</v>
       </c>
@@ -8568,10 +8583,10 @@
       <c r="O8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="132" t="s">
+      <c r="P8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="133"/>
+      <c r="Q8" s="144"/>
       <c r="R8" s="141" t="s">
         <v>6</v>
       </c>
@@ -8579,10 +8594,10 @@
       <c r="T8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="132" t="s">
+      <c r="U8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="133"/>
+      <c r="V8" s="144"/>
       <c r="W8" s="141" t="s">
         <v>6</v>
       </c>
@@ -8590,17 +8605,17 @@
       <c r="Y8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="132" t="s">
+      <c r="Z8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="130"/>
+      <c r="AA8" s="144"/>
+      <c r="AB8" s="137"/>
+      <c r="AC8" s="152"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="146"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -8666,9 +8681,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="128"/>
-      <c r="AD9" s="131"/>
+      <c r="AB9" s="138"/>
+      <c r="AC9" s="153"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -10546,17 +10561,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -10573,6 +10577,17 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10585,8 +10600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="K12" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10724,10 +10739,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="143" t="s">
+      <c r="A4" s="126" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="143"/>
+      <c r="B4" s="126"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -10793,94 +10808,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="144" t="s">
+      <c r="A6" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="129" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="147" t="s">
+      <c r="C6" s="133" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="148"/>
-      <c r="E6" s="148"/>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
-      <c r="H6" s="148"/>
-      <c r="I6" s="148"/>
-      <c r="J6" s="148"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="148"/>
-      <c r="Q6" s="148"/>
-      <c r="R6" s="148"/>
-      <c r="S6" s="148"/>
-      <c r="T6" s="148"/>
-      <c r="U6" s="148"/>
-      <c r="V6" s="148"/>
-      <c r="W6" s="148"/>
-      <c r="X6" s="148"/>
-      <c r="Y6" s="148"/>
-      <c r="Z6" s="148"/>
-      <c r="AA6" s="149"/>
-      <c r="AB6" s="150" t="s">
+      <c r="D6" s="134"/>
+      <c r="E6" s="134"/>
+      <c r="F6" s="134"/>
+      <c r="G6" s="134"/>
+      <c r="H6" s="134"/>
+      <c r="I6" s="134"/>
+      <c r="J6" s="134"/>
+      <c r="K6" s="134"/>
+      <c r="L6" s="134"/>
+      <c r="M6" s="134"/>
+      <c r="N6" s="134"/>
+      <c r="O6" s="134"/>
+      <c r="P6" s="134"/>
+      <c r="Q6" s="134"/>
+      <c r="R6" s="134"/>
+      <c r="S6" s="134"/>
+      <c r="T6" s="134"/>
+      <c r="U6" s="134"/>
+      <c r="V6" s="134"/>
+      <c r="W6" s="134"/>
+      <c r="X6" s="134"/>
+      <c r="Y6" s="134"/>
+      <c r="Z6" s="134"/>
+      <c r="AA6" s="135"/>
+      <c r="AB6" s="136" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="126" t="s">
+      <c r="AC6" s="151" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="129" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="145"/>
-      <c r="B7" s="130"/>
-      <c r="C7" s="134" t="s">
+      <c r="A7" s="128"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="145" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="135"/>
-      <c r="E7" s="135"/>
-      <c r="F7" s="135"/>
-      <c r="G7" s="136"/>
-      <c r="H7" s="137" t="s">
+      <c r="D7" s="146"/>
+      <c r="E7" s="146"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="147"/>
+      <c r="H7" s="148" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="138"/>
-      <c r="J7" s="138"/>
-      <c r="K7" s="138"/>
-      <c r="L7" s="153"/>
-      <c r="M7" s="134" t="s">
+      <c r="I7" s="149"/>
+      <c r="J7" s="149"/>
+      <c r="K7" s="149"/>
+      <c r="L7" s="150"/>
+      <c r="M7" s="145" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="135"/>
-      <c r="O7" s="135"/>
-      <c r="P7" s="135"/>
-      <c r="Q7" s="136"/>
-      <c r="R7" s="137" t="s">
+      <c r="N7" s="146"/>
+      <c r="O7" s="146"/>
+      <c r="P7" s="146"/>
+      <c r="Q7" s="147"/>
+      <c r="R7" s="148" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="138"/>
-      <c r="T7" s="138"/>
-      <c r="U7" s="138"/>
-      <c r="V7" s="138"/>
-      <c r="W7" s="134" t="s">
+      <c r="S7" s="149"/>
+      <c r="T7" s="149"/>
+      <c r="U7" s="149"/>
+      <c r="V7" s="149"/>
+      <c r="W7" s="145" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="135"/>
-      <c r="Y7" s="135"/>
-      <c r="Z7" s="135"/>
-      <c r="AA7" s="136"/>
-      <c r="AB7" s="151"/>
-      <c r="AC7" s="127"/>
-      <c r="AD7" s="130"/>
+      <c r="X7" s="146"/>
+      <c r="Y7" s="146"/>
+      <c r="Z7" s="146"/>
+      <c r="AA7" s="147"/>
+      <c r="AB7" s="137"/>
+      <c r="AC7" s="152"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="145"/>
-      <c r="B8" s="130"/>
+      <c r="A8" s="128"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="141" t="s">
         <v>6</v>
       </c>
@@ -10888,10 +10903,10 @@
       <c r="E8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="132" t="s">
+      <c r="F8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="133"/>
+      <c r="G8" s="144"/>
       <c r="H8" s="141" t="s">
         <v>6</v>
       </c>
@@ -10899,10 +10914,10 @@
       <c r="J8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="132" t="s">
+      <c r="K8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="133"/>
+      <c r="L8" s="144"/>
       <c r="M8" s="141" t="s">
         <v>6</v>
       </c>
@@ -10910,10 +10925,10 @@
       <c r="O8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="132" t="s">
+      <c r="P8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="133"/>
+      <c r="Q8" s="144"/>
       <c r="R8" s="141" t="s">
         <v>6</v>
       </c>
@@ -10921,10 +10936,10 @@
       <c r="T8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="132" t="s">
+      <c r="U8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="133"/>
+      <c r="V8" s="144"/>
       <c r="W8" s="141" t="s">
         <v>6</v>
       </c>
@@ -10932,17 +10947,17 @@
       <c r="Y8" s="139" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="132" t="s">
+      <c r="Z8" s="143" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="133"/>
-      <c r="AB8" s="151"/>
-      <c r="AC8" s="127"/>
-      <c r="AD8" s="130"/>
+      <c r="AA8" s="144"/>
+      <c r="AB8" s="137"/>
+      <c r="AC8" s="152"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="146"/>
-      <c r="B9" s="131"/>
+      <c r="A9" s="129"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -11008,9 +11023,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="152"/>
-      <c r="AC9" s="128"/>
-      <c r="AD9" s="131"/>
+      <c r="AB9" s="138"/>
+      <c r="AC9" s="153"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -11121,20 +11136,20 @@
     <row r="13" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="36"/>
       <c r="B13" s="118"/>
-      <c r="C13" s="43" t="s">
-        <v>153</v>
-      </c>
-      <c r="D13" s="116" t="s">
-        <v>149</v>
-      </c>
-      <c r="E13" s="42" t="s">
-        <v>97</v>
-      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="42"/>
       <c r="G13" s="38"/>
-      <c r="H13" s="43"/>
-      <c r="I13" s="101"/>
-      <c r="J13" s="42"/>
+      <c r="H13" s="43" t="s">
+        <v>153</v>
+      </c>
+      <c r="I13" s="101" t="s">
+        <v>149</v>
+      </c>
+      <c r="J13" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="K13" s="114"/>
       <c r="L13" s="38"/>
       <c r="M13" s="43"/>
@@ -11142,15 +11157,9 @@
       <c r="O13" s="101"/>
       <c r="P13" s="114"/>
       <c r="Q13" s="38"/>
-      <c r="R13" s="43" t="s">
-        <v>123</v>
-      </c>
-      <c r="S13" s="101" t="s">
-        <v>125</v>
-      </c>
-      <c r="T13" s="42" t="s">
-        <v>97</v>
-      </c>
+      <c r="R13" s="43"/>
+      <c r="S13" s="101"/>
+      <c r="T13" s="42"/>
       <c r="U13" s="42"/>
       <c r="V13" s="38"/>
       <c r="W13" s="43"/>
@@ -11165,20 +11174,20 @@
     <row r="14" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="36"/>
       <c r="B14" s="118"/>
-      <c r="C14" s="42" t="s">
-        <v>154</v>
-      </c>
-      <c r="D14" s="116" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="42" t="s">
-        <v>159</v>
-      </c>
+      <c r="C14" s="42"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="42"/>
       <c r="F14" s="42"/>
       <c r="G14" s="38"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="101"/>
-      <c r="J14" s="42"/>
+      <c r="H14" s="43" t="s">
+        <v>154</v>
+      </c>
+      <c r="I14" s="101" t="s">
+        <v>149</v>
+      </c>
+      <c r="J14" s="42" t="s">
+        <v>159</v>
+      </c>
       <c r="K14" s="114"/>
       <c r="L14" s="38"/>
       <c r="M14" s="43"/>
@@ -11203,20 +11212,20 @@
     <row r="15" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="36"/>
       <c r="B15" s="118"/>
-      <c r="C15" s="121" t="s">
-        <v>155</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>157</v>
-      </c>
-      <c r="E15" s="42" t="s">
-        <v>97</v>
-      </c>
+      <c r="C15" s="121"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="42"/>
       <c r="F15" s="42"/>
       <c r="G15" s="38"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="101"/>
-      <c r="J15" s="42"/>
+      <c r="H15" s="43" t="s">
+        <v>155</v>
+      </c>
+      <c r="I15" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="J15" s="42" t="s">
+        <v>97</v>
+      </c>
       <c r="K15" s="114"/>
       <c r="L15" s="38"/>
       <c r="M15" s="43"/>
@@ -11224,15 +11233,9 @@
       <c r="O15" s="101"/>
       <c r="P15" s="114"/>
       <c r="Q15" s="38"/>
-      <c r="R15" s="43" t="s">
-        <v>124</v>
-      </c>
-      <c r="S15" s="101" t="s">
-        <v>125</v>
-      </c>
-      <c r="T15" s="42" t="s">
-        <v>103</v>
-      </c>
+      <c r="R15" s="43"/>
+      <c r="S15" s="101"/>
+      <c r="T15" s="42"/>
       <c r="U15" s="42"/>
       <c r="V15" s="38"/>
       <c r="W15" s="43"/>
@@ -11252,22 +11255,28 @@
       <c r="E16" s="42"/>
       <c r="F16" s="42"/>
       <c r="G16" s="38"/>
-      <c r="H16" s="43" t="s">
-        <v>162</v>
-      </c>
-      <c r="I16" s="101" t="s">
-        <v>166</v>
-      </c>
+      <c r="H16" s="43"/>
+      <c r="I16" s="101"/>
       <c r="J16" s="42"/>
       <c r="K16" s="114"/>
       <c r="L16" s="38"/>
-      <c r="M16" s="43"/>
-      <c r="N16" s="101"/>
-      <c r="O16" s="101"/>
+      <c r="M16" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="N16" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="O16" s="101" t="s">
+        <v>171</v>
+      </c>
       <c r="P16" s="114"/>
       <c r="Q16" s="38"/>
-      <c r="R16" s="43"/>
-      <c r="S16" s="101"/>
+      <c r="R16" s="43" t="s">
+        <v>162</v>
+      </c>
+      <c r="S16" s="101" t="s">
+        <v>170</v>
+      </c>
       <c r="T16" s="42"/>
       <c r="U16" s="42"/>
       <c r="V16" s="38"/>
@@ -11290,22 +11299,28 @@
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
       <c r="G17" s="38"/>
-      <c r="H17" s="43" t="s">
-        <v>163</v>
-      </c>
-      <c r="I17" s="101" t="s">
-        <v>166</v>
-      </c>
+      <c r="H17" s="43"/>
+      <c r="I17" s="101"/>
       <c r="J17" s="42"/>
       <c r="K17" s="114"/>
       <c r="L17" s="38"/>
-      <c r="M17" s="43"/>
-      <c r="N17" s="101"/>
-      <c r="O17" s="101"/>
+      <c r="M17" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="N17" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="O17" s="101" t="s">
+        <v>171</v>
+      </c>
       <c r="P17" s="114"/>
       <c r="Q17" s="38"/>
-      <c r="R17" s="43"/>
-      <c r="S17" s="101"/>
+      <c r="R17" s="43" t="s">
+        <v>163</v>
+      </c>
+      <c r="S17" s="101" t="s">
+        <v>170</v>
+      </c>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
       <c r="V17" s="38"/>
@@ -11326,18 +11341,20 @@
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
       <c r="G18" s="38"/>
-      <c r="H18" s="43" t="s">
-        <v>164</v>
-      </c>
-      <c r="I18" s="101" t="s">
-        <v>157</v>
-      </c>
+      <c r="H18" s="43"/>
+      <c r="I18" s="101"/>
       <c r="J18" s="42"/>
       <c r="K18" s="114"/>
       <c r="L18" s="38"/>
-      <c r="M18" s="43"/>
-      <c r="N18" s="101"/>
-      <c r="O18" s="101"/>
+      <c r="M18" s="43" t="s">
+        <v>164</v>
+      </c>
+      <c r="N18" s="101" t="s">
+        <v>157</v>
+      </c>
+      <c r="O18" s="101" t="s">
+        <v>97</v>
+      </c>
       <c r="P18" s="114"/>
       <c r="Q18" s="38"/>
       <c r="R18" s="43"/>
@@ -11362,22 +11379,28 @@
       <c r="E19" s="42"/>
       <c r="F19" s="42"/>
       <c r="G19" s="38"/>
-      <c r="H19" s="43" t="s">
-        <v>165</v>
-      </c>
-      <c r="I19" s="101" t="s">
-        <v>166</v>
-      </c>
+      <c r="H19" s="43"/>
+      <c r="I19" s="101"/>
       <c r="J19" s="42"/>
       <c r="K19" s="114"/>
       <c r="L19" s="38"/>
-      <c r="M19" s="43"/>
-      <c r="N19" s="101"/>
-      <c r="O19" s="101"/>
+      <c r="M19" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="N19" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="O19" s="101" t="s">
+        <v>84</v>
+      </c>
       <c r="P19" s="114"/>
       <c r="Q19" s="38"/>
-      <c r="R19" s="43"/>
-      <c r="S19" s="101"/>
+      <c r="R19" s="43" t="s">
+        <v>165</v>
+      </c>
+      <c r="S19" s="101" t="s">
+        <v>170</v>
+      </c>
       <c r="T19" s="42"/>
       <c r="U19" s="42"/>
       <c r="V19" s="38"/>
@@ -11398,22 +11421,28 @@
       <c r="E20" s="42"/>
       <c r="F20" s="42"/>
       <c r="G20" s="38"/>
-      <c r="H20" s="43" t="s">
-        <v>167</v>
-      </c>
-      <c r="I20" s="101" t="s">
-        <v>166</v>
-      </c>
+      <c r="H20" s="43"/>
+      <c r="I20" s="101"/>
       <c r="J20" s="42"/>
       <c r="K20" s="114"/>
       <c r="L20" s="38"/>
-      <c r="M20" s="43"/>
-      <c r="N20" s="101"/>
-      <c r="O20" s="101"/>
+      <c r="M20" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="N20" s="101" t="s">
+        <v>166</v>
+      </c>
+      <c r="O20" s="101" t="s">
+        <v>172</v>
+      </c>
       <c r="P20" s="114"/>
       <c r="Q20" s="38"/>
-      <c r="R20" s="43"/>
-      <c r="S20" s="101"/>
+      <c r="R20" s="43" t="s">
+        <v>167</v>
+      </c>
+      <c r="S20" s="101" t="s">
+        <v>170</v>
+      </c>
       <c r="T20" s="42"/>
       <c r="U20" s="42"/>
       <c r="V20" s="38"/>
@@ -11436,19 +11465,21 @@
       <c r="E21" s="42"/>
       <c r="F21" s="42"/>
       <c r="G21" s="38"/>
-      <c r="H21" s="43" t="s">
-        <v>161</v>
-      </c>
+      <c r="H21" s="43"/>
       <c r="I21" s="101"/>
       <c r="J21" s="42"/>
       <c r="K21" s="114"/>
       <c r="L21" s="38"/>
-      <c r="M21" s="43"/>
+      <c r="M21" s="43" t="s">
+        <v>161</v>
+      </c>
       <c r="N21" s="101"/>
       <c r="O21" s="101"/>
       <c r="P21" s="114"/>
       <c r="Q21" s="38"/>
-      <c r="R21" s="43"/>
+      <c r="R21" s="43" t="s">
+        <v>161</v>
+      </c>
       <c r="S21" s="101"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
@@ -11465,15 +11496,9 @@
     <row r="22" spans="1:30" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="36"/>
       <c r="B22" s="26"/>
-      <c r="C22" s="124" t="s">
-        <v>140</v>
-      </c>
-      <c r="D22" s="43" t="s">
-        <v>156</v>
-      </c>
-      <c r="E22" s="42" t="s">
-        <v>160</v>
-      </c>
+      <c r="C22" s="124"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="42"/>
       <c r="F22" s="42"/>
       <c r="G22" s="38"/>
       <c r="H22" s="124" t="s">
@@ -11482,23 +11507,29 @@
       <c r="I22" s="43" t="s">
         <v>156</v>
       </c>
-      <c r="J22" s="42"/>
+      <c r="J22" s="42" t="s">
+        <v>160</v>
+      </c>
       <c r="K22" s="114"/>
       <c r="L22" s="38"/>
-      <c r="M22" s="43"/>
-      <c r="N22" s="101"/>
-      <c r="O22" s="101"/>
+      <c r="M22" s="124" t="s">
+        <v>140</v>
+      </c>
+      <c r="N22" s="43" t="s">
+        <v>156</v>
+      </c>
+      <c r="O22" s="101" t="s">
+        <v>173</v>
+      </c>
       <c r="P22" s="114"/>
       <c r="Q22" s="38"/>
       <c r="R22" s="43" t="s">
         <v>140</v>
       </c>
       <c r="S22" s="101" t="s">
-        <v>125</v>
-      </c>
-      <c r="T22" s="42" t="s">
-        <v>150</v>
-      </c>
+        <v>156</v>
+      </c>
+      <c r="T22" s="42"/>
       <c r="U22" s="42"/>
       <c r="V22" s="38"/>
       <c r="W22" s="43"/>
@@ -12055,17 +12086,17 @@
     <row r="39" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="36"/>
       <c r="B39" s="26"/>
-      <c r="C39" s="47" t="s">
-        <v>132</v>
-      </c>
-      <c r="D39" s="123" t="s">
-        <v>156</v>
-      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="123"/>
       <c r="E39" s="67"/>
       <c r="F39" s="51"/>
       <c r="G39" s="111"/>
-      <c r="H39" s="47"/>
-      <c r="I39" s="122"/>
+      <c r="H39" s="47" t="s">
+        <v>132</v>
+      </c>
+      <c r="I39" s="122" t="s">
+        <v>156</v>
+      </c>
       <c r="J39" s="42"/>
       <c r="K39" s="72"/>
       <c r="L39" s="111"/>
@@ -12122,20 +12153,20 @@
       <c r="AC40" s="45"/>
       <c r="AD40" s="46"/>
     </row>
-    <row r="41" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A41" s="36"/>
       <c r="B41" s="26"/>
-      <c r="C41" s="47" t="s">
-        <v>142</v>
-      </c>
-      <c r="D41" s="123" t="s">
-        <v>156</v>
-      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="123"/>
       <c r="E41" s="67"/>
       <c r="F41" s="51"/>
       <c r="G41" s="111"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="122"/>
+      <c r="H41" s="47" t="s">
+        <v>142</v>
+      </c>
+      <c r="I41" s="122" t="s">
+        <v>156</v>
+      </c>
       <c r="J41" s="42"/>
       <c r="K41" s="72"/>
       <c r="L41" s="111"/>
@@ -12268,22 +12299,28 @@
       <c r="E45" s="51"/>
       <c r="F45" s="51"/>
       <c r="G45" s="108"/>
-      <c r="H45" s="47" t="s">
-        <v>169</v>
-      </c>
-      <c r="I45" s="122" t="s">
-        <v>156</v>
-      </c>
+      <c r="H45" s="47"/>
+      <c r="I45" s="122"/>
       <c r="J45" s="42"/>
       <c r="K45" s="51"/>
       <c r="L45" s="108"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="42"/>
-      <c r="O45" s="42"/>
+      <c r="M45" s="47" t="s">
+        <v>169</v>
+      </c>
+      <c r="N45" s="122" t="s">
+        <v>156</v>
+      </c>
+      <c r="O45" s="114" t="s">
+        <v>174</v>
+      </c>
       <c r="P45" s="51"/>
       <c r="Q45" s="108"/>
-      <c r="R45" s="43"/>
-      <c r="S45" s="42"/>
+      <c r="R45" s="43" t="s">
+        <v>169</v>
+      </c>
+      <c r="S45" s="42" t="s">
+        <v>156</v>
+      </c>
       <c r="T45" s="42"/>
       <c r="U45" s="51"/>
       <c r="V45" s="108"/>
@@ -12398,20 +12435,20 @@
       <c r="AC48" s="45"/>
       <c r="AD48" s="46"/>
     </row>
-    <row r="49" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="36"/>
       <c r="B49" s="26"/>
-      <c r="C49" s="47" t="s">
-        <v>158</v>
-      </c>
-      <c r="D49" s="51" t="s">
-        <v>156</v>
-      </c>
+      <c r="C49" s="47"/>
+      <c r="D49" s="51"/>
       <c r="E49" s="67"/>
       <c r="F49" s="51"/>
       <c r="G49" s="108"/>
-      <c r="H49" s="74"/>
-      <c r="I49" s="51"/>
+      <c r="H49" s="74" t="s">
+        <v>158</v>
+      </c>
+      <c r="I49" s="51" t="s">
+        <v>156</v>
+      </c>
       <c r="J49" s="42"/>
       <c r="K49" s="51"/>
       <c r="L49" s="108"/>
@@ -12942,15 +12979,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -12967,6 +12995,15 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
     <mergeCell ref="W8:X8"/>
     <mergeCell ref="Y8:Y9"/>
   </mergeCells>

</xml_diff>

<commit_message>
change bao cao tuan
</commit_message>
<xml_diff>
--- a/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
+++ b/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="1"/>
@@ -465,7 +465,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="124">
   <si>
     <t>TT</t>
   </si>
@@ -821,6 +821,24 @@
   </si>
   <si>
     <t>25/07/2014</t>
+  </si>
+  <si>
+    <t>Hoàn thành, đang đợi PKT bổ sung thêm phần cứng</t>
+  </si>
+  <si>
+    <t>Pending do hệ thống chuyển xuông tầng 6, mất kết nối</t>
+  </si>
+  <si>
+    <t>Hoàn thành 60%</t>
+  </si>
+  <si>
+    <t>Dựng eOneRate đấu nối vào hệ thống POC, test full luồng</t>
+  </si>
+  <si>
+    <t>Upgrage POC</t>
+  </si>
+  <si>
+    <t>01/08/2014</t>
   </si>
 </sst>
 </file>
@@ -1708,7 +1726,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2032,6 +2050,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -2044,15 +2113,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2071,50 +2131,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="16" fontId="6" fillId="8" borderId="32" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2704,10 +2725,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="121"/>
+      <c r="B4" s="138"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -2773,94 +2794,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="131" t="s">
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
+      <c r="R6" s="143"/>
+      <c r="S6" s="143"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="143"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="143"/>
+      <c r="Z6" s="143"/>
+      <c r="AA6" s="144"/>
+      <c r="AB6" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="146" t="s">
+      <c r="AC6" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="125" t="s">
+      <c r="AD6" s="124" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="140" t="s">
+      <c r="A7" s="140"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="143" t="s">
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="140" t="s">
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="143" t="s">
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="132" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="140" t="s">
+      <c r="S7" s="133"/>
+      <c r="T7" s="133"/>
+      <c r="U7" s="133"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="142"/>
-      <c r="AB7" s="132"/>
-      <c r="AC7" s="147"/>
-      <c r="AD7" s="126"/>
+      <c r="X7" s="130"/>
+      <c r="Y7" s="130"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="131"/>
+      <c r="AB7" s="146"/>
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="125"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="136" t="s">
         <v>6</v>
       </c>
@@ -2868,10 +2889,10 @@
       <c r="E8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="139"/>
+      <c r="G8" s="128"/>
       <c r="H8" s="136" t="s">
         <v>6</v>
       </c>
@@ -2879,10 +2900,10 @@
       <c r="J8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="138" t="s">
+      <c r="K8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="139"/>
+      <c r="L8" s="128"/>
       <c r="M8" s="136" t="s">
         <v>6</v>
       </c>
@@ -2890,10 +2911,10 @@
       <c r="O8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="138" t="s">
+      <c r="P8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="139"/>
+      <c r="Q8" s="128"/>
       <c r="R8" s="136" t="s">
         <v>6</v>
       </c>
@@ -2901,10 +2922,10 @@
       <c r="T8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="138" t="s">
+      <c r="U8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="139"/>
+      <c r="V8" s="128"/>
       <c r="W8" s="136" t="s">
         <v>6</v>
       </c>
@@ -2912,17 +2933,17 @@
       <c r="Y8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="138" t="s">
+      <c r="Z8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="139"/>
-      <c r="AB8" s="132"/>
-      <c r="AC8" s="147"/>
-      <c r="AD8" s="126"/>
+      <c r="AA8" s="128"/>
+      <c r="AB8" s="146"/>
+      <c r="AC8" s="122"/>
+      <c r="AD8" s="125"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="141"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -2988,9 +3009,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="133"/>
-      <c r="AC9" s="148"/>
-      <c r="AD9" s="127"/>
+      <c r="AB9" s="147"/>
+      <c r="AC9" s="123"/>
+      <c r="AD9" s="126"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -5224,17 +5245,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AC6:AC9"/>
-    <mergeCell ref="AD6:AD9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:AA8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
@@ -5251,6 +5261,17 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="AC6:AC9"/>
+    <mergeCell ref="AD6:AD9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:AA8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5261,10 +5282,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD65"/>
+  <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M15" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5402,10 +5423,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="121" t="s">
+      <c r="A4" s="138" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="121"/>
+      <c r="B4" s="138"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -5471,94 +5492,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="122" t="s">
+      <c r="A6" s="139" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="125" t="s">
+      <c r="B6" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="128" t="s">
+      <c r="C6" s="142" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="129"/>
-      <c r="E6" s="129"/>
-      <c r="F6" s="129"/>
-      <c r="G6" s="129"/>
-      <c r="H6" s="129"/>
-      <c r="I6" s="129"/>
-      <c r="J6" s="129"/>
-      <c r="K6" s="129"/>
-      <c r="L6" s="129"/>
-      <c r="M6" s="129"/>
-      <c r="N6" s="129"/>
-      <c r="O6" s="129"/>
-      <c r="P6" s="129"/>
-      <c r="Q6" s="129"/>
-      <c r="R6" s="129"/>
-      <c r="S6" s="129"/>
-      <c r="T6" s="129"/>
-      <c r="U6" s="129"/>
-      <c r="V6" s="129"/>
-      <c r="W6" s="129"/>
-      <c r="X6" s="129"/>
-      <c r="Y6" s="129"/>
-      <c r="Z6" s="129"/>
-      <c r="AA6" s="130"/>
-      <c r="AB6" s="131" t="s">
+      <c r="D6" s="143"/>
+      <c r="E6" s="143"/>
+      <c r="F6" s="143"/>
+      <c r="G6" s="143"/>
+      <c r="H6" s="143"/>
+      <c r="I6" s="143"/>
+      <c r="J6" s="143"/>
+      <c r="K6" s="143"/>
+      <c r="L6" s="143"/>
+      <c r="M6" s="143"/>
+      <c r="N6" s="143"/>
+      <c r="O6" s="143"/>
+      <c r="P6" s="143"/>
+      <c r="Q6" s="143"/>
+      <c r="R6" s="143"/>
+      <c r="S6" s="143"/>
+      <c r="T6" s="143"/>
+      <c r="U6" s="143"/>
+      <c r="V6" s="143"/>
+      <c r="W6" s="143"/>
+      <c r="X6" s="143"/>
+      <c r="Y6" s="143"/>
+      <c r="Z6" s="143"/>
+      <c r="AA6" s="144"/>
+      <c r="AB6" s="145" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="146" t="s">
+      <c r="AC6" s="121" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="125" t="s">
+      <c r="AD6" s="124" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="123"/>
-      <c r="B7" s="126"/>
-      <c r="C7" s="140" t="s">
+      <c r="A7" s="140"/>
+      <c r="B7" s="125"/>
+      <c r="C7" s="129" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="141"/>
-      <c r="E7" s="141"/>
-      <c r="F7" s="141"/>
-      <c r="G7" s="142"/>
-      <c r="H7" s="143" t="s">
+      <c r="D7" s="130"/>
+      <c r="E7" s="130"/>
+      <c r="F7" s="130"/>
+      <c r="G7" s="131"/>
+      <c r="H7" s="132" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="145"/>
-      <c r="M7" s="140" t="s">
+      <c r="I7" s="133"/>
+      <c r="J7" s="133"/>
+      <c r="K7" s="133"/>
+      <c r="L7" s="148"/>
+      <c r="M7" s="129" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="141"/>
-      <c r="O7" s="141"/>
-      <c r="P7" s="141"/>
-      <c r="Q7" s="142"/>
-      <c r="R7" s="143" t="s">
+      <c r="N7" s="130"/>
+      <c r="O7" s="130"/>
+      <c r="P7" s="130"/>
+      <c r="Q7" s="131"/>
+      <c r="R7" s="132" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="144"/>
-      <c r="T7" s="144"/>
-      <c r="U7" s="144"/>
-      <c r="V7" s="144"/>
-      <c r="W7" s="140" t="s">
+      <c r="S7" s="133"/>
+      <c r="T7" s="133"/>
+      <c r="U7" s="133"/>
+      <c r="V7" s="133"/>
+      <c r="W7" s="129" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="141"/>
-      <c r="Y7" s="141"/>
-      <c r="Z7" s="141"/>
-      <c r="AA7" s="142"/>
-      <c r="AB7" s="132"/>
-      <c r="AC7" s="147"/>
-      <c r="AD7" s="126"/>
+      <c r="X7" s="130"/>
+      <c r="Y7" s="130"/>
+      <c r="Z7" s="130"/>
+      <c r="AA7" s="131"/>
+      <c r="AB7" s="146"/>
+      <c r="AC7" s="122"/>
+      <c r="AD7" s="125"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="123"/>
-      <c r="B8" s="126"/>
+      <c r="A8" s="140"/>
+      <c r="B8" s="125"/>
       <c r="C8" s="136" t="s">
         <v>6</v>
       </c>
@@ -5566,10 +5587,10 @@
       <c r="E8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="138" t="s">
+      <c r="F8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="139"/>
+      <c r="G8" s="128"/>
       <c r="H8" s="136" t="s">
         <v>6</v>
       </c>
@@ -5577,10 +5598,10 @@
       <c r="J8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="138" t="s">
+      <c r="K8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="139"/>
+      <c r="L8" s="128"/>
       <c r="M8" s="136" t="s">
         <v>6</v>
       </c>
@@ -5588,10 +5609,10 @@
       <c r="O8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="138" t="s">
+      <c r="P8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="139"/>
+      <c r="Q8" s="128"/>
       <c r="R8" s="136" t="s">
         <v>6</v>
       </c>
@@ -5599,10 +5620,10 @@
       <c r="T8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="138" t="s">
+      <c r="U8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="139"/>
+      <c r="V8" s="128"/>
       <c r="W8" s="136" t="s">
         <v>6</v>
       </c>
@@ -5610,17 +5631,17 @@
       <c r="Y8" s="134" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="138" t="s">
+      <c r="Z8" s="127" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="139"/>
-      <c r="AB8" s="132"/>
-      <c r="AC8" s="147"/>
-      <c r="AD8" s="126"/>
+      <c r="AA8" s="128"/>
+      <c r="AB8" s="146"/>
+      <c r="AC8" s="122"/>
+      <c r="AD8" s="125"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="124"/>
-      <c r="B9" s="127"/>
+      <c r="A9" s="141"/>
+      <c r="B9" s="126"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -5686,9 +5707,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="133"/>
-      <c r="AC9" s="148"/>
-      <c r="AD9" s="127"/>
+      <c r="AB9" s="147"/>
+      <c r="AC9" s="123"/>
+      <c r="AD9" s="126"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -5938,7 +5959,9 @@
       <c r="S16" s="101" t="s">
         <v>102</v>
       </c>
-      <c r="T16" s="42"/>
+      <c r="T16" s="42" t="s">
+        <v>119</v>
+      </c>
       <c r="U16" s="42"/>
       <c r="V16" s="38"/>
       <c r="W16" s="43"/>
@@ -5950,33 +5973,35 @@
       <c r="AC16" s="45"/>
       <c r="AD16" s="46"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:30" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="36"/>
-      <c r="B17" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="47"/>
-      <c r="D17" s="48"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="42"/>
       <c r="E17" s="42"/>
       <c r="F17" s="42"/>
       <c r="G17" s="38"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="48"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="101"/>
       <c r="J17" s="42"/>
-      <c r="K17" s="42"/>
+      <c r="K17" s="114"/>
       <c r="L17" s="38"/>
       <c r="M17" s="43"/>
-      <c r="N17" s="42"/>
+      <c r="N17" s="101"/>
       <c r="O17" s="101"/>
-      <c r="P17" s="42"/>
+      <c r="P17" s="114"/>
       <c r="Q17" s="38"/>
-      <c r="R17" s="41"/>
-      <c r="S17" s="42"/>
+      <c r="R17" s="43"/>
+      <c r="S17" s="101"/>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
       <c r="V17" s="38"/>
-      <c r="W17" s="43"/>
-      <c r="X17" s="42"/>
+      <c r="W17" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="X17" s="149" t="s">
+        <v>123</v>
+      </c>
       <c r="Y17" s="42"/>
       <c r="Z17" s="42"/>
       <c r="AA17" s="38"/>
@@ -5984,33 +6009,35 @@
       <c r="AC17" s="45"/>
       <c r="AD17" s="46"/>
     </row>
-    <row r="18" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:30" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="36"/>
-      <c r="B18" s="26" t="s">
-        <v>34</v>
-      </c>
-      <c r="C18" s="47"/>
-      <c r="D18" s="48"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="42"/>
       <c r="E18" s="42"/>
       <c r="F18" s="42"/>
       <c r="G18" s="38"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="48"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="101"/>
       <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
+      <c r="K18" s="114"/>
       <c r="L18" s="38"/>
       <c r="M18" s="43"/>
-      <c r="N18" s="42"/>
+      <c r="N18" s="101"/>
       <c r="O18" s="101"/>
-      <c r="P18" s="42"/>
+      <c r="P18" s="114"/>
       <c r="Q18" s="38"/>
-      <c r="R18" s="41"/>
-      <c r="S18" s="42"/>
+      <c r="R18" s="43"/>
+      <c r="S18" s="101"/>
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
       <c r="V18" s="38"/>
-      <c r="W18" s="43"/>
-      <c r="X18" s="42"/>
+      <c r="W18" s="43" t="s">
+        <v>122</v>
+      </c>
+      <c r="X18" s="101" t="s">
+        <v>123</v>
+      </c>
       <c r="Y18" s="42"/>
       <c r="Z18" s="42"/>
       <c r="AA18" s="38"/>
@@ -6021,7 +6048,7 @@
     <row r="19" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A19" s="36"/>
       <c r="B19" s="26" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="47"/>
       <c r="D19" s="48"/>
@@ -6052,10 +6079,10 @@
       <c r="AC19" s="45"/>
       <c r="AD19" s="46"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
       <c r="A20" s="36"/>
       <c r="B20" s="26" t="s">
-        <v>116</v>
+        <v>34</v>
       </c>
       <c r="C20" s="47"/>
       <c r="D20" s="48"/>
@@ -6086,9 +6113,11 @@
       <c r="AC20" s="45"/>
       <c r="AD20" s="46"/>
     </row>
-    <row r="21" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>
-      <c r="B21" s="26"/>
+      <c r="B21" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="C21" s="47"/>
       <c r="D21" s="48"/>
       <c r="E21" s="42"/>
@@ -6104,12 +6133,8 @@
       <c r="O21" s="101"/>
       <c r="P21" s="42"/>
       <c r="Q21" s="38"/>
-      <c r="R21" s="41" t="s">
-        <v>115</v>
-      </c>
-      <c r="S21" s="42" t="s">
-        <v>117</v>
-      </c>
+      <c r="R21" s="41"/>
+      <c r="S21" s="42"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="38"/>
@@ -6122,454 +6147,438 @@
       <c r="AC21" s="45"/>
       <c r="AD21" s="46"/>
     </row>
-    <row r="22" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A22" s="14" t="s">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="38"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="45"/>
+      <c r="AD22" s="46"/>
+    </row>
+    <row r="23" spans="1:30" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="26"/>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="101"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="41" t="s">
+        <v>115</v>
+      </c>
+      <c r="S23" s="42" t="s">
+        <v>117</v>
+      </c>
+      <c r="T23" s="42" t="s">
+        <v>118</v>
+      </c>
+      <c r="U23" s="42"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="45"/>
+      <c r="AD23" s="46"/>
+    </row>
+    <row r="24" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A24" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B24" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="107"/>
-      <c r="G22" s="105"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="17"/>
-      <c r="J22" s="21"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="105"/>
-      <c r="M22" s="20"/>
-      <c r="N22" s="21"/>
-      <c r="O22" s="21"/>
-      <c r="P22" s="106"/>
-      <c r="Q22" s="105"/>
-      <c r="R22" s="20"/>
-      <c r="S22" s="21"/>
-      <c r="T22" s="21"/>
-      <c r="U22" s="106"/>
-      <c r="V22" s="105"/>
-      <c r="W22" s="20"/>
-      <c r="X22" s="21"/>
-      <c r="Y22" s="21"/>
-      <c r="Z22" s="106"/>
-      <c r="AA22" s="105"/>
-      <c r="AB22" s="22"/>
-      <c r="AC22" s="23"/>
-      <c r="AD22" s="24"/>
-    </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A23" s="25">
+      <c r="C24" s="16"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="106"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="105"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="106"/>
+      <c r="L24" s="105"/>
+      <c r="M24" s="20"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="106"/>
+      <c r="Q24" s="105"/>
+      <c r="R24" s="20"/>
+      <c r="S24" s="21"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="106"/>
+      <c r="V24" s="105"/>
+      <c r="W24" s="20"/>
+      <c r="X24" s="21"/>
+      <c r="Y24" s="21"/>
+      <c r="Z24" s="106"/>
+      <c r="AA24" s="105"/>
+      <c r="AB24" s="22"/>
+      <c r="AC24" s="23"/>
+      <c r="AD24" s="24"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="25">
         <v>1</v>
       </c>
-      <c r="B23" s="26" t="s">
+      <c r="B25" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="53"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="50"/>
-      <c r="G23" s="108"/>
-      <c r="H23" s="52"/>
-      <c r="I23" s="53"/>
-      <c r="J23" s="32"/>
-      <c r="K23" s="51"/>
-      <c r="L23" s="108"/>
-      <c r="M23" s="30"/>
-      <c r="N23" s="32"/>
-      <c r="O23" s="32"/>
-      <c r="P23" s="51"/>
-      <c r="Q23" s="108"/>
-      <c r="R23" s="30"/>
-      <c r="S23" s="32"/>
-      <c r="T23" s="32"/>
-      <c r="U23" s="51"/>
-      <c r="V23" s="108"/>
-      <c r="W23" s="30"/>
-      <c r="X23" s="32"/>
-      <c r="Y23" s="32"/>
-      <c r="Z23" s="51"/>
-      <c r="AA23" s="108"/>
-      <c r="AB23" s="33"/>
-      <c r="AC23" s="34"/>
-      <c r="AD23" s="35"/>
-    </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A24" s="25">
+      <c r="C25" s="52"/>
+      <c r="D25" s="53"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="50"/>
+      <c r="G25" s="108"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="51"/>
+      <c r="L25" s="108"/>
+      <c r="M25" s="30"/>
+      <c r="N25" s="32"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="108"/>
+      <c r="R25" s="30"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="51"/>
+      <c r="V25" s="108"/>
+      <c r="W25" s="30"/>
+      <c r="X25" s="32"/>
+      <c r="Y25" s="32"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="108"/>
+      <c r="AB25" s="33"/>
+      <c r="AC25" s="34"/>
+      <c r="AD25" s="35"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A26" s="25">
         <v>2</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="B26" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="52"/>
-      <c r="D24" s="53"/>
-      <c r="E24" s="110"/>
-      <c r="F24" s="50"/>
-      <c r="G24" s="108"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="32"/>
-      <c r="K24" s="51"/>
-      <c r="L24" s="108"/>
-      <c r="M24" s="30"/>
-      <c r="N24" s="32"/>
-      <c r="O24" s="32"/>
-      <c r="P24" s="51"/>
-      <c r="Q24" s="108"/>
-      <c r="R24" s="30"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="32"/>
-      <c r="U24" s="51"/>
-      <c r="V24" s="108"/>
-      <c r="W24" s="30"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="32"/>
-      <c r="Z24" s="51"/>
-      <c r="AA24" s="108"/>
-      <c r="AB24" s="33"/>
-      <c r="AC24" s="34"/>
-      <c r="AD24" s="35"/>
-    </row>
-    <row r="25" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="37"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="68"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="38"/>
-      <c r="L25" s="38"/>
-      <c r="M25" s="43"/>
-      <c r="N25" s="42"/>
-      <c r="O25" s="42"/>
-      <c r="P25" s="38"/>
-      <c r="Q25" s="38"/>
-      <c r="R25" s="43"/>
-      <c r="S25" s="42"/>
-      <c r="T25" s="42"/>
-      <c r="U25" s="38"/>
-      <c r="V25" s="38"/>
-      <c r="W25" s="43"/>
-      <c r="X25" s="42"/>
-      <c r="Y25" s="42"/>
-      <c r="Z25" s="38"/>
-      <c r="AA25" s="38"/>
-      <c r="AB25" s="44"/>
-      <c r="AC25" s="45"/>
-      <c r="AD25" s="46"/>
-    </row>
-    <row r="26" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="36"/>
-      <c r="B26" s="37"/>
-      <c r="C26" s="47"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="51"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="38"/>
-      <c r="M26" s="43"/>
-      <c r="N26" s="42"/>
-      <c r="O26" s="42"/>
-      <c r="P26" s="38"/>
-      <c r="Q26" s="38"/>
-      <c r="R26" s="43"/>
-      <c r="S26" s="42"/>
-      <c r="T26" s="42"/>
-      <c r="U26" s="38"/>
-      <c r="V26" s="38"/>
-      <c r="W26" s="43"/>
-      <c r="X26" s="42"/>
-      <c r="Y26" s="42"/>
-      <c r="Z26" s="38"/>
-      <c r="AA26" s="38"/>
-      <c r="AB26" s="44"/>
-      <c r="AC26" s="45"/>
-      <c r="AD26" s="46"/>
-    </row>
-    <row r="27" spans="1:30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C26" s="52"/>
+      <c r="D26" s="53"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="108"/>
+      <c r="H26" s="52"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="32"/>
+      <c r="K26" s="51"/>
+      <c r="L26" s="108"/>
+      <c r="M26" s="30"/>
+      <c r="N26" s="32"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="108"/>
+      <c r="R26" s="30"/>
+      <c r="S26" s="32"/>
+      <c r="T26" s="32"/>
+      <c r="U26" s="51"/>
+      <c r="V26" s="108"/>
+      <c r="W26" s="30"/>
+      <c r="X26" s="32"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="108"/>
+      <c r="AB26" s="33"/>
+      <c r="AC26" s="34"/>
+      <c r="AD26" s="35"/>
+    </row>
+    <row r="27" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="36"/>
       <c r="B27" s="37"/>
-      <c r="C27" s="47"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="38"/>
-      <c r="F27" s="18"/>
-      <c r="G27" s="18"/>
-      <c r="H27" s="47"/>
-      <c r="I27" s="51"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="67"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="38"/>
+      <c r="G27" s="38"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="67"/>
       <c r="J27" s="42"/>
-      <c r="K27" s="18"/>
-      <c r="L27" s="18"/>
+      <c r="K27" s="38"/>
+      <c r="L27" s="38"/>
       <c r="M27" s="43"/>
       <c r="N27" s="42"/>
       <c r="O27" s="42"/>
-      <c r="P27" s="18"/>
-      <c r="Q27" s="18"/>
+      <c r="P27" s="38"/>
+      <c r="Q27" s="38"/>
       <c r="R27" s="43"/>
       <c r="S27" s="42"/>
       <c r="T27" s="42"/>
-      <c r="U27" s="18"/>
-      <c r="V27" s="18"/>
+      <c r="U27" s="38"/>
+      <c r="V27" s="38"/>
       <c r="W27" s="43"/>
       <c r="X27" s="42"/>
       <c r="Y27" s="42"/>
-      <c r="Z27" s="18"/>
-      <c r="AA27" s="18"/>
+      <c r="Z27" s="38"/>
+      <c r="AA27" s="38"/>
       <c r="AB27" s="44"/>
       <c r="AC27" s="45"/>
       <c r="AD27" s="46"/>
     </row>
     <row r="28" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="25"/>
-      <c r="B28" s="26"/>
-      <c r="C28" s="70"/>
-      <c r="D28" s="71"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="28"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="71"/>
-      <c r="J28" s="32"/>
-      <c r="K28" s="28"/>
-      <c r="L28" s="28"/>
-      <c r="M28" s="30"/>
-      <c r="N28" s="32"/>
-      <c r="O28" s="32"/>
-      <c r="P28" s="28"/>
-      <c r="Q28" s="28"/>
-      <c r="R28" s="30"/>
-      <c r="S28" s="32"/>
-      <c r="T28" s="32"/>
-      <c r="U28" s="28"/>
-      <c r="V28" s="28"/>
-      <c r="W28" s="30"/>
-      <c r="X28" s="32"/>
-      <c r="Y28" s="32"/>
-      <c r="Z28" s="28"/>
-      <c r="AA28" s="28"/>
-      <c r="AB28" s="33"/>
-      <c r="AC28" s="34"/>
-      <c r="AD28" s="35"/>
-    </row>
-    <row r="29" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="36"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="47"/>
+      <c r="D28" s="51"/>
+      <c r="E28" s="38"/>
+      <c r="F28" s="38"/>
+      <c r="G28" s="38"/>
+      <c r="H28" s="47"/>
+      <c r="I28" s="51"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="38"/>
+      <c r="L28" s="38"/>
+      <c r="M28" s="43"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="38"/>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="43"/>
+      <c r="S28" s="42"/>
+      <c r="T28" s="42"/>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38"/>
+      <c r="W28" s="43"/>
+      <c r="X28" s="42"/>
+      <c r="Y28" s="42"/>
+      <c r="Z28" s="38"/>
+      <c r="AA28" s="38"/>
+      <c r="AB28" s="44"/>
+      <c r="AC28" s="45"/>
+      <c r="AD28" s="46"/>
+    </row>
+    <row r="29" spans="1:30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="36"/>
       <c r="B29" s="37"/>
       <c r="C29" s="47"/>
       <c r="D29" s="51"/>
       <c r="E29" s="38"/>
-      <c r="F29" s="38"/>
-      <c r="G29" s="38"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
       <c r="H29" s="47"/>
       <c r="I29" s="51"/>
       <c r="J29" s="42"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="38"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
       <c r="M29" s="43"/>
       <c r="N29" s="42"/>
       <c r="O29" s="42"/>
-      <c r="P29" s="38"/>
-      <c r="Q29" s="38"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
       <c r="R29" s="43"/>
       <c r="S29" s="42"/>
       <c r="T29" s="42"/>
-      <c r="U29" s="38"/>
-      <c r="V29" s="38"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
       <c r="W29" s="43"/>
       <c r="X29" s="42"/>
       <c r="Y29" s="42"/>
-      <c r="Z29" s="38"/>
-      <c r="AA29" s="38"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
       <c r="AB29" s="44"/>
       <c r="AC29" s="45"/>
       <c r="AD29" s="46"/>
     </row>
-    <row r="30" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="C30" s="16"/>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
-      <c r="F30" s="17"/>
-      <c r="G30" s="105"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="17"/>
-      <c r="J30" s="21"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="20"/>
-      <c r="N30" s="21"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="17"/>
-      <c r="Q30" s="105"/>
-      <c r="R30" s="20"/>
-      <c r="S30" s="21"/>
-      <c r="T30" s="21"/>
-      <c r="U30" s="17"/>
-      <c r="V30" s="105"/>
-      <c r="W30" s="20"/>
-      <c r="X30" s="21"/>
-      <c r="Y30" s="21"/>
-      <c r="Z30" s="17"/>
-      <c r="AA30" s="105"/>
-      <c r="AB30" s="22"/>
-      <c r="AC30" s="23"/>
-      <c r="AD30" s="24"/>
-    </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A31" s="25"/>
-      <c r="B31" s="26" t="s">
-        <v>40</v>
-      </c>
+    <row r="30" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="28"/>
+      <c r="G30" s="28"/>
+      <c r="H30" s="70"/>
+      <c r="I30" s="71"/>
+      <c r="J30" s="32"/>
+      <c r="K30" s="28"/>
+      <c r="L30" s="28"/>
+      <c r="M30" s="30"/>
+      <c r="N30" s="32"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="28"/>
+      <c r="Q30" s="28"/>
+      <c r="R30" s="30"/>
+      <c r="S30" s="32"/>
+      <c r="T30" s="32"/>
+      <c r="U30" s="28"/>
+      <c r="V30" s="28"/>
+      <c r="W30" s="30"/>
+      <c r="X30" s="32"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="28"/>
+      <c r="AA30" s="28"/>
+      <c r="AB30" s="33"/>
+      <c r="AC30" s="34"/>
+      <c r="AD30" s="35"/>
+    </row>
+    <row r="31" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="47"/>
       <c r="D31" s="51"/>
-      <c r="E31" s="67"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="108"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
       <c r="H31" s="47"/>
       <c r="I31" s="51"/>
-      <c r="J31" s="32"/>
-      <c r="K31" s="51"/>
-      <c r="L31" s="108"/>
-      <c r="M31" s="30"/>
-      <c r="N31" s="32"/>
-      <c r="O31" s="32"/>
-      <c r="P31" s="51"/>
-      <c r="Q31" s="108"/>
-      <c r="R31" s="30"/>
-      <c r="S31" s="32"/>
-      <c r="T31" s="32"/>
-      <c r="U31" s="51"/>
-      <c r="V31" s="108"/>
-      <c r="W31" s="30"/>
-      <c r="X31" s="32"/>
-      <c r="Y31" s="32"/>
-      <c r="Z31" s="51"/>
-      <c r="AA31" s="108"/>
-      <c r="AB31" s="33"/>
-      <c r="AC31" s="34"/>
-      <c r="AD31" s="35"/>
-    </row>
-    <row r="32" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36"/>
-      <c r="B32" s="26" t="s">
-        <v>44</v>
-      </c>
-      <c r="C32" s="47"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="67"/>
-      <c r="F32" s="51"/>
-      <c r="G32" s="108"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="51"/>
-      <c r="J32" s="42"/>
-      <c r="K32" s="51"/>
-      <c r="L32" s="108"/>
-      <c r="M32" s="43"/>
-      <c r="N32" s="42"/>
-      <c r="O32" s="42"/>
-      <c r="P32" s="51"/>
-      <c r="Q32" s="108"/>
-      <c r="R32" s="43"/>
-      <c r="S32" s="42"/>
-      <c r="T32" s="42"/>
-      <c r="U32" s="51"/>
-      <c r="V32" s="108"/>
-      <c r="W32" s="43"/>
-      <c r="X32" s="42"/>
-      <c r="Y32" s="42"/>
-      <c r="Z32" s="51"/>
-      <c r="AA32" s="108"/>
-      <c r="AB32" s="44"/>
-      <c r="AC32" s="45"/>
-      <c r="AD32" s="46"/>
-    </row>
-    <row r="33" spans="1:30" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="36"/>
-      <c r="B33" s="26"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="38"/>
+      <c r="L31" s="38"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="38"/>
+      <c r="Q31" s="38"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="38"/>
+      <c r="V31" s="38"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="38"/>
+      <c r="AA31" s="38"/>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="45"/>
+      <c r="AD31" s="46"/>
+    </row>
+    <row r="32" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A32" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="16"/>
+      <c r="D32" s="17"/>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="105"/>
+      <c r="H32" s="16"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="105"/>
+      <c r="M32" s="20"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="17"/>
+      <c r="Q32" s="105"/>
+      <c r="R32" s="20"/>
+      <c r="S32" s="21"/>
+      <c r="T32" s="21"/>
+      <c r="U32" s="17"/>
+      <c r="V32" s="105"/>
+      <c r="W32" s="20"/>
+      <c r="X32" s="21"/>
+      <c r="Y32" s="21"/>
+      <c r="Z32" s="17"/>
+      <c r="AA32" s="105"/>
+      <c r="AB32" s="22"/>
+      <c r="AC32" s="23"/>
+      <c r="AD32" s="24"/>
+    </row>
+    <row r="33" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A33" s="25"/>
+      <c r="B33" s="26" t="s">
+        <v>40</v>
+      </c>
       <c r="C33" s="47"/>
       <c r="D33" s="51"/>
-      <c r="E33" s="114"/>
+      <c r="E33" s="67"/>
       <c r="F33" s="51"/>
       <c r="G33" s="108"/>
-      <c r="H33" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="I33" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="J33" s="42"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="32"/>
       <c r="K33" s="51"/>
       <c r="L33" s="108"/>
-      <c r="M33" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="N33" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="O33" s="42"/>
+      <c r="M33" s="30"/>
+      <c r="N33" s="32"/>
+      <c r="O33" s="32"/>
       <c r="P33" s="51"/>
       <c r="Q33" s="108"/>
-      <c r="R33" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="S33" s="51" t="s">
-        <v>102</v>
-      </c>
-      <c r="T33" s="42"/>
+      <c r="R33" s="30"/>
+      <c r="S33" s="32"/>
+      <c r="T33" s="32"/>
       <c r="U33" s="51"/>
       <c r="V33" s="108"/>
-      <c r="W33" s="43"/>
-      <c r="X33" s="42"/>
-      <c r="Y33" s="42"/>
+      <c r="W33" s="30"/>
+      <c r="X33" s="32"/>
+      <c r="Y33" s="32"/>
       <c r="Z33" s="51"/>
       <c r="AA33" s="108"/>
-      <c r="AB33" s="44"/>
-      <c r="AC33" s="45"/>
-      <c r="AD33" s="46"/>
+      <c r="AB33" s="33"/>
+      <c r="AC33" s="34"/>
+      <c r="AD33" s="35"/>
     </row>
     <row r="34" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="36"/>
-      <c r="B34" s="26"/>
+      <c r="B34" s="26" t="s">
+        <v>44</v>
+      </c>
       <c r="C34" s="47"/>
       <c r="D34" s="51"/>
-      <c r="E34" s="114"/>
+      <c r="E34" s="67"/>
       <c r="F34" s="51"/>
       <c r="G34" s="108"/>
-      <c r="H34" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="I34" s="51" t="s">
-        <v>102</v>
-      </c>
+      <c r="H34" s="47"/>
+      <c r="I34" s="51"/>
       <c r="J34" s="42"/>
       <c r="K34" s="51"/>
       <c r="L34" s="108"/>
-      <c r="M34" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="N34" s="51" t="s">
-        <v>102</v>
-      </c>
+      <c r="M34" s="43"/>
+      <c r="N34" s="42"/>
       <c r="O34" s="42"/>
       <c r="P34" s="51"/>
       <c r="Q34" s="108"/>
-      <c r="R34" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="S34" s="51" t="s">
-        <v>102</v>
-      </c>
+      <c r="R34" s="43"/>
+      <c r="S34" s="42"/>
       <c r="T34" s="42"/>
       <c r="U34" s="51"/>
       <c r="V34" s="108"/>
@@ -6582,41 +6591,57 @@
       <c r="AC34" s="45"/>
       <c r="AD34" s="46"/>
     </row>
-    <row r="35" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:30" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="36"/>
-      <c r="B35" s="26" t="s">
-        <v>45</v>
-      </c>
+      <c r="B35" s="26"/>
       <c r="C35" s="47"/>
       <c r="D35" s="51"/>
-      <c r="E35" s="67"/>
+      <c r="E35" s="114"/>
       <c r="F35" s="51"/>
-      <c r="G35" s="111"/>
-      <c r="H35" s="47"/>
-      <c r="I35" s="51"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="I35" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="J35" s="42"/>
-      <c r="K35" s="72"/>
-      <c r="L35" s="111"/>
-      <c r="M35" s="47"/>
-      <c r="N35" s="51"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="108"/>
+      <c r="M35" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="N35" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="O35" s="42"/>
-      <c r="P35" s="72"/>
-      <c r="Q35" s="111"/>
-      <c r="R35" s="47"/>
-      <c r="S35" s="51"/>
-      <c r="T35" s="42"/>
-      <c r="U35" s="72"/>
-      <c r="V35" s="111"/>
-      <c r="W35" s="43"/>
-      <c r="X35" s="42"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="S35" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="T35" s="42" t="s">
+        <v>120</v>
+      </c>
+      <c r="U35" s="51"/>
+      <c r="V35" s="108"/>
+      <c r="W35" s="47" t="s">
+        <v>62</v>
+      </c>
+      <c r="X35" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="Y35" s="42"/>
-      <c r="Z35" s="72"/>
-      <c r="AA35" s="111"/>
+      <c r="Z35" s="51"/>
+      <c r="AA35" s="108"/>
       <c r="AB35" s="44"/>
       <c r="AC35" s="45"/>
       <c r="AD35" s="46"/>
     </row>
-    <row r="36" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="36"/>
       <c r="B36" s="26"/>
       <c r="C36" s="47"/>
@@ -6625,7 +6650,7 @@
       <c r="F36" s="51"/>
       <c r="G36" s="108"/>
       <c r="H36" s="47" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="I36" s="51" t="s">
         <v>102</v>
@@ -6634,7 +6659,7 @@
       <c r="K36" s="51"/>
       <c r="L36" s="108"/>
       <c r="M36" s="47" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="N36" s="51" t="s">
         <v>102</v>
@@ -6643,16 +6668,22 @@
       <c r="P36" s="51"/>
       <c r="Q36" s="108"/>
       <c r="R36" s="47" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="S36" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="T36" s="42"/>
+      <c r="T36" s="42" t="s">
+        <v>120</v>
+      </c>
       <c r="U36" s="51"/>
       <c r="V36" s="108"/>
-      <c r="W36" s="43"/>
-      <c r="X36" s="42"/>
+      <c r="W36" s="47" t="s">
+        <v>61</v>
+      </c>
+      <c r="X36" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="Y36" s="42"/>
       <c r="Z36" s="51"/>
       <c r="AA36" s="108"/>
@@ -6663,66 +6694,80 @@
     <row r="37" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="36"/>
       <c r="B37" s="26" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C37" s="47"/>
       <c r="D37" s="51"/>
-      <c r="E37" s="51"/>
+      <c r="E37" s="67"/>
       <c r="F37" s="51"/>
-      <c r="G37" s="108"/>
+      <c r="G37" s="111"/>
       <c r="H37" s="47"/>
       <c r="I37" s="51"/>
       <c r="J37" s="42"/>
-      <c r="K37" s="51"/>
-      <c r="L37" s="108"/>
-      <c r="M37" s="43"/>
-      <c r="N37" s="42"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="51"/>
       <c r="O37" s="42"/>
-      <c r="P37" s="51"/>
-      <c r="Q37" s="108"/>
-      <c r="R37" s="43"/>
-      <c r="S37" s="42"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="111"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="51"/>
       <c r="T37" s="42"/>
-      <c r="U37" s="51"/>
-      <c r="V37" s="108"/>
-      <c r="W37" s="43"/>
-      <c r="X37" s="42"/>
+      <c r="U37" s="72"/>
+      <c r="V37" s="111"/>
+      <c r="W37" s="47"/>
+      <c r="X37" s="51"/>
       <c r="Y37" s="42"/>
-      <c r="Z37" s="51"/>
-      <c r="AA37" s="108"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="111"/>
       <c r="AB37" s="44"/>
       <c r="AC37" s="45"/>
       <c r="AD37" s="46"/>
     </row>
     <row r="38" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="36"/>
-      <c r="B38" s="120"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="116"/>
-      <c r="E38" s="42"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="47"/>
+      <c r="D38" s="51"/>
+      <c r="E38" s="114"/>
       <c r="F38" s="51"/>
       <c r="G38" s="108"/>
-      <c r="H38" s="43" t="s">
-        <v>112</v>
-      </c>
-      <c r="I38" s="116" t="s">
-        <v>111</v>
+      <c r="H38" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="I38" s="51" t="s">
+        <v>102</v>
       </c>
       <c r="J38" s="42"/>
       <c r="K38" s="51"/>
       <c r="L38" s="108"/>
-      <c r="M38" s="43"/>
-      <c r="N38" s="42"/>
+      <c r="M38" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="N38" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="O38" s="42"/>
       <c r="P38" s="51"/>
       <c r="Q38" s="108"/>
-      <c r="R38" s="43"/>
-      <c r="S38" s="42"/>
-      <c r="T38" s="42"/>
+      <c r="R38" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="S38" s="51" t="s">
+        <v>102</v>
+      </c>
+      <c r="T38" s="42" t="s">
+        <v>120</v>
+      </c>
       <c r="U38" s="51"/>
       <c r="V38" s="108"/>
-      <c r="W38" s="43"/>
-      <c r="X38" s="42"/>
+      <c r="W38" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="X38" s="51" t="s">
+        <v>102</v>
+      </c>
       <c r="Y38" s="42"/>
       <c r="Z38" s="51"/>
       <c r="AA38" s="108"/>
@@ -6732,268 +6777,292 @@
     </row>
     <row r="39" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="36"/>
-      <c r="B39" s="119"/>
-      <c r="C39" s="43"/>
-      <c r="D39" s="116"/>
-      <c r="E39" s="114"/>
-      <c r="F39" s="115"/>
+      <c r="B39" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
       <c r="G39" s="108"/>
-      <c r="H39" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="I39" s="116" t="s">
-        <v>111</v>
-      </c>
+      <c r="H39" s="47"/>
+      <c r="I39" s="51"/>
       <c r="J39" s="42"/>
-      <c r="K39" s="115"/>
+      <c r="K39" s="51"/>
       <c r="L39" s="108"/>
-      <c r="M39" s="47"/>
-      <c r="N39" s="51"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="42"/>
       <c r="O39" s="42"/>
-      <c r="P39" s="115"/>
+      <c r="P39" s="51"/>
       <c r="Q39" s="108"/>
-      <c r="R39" s="47"/>
-      <c r="S39" s="51"/>
-      <c r="T39" s="114"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
       <c r="U39" s="51"/>
       <c r="V39" s="108"/>
       <c r="W39" s="43"/>
       <c r="X39" s="42"/>
-      <c r="Y39" s="114"/>
+      <c r="Y39" s="42"/>
       <c r="Z39" s="51"/>
       <c r="AA39" s="108"/>
       <c r="AB39" s="44"/>
       <c r="AC39" s="45"/>
       <c r="AD39" s="46"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A40" s="75"/>
-      <c r="B40" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="77"/>
-      <c r="D40" s="76"/>
-      <c r="E40" s="76"/>
-      <c r="F40" s="76"/>
-      <c r="G40" s="76"/>
-      <c r="H40" s="76"/>
-      <c r="I40" s="76"/>
-      <c r="J40" s="76"/>
-      <c r="K40" s="76"/>
-      <c r="L40" s="76"/>
-      <c r="M40" s="76"/>
-      <c r="N40" s="76"/>
-      <c r="O40" s="76"/>
-      <c r="P40" s="76"/>
-      <c r="Q40" s="76"/>
-      <c r="R40" s="76"/>
-      <c r="S40" s="76"/>
-      <c r="T40" s="76"/>
-      <c r="U40" s="76"/>
-      <c r="V40" s="76"/>
-      <c r="W40" s="76"/>
-      <c r="X40" s="76"/>
-      <c r="Y40" s="76"/>
-      <c r="Z40" s="76"/>
-      <c r="AA40" s="76"/>
-      <c r="AB40" s="76"/>
-      <c r="AC40" s="76"/>
-      <c r="AD40" s="78"/>
-    </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="36"/>
+      <c r="B40" s="120"/>
+      <c r="C40" s="43"/>
+      <c r="D40" s="116"/>
+      <c r="E40" s="42"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="I40" s="116" t="s">
+        <v>111</v>
+      </c>
+      <c r="J40" s="42"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="108"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="51"/>
+      <c r="V40" s="108"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="108"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="45"/>
+      <c r="AD40" s="46"/>
+    </row>
+    <row r="41" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="36"/>
-      <c r="B41" s="37"/>
-      <c r="C41" s="47"/>
-      <c r="D41" s="51"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="113"/>
+      <c r="B41" s="119"/>
+      <c r="C41" s="43"/>
+      <c r="D41" s="116"/>
+      <c r="E41" s="114"/>
+      <c r="F41" s="115"/>
       <c r="G41" s="108"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="51"/>
+      <c r="H41" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="I41" s="116" t="s">
+        <v>111</v>
+      </c>
       <c r="J41" s="42"/>
-      <c r="K41" s="113"/>
+      <c r="K41" s="115"/>
       <c r="L41" s="108"/>
-      <c r="M41" s="43" t="s">
-        <v>114</v>
-      </c>
-      <c r="N41" s="101" t="s">
-        <v>100</v>
-      </c>
+      <c r="M41" s="47"/>
+      <c r="N41" s="51"/>
       <c r="O41" s="42"/>
-      <c r="P41" s="113"/>
+      <c r="P41" s="115"/>
       <c r="Q41" s="108"/>
-      <c r="R41" s="43"/>
-      <c r="S41" s="42"/>
-      <c r="T41" s="42"/>
-      <c r="U41" s="113"/>
+      <c r="R41" s="47"/>
+      <c r="S41" s="51"/>
+      <c r="T41" s="114"/>
+      <c r="U41" s="51"/>
       <c r="V41" s="108"/>
       <c r="W41" s="43"/>
       <c r="X41" s="42"/>
-      <c r="Y41" s="42"/>
-      <c r="Z41" s="113"/>
+      <c r="Y41" s="114"/>
+      <c r="Z41" s="51"/>
       <c r="AA41" s="108"/>
       <c r="AB41" s="44"/>
       <c r="AC41" s="45"/>
       <c r="AD41" s="46"/>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A42" s="36"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="47"/>
-      <c r="D42" s="51"/>
-      <c r="E42" s="67"/>
-      <c r="F42" s="51"/>
-      <c r="G42" s="108"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="51"/>
-      <c r="J42" s="42"/>
-      <c r="K42" s="51"/>
-      <c r="L42" s="108"/>
-      <c r="M42" s="43"/>
-      <c r="N42" s="42"/>
-      <c r="O42" s="42"/>
-      <c r="P42" s="51"/>
-      <c r="Q42" s="108"/>
-      <c r="R42" s="43"/>
-      <c r="S42" s="42"/>
-      <c r="T42" s="42"/>
-      <c r="U42" s="51"/>
-      <c r="V42" s="108"/>
-      <c r="W42" s="43"/>
-      <c r="X42" s="42"/>
-      <c r="Y42" s="42"/>
-      <c r="Z42" s="51"/>
-      <c r="AA42" s="108"/>
-      <c r="AB42" s="44"/>
-      <c r="AC42" s="45"/>
-      <c r="AD42" s="46"/>
+      <c r="A42" s="75"/>
+      <c r="B42" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="77"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="76"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
+      <c r="V42" s="76"/>
+      <c r="W42" s="76"/>
+      <c r="X42" s="76"/>
+      <c r="Y42" s="76"/>
+      <c r="Z42" s="76"/>
+      <c r="AA42" s="76"/>
+      <c r="AB42" s="76"/>
+      <c r="AC42" s="76"/>
+      <c r="AD42" s="78"/>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A43" s="36"/>
       <c r="B43" s="37"/>
       <c r="C43" s="47"/>
       <c r="D43" s="51"/>
-      <c r="E43" s="51"/>
-      <c r="F43" s="51"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="113"/>
       <c r="G43" s="108"/>
-      <c r="H43" s="50"/>
+      <c r="H43" s="74"/>
       <c r="I43" s="51"/>
       <c r="J43" s="42"/>
-      <c r="K43" s="51"/>
+      <c r="K43" s="113"/>
       <c r="L43" s="108"/>
-      <c r="M43" s="43"/>
-      <c r="N43" s="42"/>
+      <c r="M43" s="43" t="s">
+        <v>114</v>
+      </c>
+      <c r="N43" s="101" t="s">
+        <v>100</v>
+      </c>
       <c r="O43" s="42"/>
-      <c r="P43" s="51"/>
+      <c r="P43" s="113"/>
       <c r="Q43" s="108"/>
       <c r="R43" s="43"/>
       <c r="S43" s="42"/>
       <c r="T43" s="42"/>
-      <c r="U43" s="51"/>
+      <c r="U43" s="113"/>
       <c r="V43" s="108"/>
       <c r="W43" s="43"/>
       <c r="X43" s="42"/>
       <c r="Y43" s="42"/>
-      <c r="Z43" s="51"/>
+      <c r="Z43" s="113"/>
       <c r="AA43" s="108"/>
       <c r="AB43" s="44"/>
       <c r="AC43" s="45"/>
       <c r="AD43" s="46"/>
     </row>
-    <row r="44" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="79"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="81"/>
-      <c r="D44" s="82"/>
-      <c r="E44" s="82"/>
-      <c r="F44" s="82"/>
-      <c r="G44" s="88"/>
-      <c r="H44" s="83"/>
-      <c r="I44" s="82"/>
-      <c r="J44" s="85"/>
-      <c r="K44" s="82"/>
-      <c r="L44" s="88"/>
-      <c r="M44" s="84"/>
-      <c r="N44" s="85"/>
-      <c r="O44" s="85"/>
-      <c r="P44" s="82"/>
-      <c r="Q44" s="88"/>
-      <c r="R44" s="84"/>
-      <c r="S44" s="85"/>
-      <c r="T44" s="85"/>
-      <c r="U44" s="82"/>
-      <c r="V44" s="88"/>
-      <c r="W44" s="84"/>
-      <c r="X44" s="85"/>
-      <c r="Y44" s="85"/>
-      <c r="Z44" s="82"/>
-      <c r="AA44" s="88"/>
-      <c r="AB44" s="86"/>
-      <c r="AC44" s="87"/>
-      <c r="AD44" s="88"/>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="36"/>
+      <c r="B44" s="37"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="42"/>
+      <c r="O44" s="42"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="108"/>
+      <c r="R44" s="43"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="51"/>
+      <c r="V44" s="108"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="51"/>
+      <c r="AA44" s="108"/>
+      <c r="AB44" s="44"/>
+      <c r="AC44" s="45"/>
+      <c r="AD44" s="46"/>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A45" s="63"/>
-      <c r="B45" s="64"/>
-      <c r="AB45" s="63"/>
-      <c r="AC45" s="63"/>
-    </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A46" s="63"/>
-      <c r="B46" s="64"/>
-      <c r="AB46" s="63"/>
-      <c r="AC46" s="63"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="37"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="51"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="108"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="42"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="108"/>
+      <c r="W45" s="43"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="51"/>
+      <c r="AA45" s="108"/>
+      <c r="AB45" s="44"/>
+      <c r="AC45" s="45"/>
+      <c r="AD45" s="46"/>
+    </row>
+    <row r="46" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="79"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
+      <c r="P46" s="82"/>
+      <c r="Q46" s="88"/>
+      <c r="R46" s="84"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="85"/>
+      <c r="U46" s="82"/>
+      <c r="V46" s="88"/>
+      <c r="W46" s="84"/>
+      <c r="X46" s="85"/>
+      <c r="Y46" s="85"/>
+      <c r="Z46" s="82"/>
+      <c r="AA46" s="88"/>
+      <c r="AB46" s="86"/>
+      <c r="AC46" s="87"/>
+      <c r="AD46" s="88"/>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A47" s="89"/>
-      <c r="B47" s="90" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="91"/>
-      <c r="D47" s="91"/>
-      <c r="E47" s="91"/>
-      <c r="H47" s="91"/>
-      <c r="I47" s="91"/>
-      <c r="J47" s="91"/>
-      <c r="M47" s="91"/>
-      <c r="N47" s="91"/>
-      <c r="O47" s="89"/>
-      <c r="R47" s="89"/>
-      <c r="S47" s="91"/>
-      <c r="T47" s="91"/>
-      <c r="W47" s="89"/>
-      <c r="X47" s="91"/>
-      <c r="Y47" s="91"/>
-      <c r="AB47" s="91"/>
-      <c r="AC47" s="91"/>
-      <c r="AD47" s="91"/>
+      <c r="A47" s="63"/>
+      <c r="B47" s="64"/>
+      <c r="AB47" s="63"/>
+      <c r="AC47" s="63"/>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A48" s="89"/>
-      <c r="B48" s="90"/>
-      <c r="C48" s="91"/>
-      <c r="D48" s="91"/>
-      <c r="E48" s="91"/>
-      <c r="H48" s="91"/>
-      <c r="I48" s="91"/>
-      <c r="J48" s="91"/>
-      <c r="M48" s="91"/>
-      <c r="N48" s="91"/>
-      <c r="O48" s="89"/>
-      <c r="R48" s="89"/>
-      <c r="S48" s="91"/>
-      <c r="T48" s="91"/>
-      <c r="W48" s="89"/>
-      <c r="X48" s="91"/>
-      <c r="Y48" s="91"/>
-      <c r="AB48" s="91"/>
-      <c r="AC48" s="91"/>
-      <c r="AD48" s="91"/>
+      <c r="A48" s="63"/>
+      <c r="B48" s="64"/>
+      <c r="AB48" s="63"/>
+      <c r="AC48" s="63"/>
     </row>
     <row r="49" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A49" s="89"/>
-      <c r="B49" s="92" t="s">
-        <v>21</v>
+      <c r="B49" s="90" t="s">
+        <v>20</v>
       </c>
       <c r="C49" s="91"/>
       <c r="D49" s="91"/>
@@ -7016,10 +7085,8 @@
     </row>
     <row r="50" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A50" s="89"/>
-      <c r="B50" s="92" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="92"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="91"/>
       <c r="D50" s="91"/>
       <c r="E50" s="91"/>
       <c r="H50" s="91"/>
@@ -7039,91 +7106,77 @@
       <c r="AD50" s="91"/>
     </row>
     <row r="51" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A51" s="63"/>
-      <c r="B51" s="93"/>
-      <c r="C51" s="94"/>
-      <c r="D51" s="94"/>
-      <c r="E51" s="94"/>
-      <c r="H51" s="94"/>
-      <c r="I51" s="94"/>
-      <c r="J51" s="94"/>
-      <c r="M51" s="94"/>
-      <c r="N51" s="94"/>
-      <c r="O51" s="94"/>
-      <c r="R51" s="94"/>
-      <c r="S51" s="94"/>
-      <c r="T51" s="94"/>
-      <c r="W51" s="94"/>
-      <c r="X51" s="94"/>
-      <c r="Y51" s="94"/>
-      <c r="AB51" s="63"/>
-      <c r="AC51" s="63"/>
+      <c r="A51" s="89"/>
+      <c r="B51" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="M51" s="91"/>
+      <c r="N51" s="91"/>
+      <c r="O51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="91"/>
+      <c r="T51" s="91"/>
+      <c r="W51" s="89"/>
+      <c r="X51" s="91"/>
+      <c r="Y51" s="91"/>
+      <c r="AB51" s="91"/>
+      <c r="AC51" s="91"/>
+      <c r="AD51" s="91"/>
     </row>
     <row r="52" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A52" s="63"/>
-      <c r="B52" s="93"/>
-      <c r="C52" s="94"/>
-      <c r="D52" s="94"/>
-      <c r="E52" s="94"/>
-      <c r="F52" s="91"/>
-      <c r="G52" s="91"/>
-      <c r="H52" s="94"/>
-      <c r="I52" s="94"/>
-      <c r="J52" s="94"/>
-      <c r="K52" s="91"/>
-      <c r="L52" s="91"/>
-      <c r="M52" s="94"/>
-      <c r="N52" s="94"/>
-      <c r="O52" s="94"/>
-      <c r="P52" s="91"/>
-      <c r="Q52" s="91"/>
-      <c r="R52" s="94"/>
-      <c r="S52" s="94"/>
-      <c r="T52" s="94"/>
-      <c r="U52" s="91"/>
-      <c r="V52" s="91"/>
-      <c r="W52" s="94"/>
-      <c r="X52" s="94"/>
-      <c r="Y52" s="94"/>
-      <c r="Z52" s="91"/>
-      <c r="AA52" s="91"/>
-      <c r="AB52" s="63"/>
-      <c r="AC52" s="63"/>
+      <c r="A52" s="89"/>
+      <c r="B52" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="92"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="M52" s="91"/>
+      <c r="N52" s="91"/>
+      <c r="O52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="91"/>
+      <c r="T52" s="91"/>
+      <c r="W52" s="89"/>
+      <c r="X52" s="91"/>
+      <c r="Y52" s="91"/>
+      <c r="AB52" s="91"/>
+      <c r="AC52" s="91"/>
+      <c r="AD52" s="91"/>
     </row>
     <row r="53" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A53" s="63"/>
-      <c r="B53" s="95"/>
+      <c r="B53" s="93"/>
       <c r="C53" s="94"/>
       <c r="D53" s="94"/>
       <c r="E53" s="94"/>
-      <c r="F53" s="91"/>
-      <c r="G53" s="91"/>
       <c r="H53" s="94"/>
       <c r="I53" s="94"/>
       <c r="J53" s="94"/>
-      <c r="K53" s="91"/>
-      <c r="L53" s="91"/>
       <c r="M53" s="94"/>
       <c r="N53" s="94"/>
       <c r="O53" s="94"/>
-      <c r="P53" s="91"/>
-      <c r="Q53" s="91"/>
       <c r="R53" s="94"/>
       <c r="S53" s="94"/>
       <c r="T53" s="94"/>
-      <c r="U53" s="91"/>
-      <c r="V53" s="91"/>
       <c r="W53" s="94"/>
       <c r="X53" s="94"/>
       <c r="Y53" s="94"/>
-      <c r="Z53" s="91"/>
-      <c r="AA53" s="91"/>
       <c r="AB53" s="63"/>
       <c r="AC53" s="63"/>
     </row>
     <row r="54" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A54" s="63"/>
-      <c r="B54" s="95"/>
+      <c r="B54" s="93"/>
       <c r="C54" s="94"/>
       <c r="D54" s="94"/>
       <c r="E54" s="94"/>
@@ -7185,125 +7238,123 @@
     </row>
     <row r="56" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A56" s="63"/>
-      <c r="B56" s="93"/>
+      <c r="B56" s="95"/>
       <c r="C56" s="94"/>
       <c r="D56" s="94"/>
       <c r="E56" s="94"/>
-      <c r="F56" s="94"/>
-      <c r="G56" s="94"/>
+      <c r="F56" s="91"/>
+      <c r="G56" s="91"/>
       <c r="H56" s="94"/>
       <c r="I56" s="94"/>
       <c r="J56" s="94"/>
-      <c r="K56" s="94"/>
-      <c r="L56" s="94"/>
+      <c r="K56" s="91"/>
+      <c r="L56" s="91"/>
       <c r="M56" s="94"/>
       <c r="N56" s="94"/>
       <c r="O56" s="94"/>
-      <c r="P56" s="94"/>
-      <c r="Q56" s="94"/>
+      <c r="P56" s="91"/>
+      <c r="Q56" s="91"/>
       <c r="R56" s="94"/>
       <c r="S56" s="94"/>
       <c r="T56" s="94"/>
-      <c r="U56" s="94"/>
-      <c r="V56" s="94"/>
+      <c r="U56" s="91"/>
+      <c r="V56" s="91"/>
       <c r="W56" s="94"/>
       <c r="X56" s="94"/>
       <c r="Y56" s="94"/>
-      <c r="Z56" s="94"/>
-      <c r="AA56" s="94"/>
+      <c r="Z56" s="91"/>
+      <c r="AA56" s="91"/>
       <c r="AB56" s="63"/>
       <c r="AC56" s="63"/>
     </row>
     <row r="57" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A57" s="63"/>
-      <c r="B57" s="93"/>
+      <c r="B57" s="95"/>
       <c r="C57" s="94"/>
       <c r="D57" s="94"/>
       <c r="E57" s="94"/>
-      <c r="F57" s="94"/>
-      <c r="G57" s="94"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
       <c r="H57" s="94"/>
       <c r="I57" s="94"/>
       <c r="J57" s="94"/>
-      <c r="K57" s="94"/>
-      <c r="L57" s="94"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="91"/>
       <c r="M57" s="94"/>
       <c r="N57" s="94"/>
       <c r="O57" s="94"/>
-      <c r="P57" s="94"/>
-      <c r="Q57" s="94"/>
+      <c r="P57" s="91"/>
+      <c r="Q57" s="91"/>
       <c r="R57" s="94"/>
       <c r="S57" s="94"/>
       <c r="T57" s="94"/>
-      <c r="U57" s="94"/>
-      <c r="V57" s="94"/>
+      <c r="U57" s="91"/>
+      <c r="V57" s="91"/>
       <c r="W57" s="94"/>
       <c r="X57" s="94"/>
       <c r="Y57" s="94"/>
-      <c r="Z57" s="94"/>
-      <c r="AA57" s="94"/>
-      <c r="AB57" s="96"/>
-      <c r="AC57" s="96"/>
-      <c r="AD57" s="97"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="63"/>
+      <c r="AC57" s="63"/>
     </row>
     <row r="58" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A58" s="63"/>
-      <c r="B58" s="97"/>
-      <c r="C58" s="97"/>
-      <c r="D58" s="97"/>
-      <c r="E58" s="97"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="94"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="94"/>
       <c r="F58" s="94"/>
       <c r="G58" s="94"/>
-      <c r="H58" s="97"/>
-      <c r="I58" s="97"/>
-      <c r="J58" s="97"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+      <c r="J58" s="94"/>
       <c r="K58" s="94"/>
       <c r="L58" s="94"/>
-      <c r="M58" s="97"/>
-      <c r="N58" s="97"/>
-      <c r="O58" s="97"/>
+      <c r="M58" s="94"/>
+      <c r="N58" s="94"/>
+      <c r="O58" s="94"/>
       <c r="P58" s="94"/>
       <c r="Q58" s="94"/>
-      <c r="R58" s="97"/>
-      <c r="S58" s="97"/>
-      <c r="T58" s="97"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="94"/>
+      <c r="T58" s="94"/>
       <c r="U58" s="94"/>
       <c r="V58" s="94"/>
-      <c r="W58" s="97"/>
-      <c r="X58" s="97"/>
-      <c r="Y58" s="97"/>
+      <c r="W58" s="94"/>
+      <c r="X58" s="94"/>
+      <c r="Y58" s="94"/>
       <c r="Z58" s="94"/>
       <c r="AA58" s="94"/>
-      <c r="AB58" s="96"/>
-      <c r="AC58" s="96"/>
-      <c r="AD58" s="97"/>
+      <c r="AB58" s="63"/>
+      <c r="AC58" s="63"/>
     </row>
     <row r="59" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A59" s="63"/>
-      <c r="B59" s="98"/>
-      <c r="C59" s="97"/>
-      <c r="D59" s="97"/>
-      <c r="E59" s="97"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
       <c r="F59" s="94"/>
       <c r="G59" s="94"/>
-      <c r="H59" s="97"/>
-      <c r="I59" s="97"/>
-      <c r="J59" s="97"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="94"/>
       <c r="K59" s="94"/>
       <c r="L59" s="94"/>
-      <c r="M59" s="97"/>
-      <c r="N59" s="97"/>
-      <c r="O59" s="97"/>
+      <c r="M59" s="94"/>
+      <c r="N59" s="94"/>
+      <c r="O59" s="94"/>
       <c r="P59" s="94"/>
       <c r="Q59" s="94"/>
-      <c r="R59" s="97"/>
-      <c r="S59" s="97"/>
-      <c r="T59" s="97"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="94"/>
+      <c r="T59" s="94"/>
       <c r="U59" s="94"/>
       <c r="V59" s="94"/>
-      <c r="W59" s="97"/>
-      <c r="X59" s="97"/>
-      <c r="Y59" s="97"/>
+      <c r="W59" s="94"/>
+      <c r="X59" s="94"/>
+      <c r="Y59" s="94"/>
       <c r="Z59" s="94"/>
       <c r="AA59" s="94"/>
       <c r="AB59" s="96"/>
@@ -7312,7 +7363,7 @@
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="63"/>
-      <c r="B60" s="98"/>
+      <c r="B60" s="97"/>
       <c r="C60" s="97"/>
       <c r="D60" s="97"/>
       <c r="E60" s="97"/>
@@ -7344,55 +7395,95 @@
     </row>
     <row r="61" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A61" s="63"/>
-      <c r="B61" s="64"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
       <c r="F61" s="94"/>
       <c r="G61" s="94"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="97"/>
       <c r="K61" s="94"/>
       <c r="L61" s="94"/>
+      <c r="M61" s="97"/>
+      <c r="N61" s="97"/>
+      <c r="O61" s="97"/>
       <c r="P61" s="94"/>
       <c r="Q61" s="94"/>
+      <c r="R61" s="97"/>
+      <c r="S61" s="97"/>
+      <c r="T61" s="97"/>
       <c r="U61" s="94"/>
       <c r="V61" s="94"/>
+      <c r="W61" s="97"/>
+      <c r="X61" s="97"/>
+      <c r="Y61" s="97"/>
       <c r="Z61" s="94"/>
       <c r="AA61" s="94"/>
-      <c r="AB61" s="63"/>
-      <c r="AC61" s="63"/>
+      <c r="AB61" s="96"/>
+      <c r="AC61" s="96"/>
+      <c r="AD61" s="97"/>
     </row>
     <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="63"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="97"/>
+      <c r="E62" s="97"/>
       <c r="F62" s="94"/>
       <c r="G62" s="94"/>
+      <c r="H62" s="97"/>
+      <c r="I62" s="97"/>
+      <c r="J62" s="97"/>
       <c r="K62" s="94"/>
       <c r="L62" s="94"/>
+      <c r="M62" s="97"/>
+      <c r="N62" s="97"/>
+      <c r="O62" s="97"/>
       <c r="P62" s="94"/>
       <c r="Q62" s="94"/>
+      <c r="R62" s="97"/>
+      <c r="S62" s="97"/>
+      <c r="T62" s="97"/>
       <c r="U62" s="94"/>
       <c r="V62" s="94"/>
+      <c r="W62" s="97"/>
+      <c r="X62" s="97"/>
+      <c r="Y62" s="97"/>
       <c r="Z62" s="94"/>
       <c r="AA62" s="94"/>
+      <c r="AB62" s="96"/>
+      <c r="AC62" s="96"/>
+      <c r="AD62" s="97"/>
     </row>
     <row r="63" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="F63" s="97"/>
-      <c r="G63" s="97"/>
-      <c r="K63" s="97"/>
-      <c r="L63" s="97"/>
-      <c r="P63" s="97"/>
-      <c r="Q63" s="97"/>
-      <c r="U63" s="97"/>
-      <c r="V63" s="97"/>
-      <c r="Z63" s="97"/>
-      <c r="AA63" s="97"/>
+      <c r="A63" s="63"/>
+      <c r="B63" s="64"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="94"/>
+      <c r="K63" s="94"/>
+      <c r="L63" s="94"/>
+      <c r="P63" s="94"/>
+      <c r="Q63" s="94"/>
+      <c r="U63" s="94"/>
+      <c r="V63" s="94"/>
+      <c r="Z63" s="94"/>
+      <c r="AA63" s="94"/>
+      <c r="AB63" s="63"/>
+      <c r="AC63" s="63"/>
     </row>
     <row r="64" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="F64" s="97"/>
-      <c r="G64" s="97"/>
-      <c r="K64" s="97"/>
-      <c r="L64" s="97"/>
-      <c r="P64" s="97"/>
-      <c r="Q64" s="97"/>
-      <c r="U64" s="97"/>
-      <c r="V64" s="97"/>
-      <c r="Z64" s="97"/>
-      <c r="AA64" s="97"/>
+      <c r="F64" s="94"/>
+      <c r="G64" s="94"/>
+      <c r="K64" s="94"/>
+      <c r="L64" s="94"/>
+      <c r="P64" s="94"/>
+      <c r="Q64" s="94"/>
+      <c r="U64" s="94"/>
+      <c r="V64" s="94"/>
+      <c r="Z64" s="94"/>
+      <c r="AA64" s="94"/>
     </row>
     <row r="65" spans="6:27" x14ac:dyDescent="0.25">
       <c r="F65" s="97"/>
@@ -7406,8 +7497,43 @@
       <c r="Z65" s="97"/>
       <c r="AA65" s="97"/>
     </row>
+    <row r="66" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="97"/>
+      <c r="P66" s="97"/>
+      <c r="Q66" s="97"/>
+      <c r="U66" s="97"/>
+      <c r="V66" s="97"/>
+      <c r="Z66" s="97"/>
+      <c r="AA66" s="97"/>
+    </row>
+    <row r="67" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F67" s="97"/>
+      <c r="G67" s="97"/>
+      <c r="K67" s="97"/>
+      <c r="L67" s="97"/>
+      <c r="P67" s="97"/>
+      <c r="Q67" s="97"/>
+      <c r="U67" s="97"/>
+      <c r="V67" s="97"/>
+      <c r="Z67" s="97"/>
+      <c r="AA67" s="97"/>
+    </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -7424,17 +7550,6 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
2015-02-12: add to sync
</commit_message>
<xml_diff>
--- a/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
+++ b/Document/Report & Plan/30 BM QTQT CORP_Ke hoach bao cao cong viec_form.DGCV_NguyenTH.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="5"/>
+    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="2014_Thang6" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="2014_Thang9" sheetId="7" r:id="rId4"/>
     <sheet name="2014_Thang10" sheetId="8" r:id="rId5"/>
     <sheet name="2014_Thang11" sheetId="9" r:id="rId6"/>
+    <sheet name="2015_Thang2" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -1362,8 +1363,232 @@
 </comments>
 </file>
 
+<file path=xl/comments7.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>SONY Y2</author>
+    <author>HinhND</author>
+  </authors>
+  <commentList>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Thuybt:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+- Lập đầu tuần (hàng tuần)
+- Các công việc được chia theo nhóm công việc/khách hàng/dự án cụ thể
+- Chi tiết các bước thực hiện cho 1 công việc cụ thể
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thuybt:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Các tuần không thực hiện có thể Hide đi và chỉ đẻ các tuần đang tác nghiệp
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Thuybt:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>- Thực hiện khi lập BC hàng tuần
+- Ghi chú đề xuất (nếu có)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+Kết quả thực tế đạt được có thể là tài liệu, source code, bản thiết kế, cuộc họp, kế hoạch,...</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Kết quả cần đưa vào khi thực hiện lập kế hoạch
+-Các đầu việc cần được chia nhỏ đủ để hoàn thành trong vòng 1 tuần
+-Kết quả cần cụ thể, đo lường được là tài liệu, sourcecode
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Thời gian thực hiện công việc đủ trong 1 tuần</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Đánh giá kết quả thực hiện so với kế hoạch
+-Đạt bao nhiêu % 
+-Kết luận đạt hay không đạt</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G9" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t>HinhND:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="163"/>
+          </rPr>
+          <t xml:space="preserve">
+-Nếu không đạt kế hoạch thì nguyên nhân do đâu?
+-Đề xuất cách thực hiện, giải pháp nâng cao chất lượng</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="873" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="238">
   <si>
     <t>TT</t>
   </si>
@@ -2037,6 +2262,48 @@
   </si>
   <si>
     <t>23/11/12014</t>
+  </si>
+  <si>
+    <t>Tích hợp module Tổng hợp cước vào phân đoạn Move dữ liệu từ HOT_RATED_CDR_1,2 qua HOT_RATED_CDR</t>
+  </si>
+  <si>
+    <t>4/2/2015</t>
+  </si>
+  <si>
+    <t>Thực hiện Retest các Issue của quá trình đối soát, chỉ raise lại các Issue đúng tới Comverse</t>
+  </si>
+  <si>
+    <t>5/5/2015</t>
+  </si>
+  <si>
+    <t>Hiện tại cần VNP trả lời 1 Issue về lệch giá cước, 1 Issue khác đang đợi Comverse tìm hiểu nguyên nhân và fix bug</t>
+  </si>
+  <si>
+    <t>Tuning, cải thiện Performance cho các Oracle Job</t>
+  </si>
+  <si>
+    <t>Hoàn thành, cài thiện đáng kể Performance các chặng chuyển dữ liệu từ TEMP -&gt; HOT_1,2 -&gt; HOT</t>
+  </si>
+  <si>
+    <t>Migrate hệ thống RAC qua SDP mới 3.106</t>
+  </si>
+  <si>
+    <t>6/2/2015</t>
+  </si>
+  <si>
+    <t>Fix Oracle Bug trên SDP mới</t>
+  </si>
+  <si>
+    <t>Đối soát, raise Issue, quản lý Issue</t>
+  </si>
+  <si>
+    <t>Các công việc DBA</t>
+  </si>
+  <si>
+    <t>Fix bug module: HotExport, kill ứng dụng đột ngột</t>
+  </si>
+  <si>
+    <t>13/2/2015</t>
   </si>
 </sst>
 </file>
@@ -2939,7 +3206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="155">
+  <cellXfs count="156">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3281,16 +3548,13 @@
     <xf numFmtId="14" fontId="6" fillId="8" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3300,36 +3564,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3353,17 +3587,53 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="5" fillId="8" borderId="36" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3817,6 +4087,79 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1134927</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>145677</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="ELCOM_LOGO_136x60pcs"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="85724" y="28575"/>
+          <a:ext cx="1382578" cy="412377"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a14:hiddenLine>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4245,10 +4588,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -4314,94 +4657,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -4409,10 +4752,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -4420,10 +4763,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -4431,10 +4774,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -4442,10 +4785,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -4453,17 +4796,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -4529,9 +4872,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -6765,17 +7108,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AC6:AC9"/>
-    <mergeCell ref="AD6:AD9"/>
-    <mergeCell ref="P8:Q8"/>
-    <mergeCell ref="M7:Q7"/>
-    <mergeCell ref="U8:V8"/>
-    <mergeCell ref="R7:V7"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="W7:AA7"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
-    <mergeCell ref="Z8:AA8"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:A9"/>
     <mergeCell ref="B6:B9"/>
@@ -6792,6 +7124,17 @@
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:E9"/>
     <mergeCell ref="H8:I8"/>
+    <mergeCell ref="AC6:AC9"/>
+    <mergeCell ref="AD6:AD9"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
+    <mergeCell ref="Z8:AA8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6943,10 +7286,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -7012,94 +7355,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -7107,10 +7450,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -7118,10 +7461,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -7129,10 +7472,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -7140,10 +7483,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -7151,17 +7494,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -7227,9 +7570,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -8965,6 +9308,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -8981,17 +9335,6 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9143,10 +9486,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -9212,94 +9555,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -9307,10 +9650,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -9318,10 +9661,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -9329,10 +9672,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -9340,10 +9683,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -9351,17 +9694,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -9427,9 +9770,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -11307,6 +11650,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -11323,17 +11677,6 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -11486,10 +11829,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -11555,94 +11898,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -11650,10 +11993,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -11661,10 +12004,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -11672,10 +12015,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -11683,10 +12026,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -11694,17 +12037,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -11770,9 +12113,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -13780,6 +14123,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -13796,17 +14150,6 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -13960,10 +14303,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -14029,94 +14372,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -14124,10 +14467,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -14135,10 +14478,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -14146,10 +14489,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -14157,10 +14500,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -14168,17 +14511,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -14244,9 +14587,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -16556,17 +16899,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A6:A9"/>
-    <mergeCell ref="B6:B9"/>
-    <mergeCell ref="C6:AA6"/>
-    <mergeCell ref="AB6:AB9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="W8:X8"/>
-    <mergeCell ref="Y8:Y9"/>
     <mergeCell ref="AD6:AD9"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="H7:L7"/>
@@ -16583,6 +16915,17 @@
     <mergeCell ref="R8:S8"/>
     <mergeCell ref="T8:T9"/>
     <mergeCell ref="U8:V8"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -16595,8 +16938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD67"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16736,10 +17079,10 @@
       <c r="AD3" s="62"/>
     </row>
     <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="144" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="127"/>
+      <c r="B4" s="144"/>
       <c r="C4" s="61" t="s">
         <v>65</v>
       </c>
@@ -16805,94 +17148,94 @@
       <c r="AC5" s="63"/>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
-      <c r="A6" s="128" t="s">
+      <c r="A6" s="145" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="131" t="s">
+      <c r="B6" s="130" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="134" t="s">
+      <c r="C6" s="148" t="s">
         <v>2</v>
       </c>
-      <c r="D6" s="135"/>
-      <c r="E6" s="135"/>
-      <c r="F6" s="135"/>
-      <c r="G6" s="135"/>
-      <c r="H6" s="135"/>
-      <c r="I6" s="135"/>
-      <c r="J6" s="135"/>
-      <c r="K6" s="135"/>
-      <c r="L6" s="135"/>
-      <c r="M6" s="135"/>
-      <c r="N6" s="135"/>
-      <c r="O6" s="135"/>
-      <c r="P6" s="135"/>
-      <c r="Q6" s="135"/>
-      <c r="R6" s="135"/>
-      <c r="S6" s="135"/>
-      <c r="T6" s="135"/>
-      <c r="U6" s="135"/>
-      <c r="V6" s="135"/>
-      <c r="W6" s="135"/>
-      <c r="X6" s="135"/>
-      <c r="Y6" s="135"/>
-      <c r="Z6" s="135"/>
-      <c r="AA6" s="136"/>
-      <c r="AB6" s="137" t="s">
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" s="152" t="s">
+      <c r="AC6" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="AD6" s="131" t="s">
+      <c r="AD6" s="130" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="129"/>
-      <c r="B7" s="132"/>
-      <c r="C7" s="146" t="s">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
         <v>69</v>
       </c>
-      <c r="D7" s="147"/>
-      <c r="E7" s="147"/>
-      <c r="F7" s="147"/>
-      <c r="G7" s="148"/>
-      <c r="H7" s="149" t="s">
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="150"/>
-      <c r="J7" s="150"/>
-      <c r="K7" s="150"/>
-      <c r="L7" s="151"/>
-      <c r="M7" s="146" t="s">
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
         <v>71</v>
       </c>
-      <c r="N7" s="147"/>
-      <c r="O7" s="147"/>
-      <c r="P7" s="147"/>
-      <c r="Q7" s="148"/>
-      <c r="R7" s="149" t="s">
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
         <v>72</v>
       </c>
-      <c r="S7" s="150"/>
-      <c r="T7" s="150"/>
-      <c r="U7" s="150"/>
-      <c r="V7" s="150"/>
-      <c r="W7" s="146" t="s">
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="147"/>
-      <c r="Y7" s="147"/>
-      <c r="Z7" s="147"/>
-      <c r="AA7" s="148"/>
-      <c r="AB7" s="138"/>
-      <c r="AC7" s="153"/>
-      <c r="AD7" s="132"/>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="129"/>
-      <c r="B8" s="132"/>
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
       <c r="C8" s="142" t="s">
         <v>6</v>
       </c>
@@ -16900,10 +17243,10 @@
       <c r="E8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="144" t="s">
+      <c r="F8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="G8" s="145"/>
+      <c r="G8" s="134"/>
       <c r="H8" s="142" t="s">
         <v>6</v>
       </c>
@@ -16911,10 +17254,10 @@
       <c r="J8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="K8" s="144" t="s">
+      <c r="K8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="L8" s="145"/>
+      <c r="L8" s="134"/>
       <c r="M8" s="142" t="s">
         <v>6</v>
       </c>
@@ -16922,10 +17265,10 @@
       <c r="O8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="P8" s="144" t="s">
+      <c r="P8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="Q8" s="145"/>
+      <c r="Q8" s="134"/>
       <c r="R8" s="142" t="s">
         <v>6</v>
       </c>
@@ -16933,10 +17276,10 @@
       <c r="T8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="U8" s="144" t="s">
+      <c r="U8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="V8" s="145"/>
+      <c r="V8" s="134"/>
       <c r="W8" s="142" t="s">
         <v>6</v>
       </c>
@@ -16944,17 +17287,17 @@
       <c r="Y8" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="Z8" s="144" t="s">
+      <c r="Z8" s="133" t="s">
         <v>23</v>
       </c>
-      <c r="AA8" s="145"/>
-      <c r="AB8" s="138"/>
-      <c r="AC8" s="153"/>
-      <c r="AD8" s="132"/>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
     </row>
     <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="130"/>
-      <c r="B9" s="133"/>
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
       <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
@@ -17020,9 +17363,9 @@
       <c r="AA9" s="100" t="s">
         <v>24</v>
       </c>
-      <c r="AB9" s="139"/>
-      <c r="AC9" s="154"/>
-      <c r="AD9" s="133"/>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
     </row>
     <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -17437,6 +17780,2230 @@
       <c r="AB20" s="44"/>
       <c r="AC20" s="45"/>
       <c r="AD20" s="46"/>
+    </row>
+    <row r="21" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="36"/>
+      <c r="B21" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="C21" s="124"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="101"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="114"/>
+      <c r="L21" s="38"/>
+      <c r="M21" s="43"/>
+      <c r="N21" s="101"/>
+      <c r="O21" s="101"/>
+      <c r="P21" s="114"/>
+      <c r="Q21" s="38"/>
+      <c r="R21" s="43"/>
+      <c r="S21" s="101"/>
+      <c r="T21" s="42"/>
+      <c r="U21" s="42"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="43"/>
+      <c r="X21" s="42"/>
+      <c r="Y21" s="42"/>
+      <c r="Z21" s="42"/>
+      <c r="AA21" s="38"/>
+      <c r="AB21" s="44"/>
+      <c r="AC21" s="45"/>
+      <c r="AD21" s="46"/>
+    </row>
+    <row r="22" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A22" s="36"/>
+      <c r="B22" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="47"/>
+      <c r="D22" s="48"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="48"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="43"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="101"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="38"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="42"/>
+      <c r="T22" s="42"/>
+      <c r="U22" s="42"/>
+      <c r="V22" s="38"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="42"/>
+      <c r="Y22" s="42"/>
+      <c r="Z22" s="42"/>
+      <c r="AA22" s="38"/>
+      <c r="AB22" s="44"/>
+      <c r="AC22" s="45"/>
+      <c r="AD22" s="46"/>
+    </row>
+    <row r="23" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="36"/>
+      <c r="B23" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="47"/>
+      <c r="D23" s="48"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="48"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="L23" s="38"/>
+      <c r="M23" s="43"/>
+      <c r="N23" s="42"/>
+      <c r="O23" s="101"/>
+      <c r="P23" s="42"/>
+      <c r="Q23" s="38"/>
+      <c r="R23" s="41"/>
+      <c r="S23" s="42"/>
+      <c r="T23" s="42"/>
+      <c r="U23" s="42"/>
+      <c r="V23" s="38"/>
+      <c r="W23" s="43"/>
+      <c r="X23" s="42"/>
+      <c r="Y23" s="42"/>
+      <c r="Z23" s="42"/>
+      <c r="AA23" s="38"/>
+      <c r="AB23" s="44"/>
+      <c r="AC23" s="45"/>
+      <c r="AD23" s="46"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A24" s="36"/>
+      <c r="B24" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="47"/>
+      <c r="D24" s="48"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="48"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="L24" s="38"/>
+      <c r="M24" s="43"/>
+      <c r="N24" s="42"/>
+      <c r="O24" s="101"/>
+      <c r="P24" s="42"/>
+      <c r="Q24" s="38"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="42"/>
+      <c r="T24" s="42"/>
+      <c r="U24" s="42"/>
+      <c r="V24" s="38"/>
+      <c r="W24" s="43"/>
+      <c r="X24" s="42"/>
+      <c r="Y24" s="42"/>
+      <c r="Z24" s="42"/>
+      <c r="AA24" s="38"/>
+      <c r="AB24" s="44"/>
+      <c r="AC24" s="45"/>
+      <c r="AD24" s="46"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C25" s="47"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="L25" s="38"/>
+      <c r="M25" s="43"/>
+      <c r="N25" s="42"/>
+      <c r="O25" s="101"/>
+      <c r="P25" s="42"/>
+      <c r="Q25" s="38"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="42"/>
+      <c r="T25" s="42"/>
+      <c r="U25" s="42"/>
+      <c r="V25" s="38"/>
+      <c r="W25" s="43"/>
+      <c r="X25" s="42"/>
+      <c r="Y25" s="42"/>
+      <c r="Z25" s="42"/>
+      <c r="AA25" s="38"/>
+      <c r="AB25" s="44"/>
+      <c r="AC25" s="45"/>
+      <c r="AD25" s="46"/>
+    </row>
+    <row r="26" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="16"/>
+      <c r="D26" s="17"/>
+      <c r="E26" s="106"/>
+      <c r="F26" s="107"/>
+      <c r="G26" s="105"/>
+      <c r="H26" s="16"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="106"/>
+      <c r="L26" s="105"/>
+      <c r="M26" s="20"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="106"/>
+      <c r="Q26" s="105"/>
+      <c r="R26" s="20"/>
+      <c r="S26" s="21"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="106"/>
+      <c r="V26" s="105"/>
+      <c r="W26" s="20"/>
+      <c r="X26" s="21"/>
+      <c r="Y26" s="21"/>
+      <c r="Z26" s="106"/>
+      <c r="AA26" s="105"/>
+      <c r="AB26" s="22"/>
+      <c r="AC26" s="23"/>
+      <c r="AD26" s="24"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A27" s="25">
+        <v>1</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="52"/>
+      <c r="D27" s="53"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="108"/>
+      <c r="H27" s="52"/>
+      <c r="I27" s="53"/>
+      <c r="J27" s="32"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="108"/>
+      <c r="M27" s="30"/>
+      <c r="N27" s="32"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="108"/>
+      <c r="R27" s="30"/>
+      <c r="S27" s="32"/>
+      <c r="T27" s="32"/>
+      <c r="U27" s="51"/>
+      <c r="V27" s="108"/>
+      <c r="W27" s="30"/>
+      <c r="X27" s="32"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="108"/>
+      <c r="AB27" s="33"/>
+      <c r="AC27" s="34"/>
+      <c r="AD27" s="35"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A28" s="25">
+        <v>2</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="50"/>
+      <c r="G28" s="108"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="32"/>
+      <c r="K28" s="51"/>
+      <c r="L28" s="108"/>
+      <c r="M28" s="30"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="108"/>
+      <c r="R28" s="30"/>
+      <c r="S28" s="32"/>
+      <c r="T28" s="32"/>
+      <c r="U28" s="51"/>
+      <c r="V28" s="108"/>
+      <c r="W28" s="30"/>
+      <c r="X28" s="32"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="108"/>
+      <c r="AB28" s="33"/>
+      <c r="AC28" s="34"/>
+      <c r="AD28" s="35"/>
+    </row>
+    <row r="29" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="67"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="38"/>
+      <c r="G29" s="38"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="67"/>
+      <c r="J29" s="42"/>
+      <c r="K29" s="38"/>
+      <c r="L29" s="38"/>
+      <c r="M29" s="43"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42"/>
+      <c r="P29" s="38"/>
+      <c r="Q29" s="38"/>
+      <c r="R29" s="43"/>
+      <c r="S29" s="42"/>
+      <c r="T29" s="42"/>
+      <c r="U29" s="38"/>
+      <c r="V29" s="38"/>
+      <c r="W29" s="43"/>
+      <c r="X29" s="42"/>
+      <c r="Y29" s="42"/>
+      <c r="Z29" s="38"/>
+      <c r="AA29" s="38"/>
+      <c r="AB29" s="44"/>
+      <c r="AC29" s="45"/>
+      <c r="AD29" s="46"/>
+    </row>
+    <row r="30" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="36"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="47"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="42"/>
+      <c r="K30" s="38"/>
+      <c r="L30" s="38"/>
+      <c r="M30" s="43"/>
+      <c r="N30" s="42"/>
+      <c r="O30" s="42"/>
+      <c r="P30" s="38"/>
+      <c r="Q30" s="38"/>
+      <c r="R30" s="43"/>
+      <c r="S30" s="42"/>
+      <c r="T30" s="42"/>
+      <c r="U30" s="38"/>
+      <c r="V30" s="38"/>
+      <c r="W30" s="43"/>
+      <c r="X30" s="42"/>
+      <c r="Y30" s="42"/>
+      <c r="Z30" s="38"/>
+      <c r="AA30" s="38"/>
+      <c r="AB30" s="44"/>
+      <c r="AC30" s="45"/>
+      <c r="AD30" s="46"/>
+    </row>
+    <row r="31" spans="1:30" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="36"/>
+      <c r="B31" s="37"/>
+      <c r="C31" s="47"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="18"/>
+      <c r="H31" s="47"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="42"/>
+      <c r="K31" s="18"/>
+      <c r="L31" s="18"/>
+      <c r="M31" s="43"/>
+      <c r="N31" s="42"/>
+      <c r="O31" s="42"/>
+      <c r="P31" s="18"/>
+      <c r="Q31" s="18"/>
+      <c r="R31" s="43"/>
+      <c r="S31" s="42"/>
+      <c r="T31" s="42"/>
+      <c r="U31" s="18"/>
+      <c r="V31" s="18"/>
+      <c r="W31" s="43"/>
+      <c r="X31" s="42"/>
+      <c r="Y31" s="42"/>
+      <c r="Z31" s="18"/>
+      <c r="AA31" s="18"/>
+      <c r="AB31" s="44"/>
+      <c r="AC31" s="45"/>
+      <c r="AD31" s="46"/>
+    </row>
+    <row r="32" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="71"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="28"/>
+      <c r="G32" s="28"/>
+      <c r="H32" s="70"/>
+      <c r="I32" s="71"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="28"/>
+      <c r="L32" s="28"/>
+      <c r="M32" s="30"/>
+      <c r="N32" s="32"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="28"/>
+      <c r="Q32" s="28"/>
+      <c r="R32" s="30"/>
+      <c r="S32" s="32"/>
+      <c r="T32" s="32"/>
+      <c r="U32" s="28"/>
+      <c r="V32" s="28"/>
+      <c r="W32" s="30"/>
+      <c r="X32" s="32"/>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="28"/>
+      <c r="AA32" s="28"/>
+      <c r="AB32" s="33"/>
+      <c r="AC32" s="34"/>
+      <c r="AD32" s="35"/>
+    </row>
+    <row r="33" spans="1:30" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="36"/>
+      <c r="B33" s="37"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="51"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="51"/>
+      <c r="J33" s="42"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="43"/>
+      <c r="N33" s="42"/>
+      <c r="O33" s="42"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="43"/>
+      <c r="S33" s="42"/>
+      <c r="T33" s="42"/>
+      <c r="U33" s="38"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="43"/>
+      <c r="X33" s="42"/>
+      <c r="Y33" s="42"/>
+      <c r="Z33" s="38"/>
+      <c r="AA33" s="38"/>
+      <c r="AB33" s="44"/>
+      <c r="AC33" s="45"/>
+      <c r="AD33" s="46"/>
+    </row>
+    <row r="34" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="105"/>
+      <c r="H34" s="16"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="105"/>
+      <c r="M34" s="20"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="17"/>
+      <c r="Q34" s="105"/>
+      <c r="R34" s="20"/>
+      <c r="S34" s="21"/>
+      <c r="T34" s="21"/>
+      <c r="U34" s="17"/>
+      <c r="V34" s="105"/>
+      <c r="W34" s="20"/>
+      <c r="X34" s="21"/>
+      <c r="Y34" s="21"/>
+      <c r="Z34" s="17"/>
+      <c r="AA34" s="105"/>
+      <c r="AB34" s="22"/>
+      <c r="AC34" s="23"/>
+      <c r="AD34" s="24"/>
+    </row>
+    <row r="35" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A35" s="25"/>
+      <c r="B35" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="47"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="67"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="47"/>
+      <c r="I35" s="51"/>
+      <c r="J35" s="32"/>
+      <c r="K35" s="51"/>
+      <c r="L35" s="108"/>
+      <c r="M35" s="30"/>
+      <c r="N35" s="32"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="108"/>
+      <c r="R35" s="30"/>
+      <c r="S35" s="32"/>
+      <c r="T35" s="32"/>
+      <c r="U35" s="51"/>
+      <c r="V35" s="108"/>
+      <c r="W35" s="30"/>
+      <c r="X35" s="32"/>
+      <c r="Y35" s="32"/>
+      <c r="Z35" s="51"/>
+      <c r="AA35" s="108"/>
+      <c r="AB35" s="33"/>
+      <c r="AC35" s="34"/>
+      <c r="AD35" s="35"/>
+    </row>
+    <row r="36" spans="1:30" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="36"/>
+      <c r="B36" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="47"/>
+      <c r="D36" s="51"/>
+      <c r="E36" s="67"/>
+      <c r="F36" s="51"/>
+      <c r="G36" s="108"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="51"/>
+      <c r="L36" s="108"/>
+      <c r="M36" s="43"/>
+      <c r="N36" s="42"/>
+      <c r="O36" s="42"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="108"/>
+      <c r="R36" s="43"/>
+      <c r="S36" s="42"/>
+      <c r="T36" s="42"/>
+      <c r="U36" s="51"/>
+      <c r="V36" s="108"/>
+      <c r="W36" s="43"/>
+      <c r="X36" s="42"/>
+      <c r="Y36" s="42"/>
+      <c r="Z36" s="51"/>
+      <c r="AA36" s="108"/>
+      <c r="AB36" s="44"/>
+      <c r="AC36" s="45"/>
+      <c r="AD36" s="46"/>
+    </row>
+    <row r="37" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C37" s="47"/>
+      <c r="D37" s="51"/>
+      <c r="E37" s="67"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="111"/>
+      <c r="H37" s="47"/>
+      <c r="I37" s="51"/>
+      <c r="J37" s="42"/>
+      <c r="K37" s="72"/>
+      <c r="L37" s="111"/>
+      <c r="M37" s="47"/>
+      <c r="N37" s="51"/>
+      <c r="O37" s="42"/>
+      <c r="P37" s="72"/>
+      <c r="Q37" s="111"/>
+      <c r="R37" s="47"/>
+      <c r="S37" s="51"/>
+      <c r="T37" s="42"/>
+      <c r="U37" s="72"/>
+      <c r="V37" s="111"/>
+      <c r="W37" s="43"/>
+      <c r="X37" s="42"/>
+      <c r="Y37" s="42"/>
+      <c r="Z37" s="72"/>
+      <c r="AA37" s="111"/>
+      <c r="AB37" s="44"/>
+      <c r="AC37" s="45"/>
+      <c r="AD37" s="46"/>
+    </row>
+    <row r="38" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="36"/>
+      <c r="B38" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" s="47"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="67"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="111"/>
+      <c r="H38" s="47"/>
+      <c r="I38" s="122"/>
+      <c r="J38" s="42"/>
+      <c r="K38" s="72"/>
+      <c r="L38" s="111"/>
+      <c r="M38" s="43"/>
+      <c r="N38" s="101"/>
+      <c r="O38" s="42"/>
+      <c r="P38" s="72"/>
+      <c r="Q38" s="111"/>
+      <c r="R38" s="43"/>
+      <c r="S38" s="101"/>
+      <c r="T38" s="42"/>
+      <c r="U38" s="72"/>
+      <c r="V38" s="111"/>
+      <c r="W38" s="43"/>
+      <c r="X38" s="42"/>
+      <c r="Y38" s="42"/>
+      <c r="Z38" s="72"/>
+      <c r="AA38" s="111"/>
+      <c r="AB38" s="44"/>
+      <c r="AC38" s="45"/>
+      <c r="AD38" s="46"/>
+    </row>
+    <row r="39" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="36"/>
+      <c r="B39" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39" s="47"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="108"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="51"/>
+      <c r="J39" s="42"/>
+      <c r="K39" s="51"/>
+      <c r="L39" s="108"/>
+      <c r="M39" s="43"/>
+      <c r="N39" s="42"/>
+      <c r="O39" s="42"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="108"/>
+      <c r="R39" s="43"/>
+      <c r="S39" s="42"/>
+      <c r="T39" s="42"/>
+      <c r="U39" s="51"/>
+      <c r="V39" s="108"/>
+      <c r="W39" s="43"/>
+      <c r="X39" s="42"/>
+      <c r="Y39" s="42"/>
+      <c r="Z39" s="51"/>
+      <c r="AA39" s="108"/>
+      <c r="AB39" s="44"/>
+      <c r="AC39" s="45"/>
+      <c r="AD39" s="46"/>
+    </row>
+    <row r="40" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="36"/>
+      <c r="B40" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C40" s="47"/>
+      <c r="D40" s="51"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="108"/>
+      <c r="H40" s="47"/>
+      <c r="I40" s="51"/>
+      <c r="J40" s="42"/>
+      <c r="K40" s="51"/>
+      <c r="L40" s="108"/>
+      <c r="M40" s="43"/>
+      <c r="N40" s="42"/>
+      <c r="O40" s="42"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="108"/>
+      <c r="R40" s="43"/>
+      <c r="S40" s="42"/>
+      <c r="T40" s="42"/>
+      <c r="U40" s="51"/>
+      <c r="V40" s="108"/>
+      <c r="W40" s="43"/>
+      <c r="X40" s="42"/>
+      <c r="Y40" s="42"/>
+      <c r="Z40" s="51"/>
+      <c r="AA40" s="108"/>
+      <c r="AB40" s="44"/>
+      <c r="AC40" s="45"/>
+      <c r="AD40" s="46"/>
+    </row>
+    <row r="41" spans="1:30" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="36"/>
+      <c r="B41" s="26" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="47"/>
+      <c r="D41" s="51"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="108"/>
+      <c r="H41" s="47"/>
+      <c r="I41" s="122"/>
+      <c r="J41" s="42"/>
+      <c r="K41" s="51"/>
+      <c r="L41" s="108"/>
+      <c r="M41" s="43"/>
+      <c r="N41" s="42"/>
+      <c r="O41" s="42"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="108"/>
+      <c r="R41" s="43"/>
+      <c r="S41" s="42"/>
+      <c r="T41" s="42"/>
+      <c r="U41" s="51"/>
+      <c r="V41" s="108"/>
+      <c r="W41" s="43"/>
+      <c r="X41" s="42"/>
+      <c r="Y41" s="42"/>
+      <c r="Z41" s="51"/>
+      <c r="AA41" s="108"/>
+      <c r="AB41" s="44"/>
+      <c r="AC41" s="45"/>
+      <c r="AD41" s="46"/>
+    </row>
+    <row r="42" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A42" s="75"/>
+      <c r="B42" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="77"/>
+      <c r="D42" s="76"/>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="76"/>
+      <c r="H42" s="76"/>
+      <c r="I42" s="76"/>
+      <c r="J42" s="76"/>
+      <c r="K42" s="76"/>
+      <c r="L42" s="76"/>
+      <c r="M42" s="76"/>
+      <c r="N42" s="76"/>
+      <c r="O42" s="76"/>
+      <c r="P42" s="76"/>
+      <c r="Q42" s="76"/>
+      <c r="R42" s="76"/>
+      <c r="S42" s="76"/>
+      <c r="T42" s="76"/>
+      <c r="U42" s="76"/>
+      <c r="V42" s="76"/>
+      <c r="W42" s="76"/>
+      <c r="X42" s="76"/>
+      <c r="Y42" s="76"/>
+      <c r="Z42" s="76"/>
+      <c r="AA42" s="76"/>
+      <c r="AB42" s="76"/>
+      <c r="AC42" s="76"/>
+      <c r="AD42" s="78"/>
+    </row>
+    <row r="43" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A43" s="36"/>
+      <c r="B43" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C43" s="47"/>
+      <c r="D43" s="51"/>
+      <c r="E43" s="112"/>
+      <c r="F43" s="113"/>
+      <c r="G43" s="108"/>
+      <c r="H43" s="74"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="42"/>
+      <c r="K43" s="113"/>
+      <c r="L43" s="108"/>
+      <c r="M43" s="43"/>
+      <c r="N43" s="101"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="113"/>
+      <c r="Q43" s="108"/>
+      <c r="R43" s="43"/>
+      <c r="S43" s="42"/>
+      <c r="T43" s="42"/>
+      <c r="U43" s="113"/>
+      <c r="V43" s="108"/>
+      <c r="W43" s="43"/>
+      <c r="X43" s="42"/>
+      <c r="Y43" s="42"/>
+      <c r="Z43" s="113"/>
+      <c r="AA43" s="108"/>
+      <c r="AB43" s="44"/>
+      <c r="AC43" s="45"/>
+      <c r="AD43" s="46"/>
+    </row>
+    <row r="44" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A44" s="36"/>
+      <c r="B44" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C44" s="47"/>
+      <c r="D44" s="51"/>
+      <c r="E44" s="51"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="108"/>
+      <c r="H44" s="74"/>
+      <c r="I44" s="51"/>
+      <c r="J44" s="42"/>
+      <c r="K44" s="51"/>
+      <c r="L44" s="108"/>
+      <c r="M44" s="43"/>
+      <c r="N44" s="101"/>
+      <c r="O44" s="101"/>
+      <c r="P44" s="42"/>
+      <c r="Q44" s="108"/>
+      <c r="R44" s="43"/>
+      <c r="S44" s="42"/>
+      <c r="T44" s="42"/>
+      <c r="U44" s="42"/>
+      <c r="V44" s="108"/>
+      <c r="W44" s="43"/>
+      <c r="X44" s="42"/>
+      <c r="Y44" s="42"/>
+      <c r="Z44" s="125"/>
+      <c r="AA44" s="108"/>
+      <c r="AB44" s="44"/>
+      <c r="AC44" s="45"/>
+      <c r="AD44" s="46"/>
+    </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A45" s="36"/>
+      <c r="B45" s="26"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="51"/>
+      <c r="E45" s="67"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="108"/>
+      <c r="H45" s="74"/>
+      <c r="I45" s="51"/>
+      <c r="J45" s="42"/>
+      <c r="K45" s="51"/>
+      <c r="L45" s="108"/>
+      <c r="M45" s="43"/>
+      <c r="N45" s="42"/>
+      <c r="O45" s="42"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="108"/>
+      <c r="R45" s="43"/>
+      <c r="S45" s="116"/>
+      <c r="T45" s="42"/>
+      <c r="U45" s="51"/>
+      <c r="V45" s="108"/>
+      <c r="W45" s="43"/>
+      <c r="X45" s="42"/>
+      <c r="Y45" s="42"/>
+      <c r="Z45" s="51"/>
+      <c r="AA45" s="108"/>
+      <c r="AB45" s="44"/>
+      <c r="AC45" s="45"/>
+      <c r="AD45" s="46"/>
+    </row>
+    <row r="46" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="79"/>
+      <c r="B46" s="80"/>
+      <c r="C46" s="81"/>
+      <c r="D46" s="82"/>
+      <c r="E46" s="82"/>
+      <c r="F46" s="82"/>
+      <c r="G46" s="88"/>
+      <c r="H46" s="83"/>
+      <c r="I46" s="82"/>
+      <c r="J46" s="85"/>
+      <c r="K46" s="82"/>
+      <c r="L46" s="88"/>
+      <c r="M46" s="84"/>
+      <c r="N46" s="85"/>
+      <c r="O46" s="85"/>
+      <c r="P46" s="82"/>
+      <c r="Q46" s="88"/>
+      <c r="R46" s="84"/>
+      <c r="S46" s="85"/>
+      <c r="T46" s="85"/>
+      <c r="U46" s="82"/>
+      <c r="V46" s="88"/>
+      <c r="W46" s="84"/>
+      <c r="X46" s="85"/>
+      <c r="Y46" s="85"/>
+      <c r="Z46" s="82"/>
+      <c r="AA46" s="88"/>
+      <c r="AB46" s="86"/>
+      <c r="AC46" s="87"/>
+      <c r="AD46" s="88"/>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A47" s="63"/>
+      <c r="B47" s="64"/>
+      <c r="AB47" s="63"/>
+      <c r="AC47" s="63"/>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A48" s="63"/>
+      <c r="B48" s="64"/>
+      <c r="AB48" s="63"/>
+      <c r="AC48" s="63"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A49" s="89"/>
+      <c r="B49" s="90" t="s">
+        <v>20</v>
+      </c>
+      <c r="C49" s="91"/>
+      <c r="D49" s="91"/>
+      <c r="E49" s="91"/>
+      <c r="H49" s="91"/>
+      <c r="I49" s="91"/>
+      <c r="J49" s="91"/>
+      <c r="M49" s="91"/>
+      <c r="N49" s="91"/>
+      <c r="O49" s="89"/>
+      <c r="R49" s="89"/>
+      <c r="S49" s="91"/>
+      <c r="T49" s="91"/>
+      <c r="W49" s="89"/>
+      <c r="X49" s="91"/>
+      <c r="Y49" s="91"/>
+      <c r="AB49" s="91"/>
+      <c r="AC49" s="91"/>
+      <c r="AD49" s="91"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A50" s="89"/>
+      <c r="B50" s="90"/>
+      <c r="C50" s="91"/>
+      <c r="D50" s="91"/>
+      <c r="E50" s="91"/>
+      <c r="H50" s="91"/>
+      <c r="I50" s="91"/>
+      <c r="J50" s="91"/>
+      <c r="M50" s="91"/>
+      <c r="N50" s="91"/>
+      <c r="O50" s="89"/>
+      <c r="R50" s="89"/>
+      <c r="S50" s="91"/>
+      <c r="T50" s="91"/>
+      <c r="W50" s="89"/>
+      <c r="X50" s="91"/>
+      <c r="Y50" s="91"/>
+      <c r="AB50" s="91"/>
+      <c r="AC50" s="91"/>
+      <c r="AD50" s="91"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A51" s="89"/>
+      <c r="B51" s="92" t="s">
+        <v>21</v>
+      </c>
+      <c r="C51" s="91"/>
+      <c r="D51" s="91"/>
+      <c r="E51" s="91"/>
+      <c r="H51" s="91"/>
+      <c r="I51" s="91"/>
+      <c r="J51" s="91"/>
+      <c r="M51" s="91"/>
+      <c r="N51" s="91"/>
+      <c r="O51" s="89"/>
+      <c r="R51" s="89"/>
+      <c r="S51" s="91"/>
+      <c r="T51" s="91"/>
+      <c r="W51" s="89"/>
+      <c r="X51" s="91"/>
+      <c r="Y51" s="91"/>
+      <c r="AB51" s="91"/>
+      <c r="AC51" s="91"/>
+      <c r="AD51" s="91"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A52" s="89"/>
+      <c r="B52" s="92" t="s">
+        <v>22</v>
+      </c>
+      <c r="C52" s="92"/>
+      <c r="D52" s="91"/>
+      <c r="E52" s="91"/>
+      <c r="H52" s="91"/>
+      <c r="I52" s="91"/>
+      <c r="J52" s="91"/>
+      <c r="M52" s="91"/>
+      <c r="N52" s="91"/>
+      <c r="O52" s="89"/>
+      <c r="R52" s="89"/>
+      <c r="S52" s="91"/>
+      <c r="T52" s="91"/>
+      <c r="W52" s="89"/>
+      <c r="X52" s="91"/>
+      <c r="Y52" s="91"/>
+      <c r="AB52" s="91"/>
+      <c r="AC52" s="91"/>
+      <c r="AD52" s="91"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A53" s="63"/>
+      <c r="B53" s="93"/>
+      <c r="C53" s="94"/>
+      <c r="D53" s="94"/>
+      <c r="E53" s="94"/>
+      <c r="H53" s="94"/>
+      <c r="I53" s="94"/>
+      <c r="J53" s="94"/>
+      <c r="M53" s="94"/>
+      <c r="N53" s="94"/>
+      <c r="O53" s="94"/>
+      <c r="R53" s="94"/>
+      <c r="S53" s="94"/>
+      <c r="T53" s="94"/>
+      <c r="W53" s="94"/>
+      <c r="X53" s="94"/>
+      <c r="Y53" s="94"/>
+      <c r="AB53" s="63"/>
+      <c r="AC53" s="63"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A54" s="63"/>
+      <c r="B54" s="93"/>
+      <c r="C54" s="94"/>
+      <c r="D54" s="94"/>
+      <c r="E54" s="94"/>
+      <c r="F54" s="91"/>
+      <c r="G54" s="91"/>
+      <c r="H54" s="94"/>
+      <c r="I54" s="94"/>
+      <c r="J54" s="94"/>
+      <c r="K54" s="91"/>
+      <c r="L54" s="91"/>
+      <c r="M54" s="94"/>
+      <c r="N54" s="94"/>
+      <c r="O54" s="94"/>
+      <c r="P54" s="91"/>
+      <c r="Q54" s="91"/>
+      <c r="R54" s="94"/>
+      <c r="S54" s="94"/>
+      <c r="T54" s="94"/>
+      <c r="U54" s="91"/>
+      <c r="V54" s="91"/>
+      <c r="W54" s="94"/>
+      <c r="X54" s="94"/>
+      <c r="Y54" s="94"/>
+      <c r="Z54" s="91"/>
+      <c r="AA54" s="91"/>
+      <c r="AB54" s="63"/>
+      <c r="AC54" s="63"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A55" s="63"/>
+      <c r="B55" s="95"/>
+      <c r="C55" s="94"/>
+      <c r="D55" s="94"/>
+      <c r="E55" s="94"/>
+      <c r="F55" s="91"/>
+      <c r="G55" s="91"/>
+      <c r="H55" s="94"/>
+      <c r="I55" s="94"/>
+      <c r="J55" s="94"/>
+      <c r="K55" s="91"/>
+      <c r="L55" s="91"/>
+      <c r="M55" s="94"/>
+      <c r="N55" s="94"/>
+      <c r="O55" s="94"/>
+      <c r="P55" s="91"/>
+      <c r="Q55" s="91"/>
+      <c r="R55" s="94"/>
+      <c r="S55" s="94"/>
+      <c r="T55" s="94"/>
+      <c r="U55" s="91"/>
+      <c r="V55" s="91"/>
+      <c r="W55" s="94"/>
+      <c r="X55" s="94"/>
+      <c r="Y55" s="94"/>
+      <c r="Z55" s="91"/>
+      <c r="AA55" s="91"/>
+      <c r="AB55" s="63"/>
+      <c r="AC55" s="63"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A56" s="63"/>
+      <c r="B56" s="95"/>
+      <c r="C56" s="94"/>
+      <c r="D56" s="94"/>
+      <c r="E56" s="94"/>
+      <c r="F56" s="91"/>
+      <c r="G56" s="91"/>
+      <c r="H56" s="94"/>
+      <c r="I56" s="94"/>
+      <c r="J56" s="94"/>
+      <c r="K56" s="91"/>
+      <c r="L56" s="91"/>
+      <c r="M56" s="94"/>
+      <c r="N56" s="94"/>
+      <c r="O56" s="94"/>
+      <c r="P56" s="91"/>
+      <c r="Q56" s="91"/>
+      <c r="R56" s="94"/>
+      <c r="S56" s="94"/>
+      <c r="T56" s="94"/>
+      <c r="U56" s="91"/>
+      <c r="V56" s="91"/>
+      <c r="W56" s="94"/>
+      <c r="X56" s="94"/>
+      <c r="Y56" s="94"/>
+      <c r="Z56" s="91"/>
+      <c r="AA56" s="91"/>
+      <c r="AB56" s="63"/>
+      <c r="AC56" s="63"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A57" s="63"/>
+      <c r="B57" s="95"/>
+      <c r="C57" s="94"/>
+      <c r="D57" s="94"/>
+      <c r="E57" s="94"/>
+      <c r="F57" s="91"/>
+      <c r="G57" s="91"/>
+      <c r="H57" s="94"/>
+      <c r="I57" s="94"/>
+      <c r="J57" s="94"/>
+      <c r="K57" s="91"/>
+      <c r="L57" s="91"/>
+      <c r="M57" s="94"/>
+      <c r="N57" s="94"/>
+      <c r="O57" s="94"/>
+      <c r="P57" s="91"/>
+      <c r="Q57" s="91"/>
+      <c r="R57" s="94"/>
+      <c r="S57" s="94"/>
+      <c r="T57" s="94"/>
+      <c r="U57" s="91"/>
+      <c r="V57" s="91"/>
+      <c r="W57" s="94"/>
+      <c r="X57" s="94"/>
+      <c r="Y57" s="94"/>
+      <c r="Z57" s="91"/>
+      <c r="AA57" s="91"/>
+      <c r="AB57" s="63"/>
+      <c r="AC57" s="63"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A58" s="63"/>
+      <c r="B58" s="93"/>
+      <c r="C58" s="94"/>
+      <c r="D58" s="94"/>
+      <c r="E58" s="94"/>
+      <c r="F58" s="94"/>
+      <c r="G58" s="94"/>
+      <c r="H58" s="94"/>
+      <c r="I58" s="94"/>
+      <c r="J58" s="94"/>
+      <c r="K58" s="94"/>
+      <c r="L58" s="94"/>
+      <c r="M58" s="94"/>
+      <c r="N58" s="94"/>
+      <c r="O58" s="94"/>
+      <c r="P58" s="94"/>
+      <c r="Q58" s="94"/>
+      <c r="R58" s="94"/>
+      <c r="S58" s="94"/>
+      <c r="T58" s="94"/>
+      <c r="U58" s="94"/>
+      <c r="V58" s="94"/>
+      <c r="W58" s="94"/>
+      <c r="X58" s="94"/>
+      <c r="Y58" s="94"/>
+      <c r="Z58" s="94"/>
+      <c r="AA58" s="94"/>
+      <c r="AB58" s="63"/>
+      <c r="AC58" s="63"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A59" s="63"/>
+      <c r="B59" s="93"/>
+      <c r="C59" s="94"/>
+      <c r="D59" s="94"/>
+      <c r="E59" s="94"/>
+      <c r="F59" s="94"/>
+      <c r="G59" s="94"/>
+      <c r="H59" s="94"/>
+      <c r="I59" s="94"/>
+      <c r="J59" s="94"/>
+      <c r="K59" s="94"/>
+      <c r="L59" s="94"/>
+      <c r="M59" s="94"/>
+      <c r="N59" s="94"/>
+      <c r="O59" s="94"/>
+      <c r="P59" s="94"/>
+      <c r="Q59" s="94"/>
+      <c r="R59" s="94"/>
+      <c r="S59" s="94"/>
+      <c r="T59" s="94"/>
+      <c r="U59" s="94"/>
+      <c r="V59" s="94"/>
+      <c r="W59" s="94"/>
+      <c r="X59" s="94"/>
+      <c r="Y59" s="94"/>
+      <c r="Z59" s="94"/>
+      <c r="AA59" s="94"/>
+      <c r="AB59" s="96"/>
+      <c r="AC59" s="96"/>
+      <c r="AD59" s="97"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A60" s="63"/>
+      <c r="B60" s="97"/>
+      <c r="C60" s="97"/>
+      <c r="D60" s="97"/>
+      <c r="E60" s="97"/>
+      <c r="F60" s="94"/>
+      <c r="G60" s="94"/>
+      <c r="H60" s="97"/>
+      <c r="I60" s="97"/>
+      <c r="J60" s="97"/>
+      <c r="K60" s="94"/>
+      <c r="L60" s="94"/>
+      <c r="M60" s="97"/>
+      <c r="N60" s="97"/>
+      <c r="O60" s="97"/>
+      <c r="P60" s="94"/>
+      <c r="Q60" s="94"/>
+      <c r="R60" s="97"/>
+      <c r="S60" s="97"/>
+      <c r="T60" s="97"/>
+      <c r="U60" s="94"/>
+      <c r="V60" s="94"/>
+      <c r="W60" s="97"/>
+      <c r="X60" s="97"/>
+      <c r="Y60" s="97"/>
+      <c r="Z60" s="94"/>
+      <c r="AA60" s="94"/>
+      <c r="AB60" s="96"/>
+      <c r="AC60" s="96"/>
+      <c r="AD60" s="97"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A61" s="63"/>
+      <c r="B61" s="98"/>
+      <c r="C61" s="97"/>
+      <c r="D61" s="97"/>
+      <c r="E61" s="97"/>
+      <c r="F61" s="94"/>
+      <c r="G61" s="94"/>
+      <c r="H61" s="97"/>
+      <c r="I61" s="97"/>
+      <c r="J61" s="97"/>
+      <c r="K61" s="94"/>
+      <c r="L61" s="94"/>
+      <c r="M61" s="97"/>
+      <c r="N61" s="97"/>
+      <c r="O61" s="97"/>
+      <c r="P61" s="94"/>
+      <c r="Q61" s="94"/>
+      <c r="R61" s="97"/>
+      <c r="S61" s="97"/>
+      <c r="T61" s="97"/>
+      <c r="U61" s="94"/>
+      <c r="V61" s="94"/>
+      <c r="W61" s="97"/>
+      <c r="X61" s="97"/>
+      <c r="Y61" s="97"/>
+      <c r="Z61" s="94"/>
+      <c r="AA61" s="94"/>
+      <c r="AB61" s="96"/>
+      <c r="AC61" s="96"/>
+      <c r="AD61" s="97"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A62" s="63"/>
+      <c r="B62" s="98"/>
+      <c r="C62" s="97"/>
+      <c r="D62" s="97"/>
+      <c r="E62" s="97"/>
+      <c r="F62" s="94"/>
+      <c r="G62" s="94"/>
+      <c r="H62" s="97"/>
+      <c r="I62" s="97"/>
+      <c r="J62" s="97"/>
+      <c r="K62" s="94"/>
+      <c r="L62" s="94"/>
+      <c r="M62" s="97"/>
+      <c r="N62" s="97"/>
+      <c r="O62" s="97"/>
+      <c r="P62" s="94"/>
+      <c r="Q62" s="94"/>
+      <c r="R62" s="97"/>
+      <c r="S62" s="97"/>
+      <c r="T62" s="97"/>
+      <c r="U62" s="94"/>
+      <c r="V62" s="94"/>
+      <c r="W62" s="97"/>
+      <c r="X62" s="97"/>
+      <c r="Y62" s="97"/>
+      <c r="Z62" s="94"/>
+      <c r="AA62" s="94"/>
+      <c r="AB62" s="96"/>
+      <c r="AC62" s="96"/>
+      <c r="AD62" s="97"/>
+    </row>
+    <row r="63" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A63" s="63"/>
+      <c r="B63" s="64"/>
+      <c r="F63" s="94"/>
+      <c r="G63" s="94"/>
+      <c r="K63" s="94"/>
+      <c r="L63" s="94"/>
+      <c r="P63" s="94"/>
+      <c r="Q63" s="94"/>
+      <c r="U63" s="94"/>
+      <c r="V63" s="94"/>
+      <c r="Z63" s="94"/>
+      <c r="AA63" s="94"/>
+      <c r="AB63" s="63"/>
+      <c r="AC63" s="63"/>
+    </row>
+    <row r="64" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="F64" s="94"/>
+      <c r="G64" s="94"/>
+      <c r="K64" s="94"/>
+      <c r="L64" s="94"/>
+      <c r="P64" s="94"/>
+      <c r="Q64" s="94"/>
+      <c r="U64" s="94"/>
+      <c r="V64" s="94"/>
+      <c r="Z64" s="94"/>
+      <c r="AA64" s="94"/>
+    </row>
+    <row r="65" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F65" s="97"/>
+      <c r="G65" s="97"/>
+      <c r="K65" s="97"/>
+      <c r="L65" s="97"/>
+      <c r="P65" s="97"/>
+      <c r="Q65" s="97"/>
+      <c r="U65" s="97"/>
+      <c r="V65" s="97"/>
+      <c r="Z65" s="97"/>
+      <c r="AA65" s="97"/>
+    </row>
+    <row r="66" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F66" s="97"/>
+      <c r="G66" s="97"/>
+      <c r="K66" s="97"/>
+      <c r="L66" s="97"/>
+      <c r="P66" s="97"/>
+      <c r="Q66" s="97"/>
+      <c r="U66" s="97"/>
+      <c r="V66" s="97"/>
+      <c r="Z66" s="97"/>
+      <c r="AA66" s="97"/>
+    </row>
+    <row r="67" spans="6:27" x14ac:dyDescent="0.25">
+      <c r="F67" s="97"/>
+      <c r="G67" s="97"/>
+      <c r="K67" s="97"/>
+      <c r="L67" s="97"/>
+      <c r="P67" s="97"/>
+      <c r="Q67" s="97"/>
+      <c r="U67" s="97"/>
+      <c r="V67" s="97"/>
+      <c r="Z67" s="97"/>
+      <c r="AA67" s="97"/>
+    </row>
+  </sheetData>
+  <mergeCells count="27">
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A6:A9"/>
+    <mergeCell ref="B6:B9"/>
+    <mergeCell ref="C6:AA6"/>
+    <mergeCell ref="AB6:AB9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="AD6:AD9"/>
+    <mergeCell ref="C7:G7"/>
+    <mergeCell ref="H7:L7"/>
+    <mergeCell ref="M7:Q7"/>
+    <mergeCell ref="R7:V7"/>
+    <mergeCell ref="W7:AA7"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="AC6:AC9"/>
+    <mergeCell ref="Z8:AA8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Y8:Y9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AD67"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B21" sqref="A21:XFD21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="2" max="2" width="33.85546875" customWidth="1"/>
+    <col min="3" max="3" width="31.140625" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
+    <col min="5" max="5" width="35" customWidth="1"/>
+    <col min="6" max="6" width="26.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="30.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.140625" customWidth="1"/>
+    <col min="13" max="13" width="36" customWidth="1"/>
+    <col min="14" max="14" width="11.5703125" customWidth="1"/>
+    <col min="15" max="15" width="31.140625" customWidth="1"/>
+    <col min="16" max="17" width="17.140625" customWidth="1"/>
+    <col min="18" max="18" width="32" customWidth="1"/>
+    <col min="19" max="19" width="16.5703125" customWidth="1"/>
+    <col min="20" max="20" width="21.140625" customWidth="1"/>
+    <col min="21" max="22" width="17.140625" customWidth="1"/>
+    <col min="23" max="23" width="31.42578125" customWidth="1"/>
+    <col min="24" max="24" width="12.5703125" customWidth="1"/>
+    <col min="25" max="25" width="17.140625" customWidth="1"/>
+    <col min="26" max="26" width="29.7109375" customWidth="1"/>
+    <col min="27" max="27" width="17.140625" customWidth="1"/>
+    <col min="28" max="29" width="10.140625" customWidth="1"/>
+    <col min="30" max="30" width="25.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
+      <c r="O1" s="55"/>
+      <c r="P1" s="55"/>
+      <c r="Q1" s="55"/>
+      <c r="R1" s="55"/>
+      <c r="S1" s="55"/>
+      <c r="T1" s="55"/>
+      <c r="U1" s="55"/>
+      <c r="V1" s="55"/>
+      <c r="W1" s="55"/>
+      <c r="X1" s="55"/>
+      <c r="Y1" s="55"/>
+      <c r="Z1" s="55"/>
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="55"/>
+    </row>
+    <row r="2" spans="1:30" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" s="58"/>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="58"/>
+      <c r="O2" s="58"/>
+      <c r="P2" s="58"/>
+      <c r="Q2" s="58"/>
+      <c r="R2" s="58"/>
+      <c r="S2" s="58"/>
+      <c r="T2" s="58"/>
+      <c r="U2" s="58"/>
+      <c r="V2" s="58"/>
+      <c r="W2" s="58"/>
+      <c r="X2" s="58"/>
+      <c r="Y2" s="58"/>
+      <c r="Z2" s="58"/>
+      <c r="AA2" s="58"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+    </row>
+    <row r="3" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="59"/>
+      <c r="B3" s="60"/>
+      <c r="C3" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="61"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="61"/>
+      <c r="H3" s="61"/>
+      <c r="I3" s="61"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="61"/>
+      <c r="L3" s="61"/>
+      <c r="M3" s="61"/>
+      <c r="N3" s="61"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="61"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="61"/>
+      <c r="U3" s="61"/>
+      <c r="V3" s="61"/>
+      <c r="W3" s="61"/>
+      <c r="X3" s="61"/>
+      <c r="Y3" s="61"/>
+      <c r="Z3" s="61"/>
+      <c r="AA3" s="61"/>
+      <c r="AB3" s="62"/>
+      <c r="AC3" s="62"/>
+      <c r="AD3" s="62"/>
+    </row>
+    <row r="4" spans="1:30" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="144" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="144"/>
+      <c r="C4" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="61"/>
+      <c r="N4" s="61"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="61"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="61"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="61"/>
+      <c r="U4" s="61"/>
+      <c r="V4" s="61"/>
+      <c r="W4" s="61"/>
+      <c r="X4" s="61"/>
+      <c r="Y4" s="61"/>
+      <c r="Z4" s="61"/>
+      <c r="AA4" s="61"/>
+      <c r="AB4" s="62"/>
+      <c r="AC4" s="62"/>
+      <c r="AD4" s="62"/>
+    </row>
+    <row r="5" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="63"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+      <c r="L5" s="65"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="65"/>
+      <c r="O5" s="65"/>
+      <c r="P5" s="65"/>
+      <c r="Q5" s="65"/>
+      <c r="R5" s="65"/>
+      <c r="S5" s="65"/>
+      <c r="T5" s="65"/>
+      <c r="U5" s="65"/>
+      <c r="V5" s="65"/>
+      <c r="W5" s="65"/>
+      <c r="X5" s="65"/>
+      <c r="Y5" s="65"/>
+      <c r="Z5" s="65"/>
+      <c r="AA5" s="65"/>
+      <c r="AB5" s="66"/>
+      <c r="AC5" s="63"/>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="145" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="130" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="148" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="149"/>
+      <c r="E6" s="149"/>
+      <c r="F6" s="149"/>
+      <c r="G6" s="149"/>
+      <c r="H6" s="149"/>
+      <c r="I6" s="149"/>
+      <c r="J6" s="149"/>
+      <c r="K6" s="149"/>
+      <c r="L6" s="149"/>
+      <c r="M6" s="149"/>
+      <c r="N6" s="149"/>
+      <c r="O6" s="149"/>
+      <c r="P6" s="149"/>
+      <c r="Q6" s="149"/>
+      <c r="R6" s="149"/>
+      <c r="S6" s="149"/>
+      <c r="T6" s="149"/>
+      <c r="U6" s="149"/>
+      <c r="V6" s="149"/>
+      <c r="W6" s="149"/>
+      <c r="X6" s="149"/>
+      <c r="Y6" s="149"/>
+      <c r="Z6" s="149"/>
+      <c r="AA6" s="150"/>
+      <c r="AB6" s="151" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC6" s="127" t="s">
+        <v>4</v>
+      </c>
+      <c r="AD6" s="130" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="146"/>
+      <c r="B7" s="131"/>
+      <c r="C7" s="135" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="136"/>
+      <c r="E7" s="136"/>
+      <c r="F7" s="136"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="138" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="139"/>
+      <c r="J7" s="139"/>
+      <c r="K7" s="139"/>
+      <c r="L7" s="154"/>
+      <c r="M7" s="135" t="s">
+        <v>71</v>
+      </c>
+      <c r="N7" s="136"/>
+      <c r="O7" s="136"/>
+      <c r="P7" s="136"/>
+      <c r="Q7" s="137"/>
+      <c r="R7" s="138" t="s">
+        <v>72</v>
+      </c>
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="135" t="s">
+        <v>73</v>
+      </c>
+      <c r="X7" s="136"/>
+      <c r="Y7" s="136"/>
+      <c r="Z7" s="136"/>
+      <c r="AA7" s="137"/>
+      <c r="AB7" s="152"/>
+      <c r="AC7" s="128"/>
+      <c r="AD7" s="131"/>
+    </row>
+    <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="146"/>
+      <c r="B8" s="131"/>
+      <c r="C8" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="143"/>
+      <c r="E8" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="134"/>
+      <c r="H8" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="143"/>
+      <c r="J8" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="134"/>
+      <c r="M8" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="N8" s="143"/>
+      <c r="O8" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q8" s="134"/>
+      <c r="R8" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="S8" s="143"/>
+      <c r="T8" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="U8" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="V8" s="134"/>
+      <c r="W8" s="142" t="s">
+        <v>6</v>
+      </c>
+      <c r="X8" s="143"/>
+      <c r="Y8" s="140" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z8" s="133" t="s">
+        <v>23</v>
+      </c>
+      <c r="AA8" s="134"/>
+      <c r="AB8" s="152"/>
+      <c r="AC8" s="128"/>
+      <c r="AD8" s="131"/>
+    </row>
+    <row r="9" spans="1:30" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="147"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="141"/>
+      <c r="F9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="141"/>
+      <c r="K9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O9" s="141"/>
+      <c r="P9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="R9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T9" s="141"/>
+      <c r="U9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y9" s="141"/>
+      <c r="Z9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA9" s="100" t="s">
+        <v>24</v>
+      </c>
+      <c r="AB9" s="153"/>
+      <c r="AC9" s="129"/>
+      <c r="AD9" s="132"/>
+    </row>
+    <row r="10" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="8"/>
+      <c r="G10" s="104"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="7"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="104"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="99"/>
+      <c r="P10" s="6"/>
+      <c r="Q10" s="104"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="10"/>
+      <c r="T10" s="99"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="104"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="99"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="104"/>
+      <c r="AB10" s="11"/>
+      <c r="AC10" s="12"/>
+      <c r="AD10" s="13"/>
+    </row>
+    <row r="11" spans="1:30" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="16"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="103"/>
+      <c r="G11" s="102"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="103"/>
+      <c r="L11" s="102"/>
+      <c r="M11" s="20"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="103"/>
+      <c r="Q11" s="102"/>
+      <c r="R11" s="20"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="21"/>
+      <c r="U11" s="103"/>
+      <c r="V11" s="102"/>
+      <c r="W11" s="20"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="21"/>
+      <c r="Z11" s="103"/>
+      <c r="AA11" s="102"/>
+      <c r="AB11" s="22"/>
+      <c r="AC11" s="23"/>
+      <c r="AD11" s="24"/>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A12" s="25">
+        <v>1</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="47"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+      <c r="L12" s="28"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="32"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="28"/>
+      <c r="R12" s="30"/>
+      <c r="S12" s="32"/>
+      <c r="T12" s="32"/>
+      <c r="U12" s="32"/>
+      <c r="V12" s="28"/>
+      <c r="W12" s="30"/>
+      <c r="X12" s="32"/>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="32"/>
+      <c r="AA12" s="28"/>
+      <c r="AB12" s="33"/>
+      <c r="AC12" s="34"/>
+      <c r="AD12" s="35"/>
+    </row>
+    <row r="13" spans="1:30" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+      <c r="C13" s="47" t="s">
+        <v>224</v>
+      </c>
+      <c r="D13" s="126" t="s">
+        <v>225</v>
+      </c>
+      <c r="E13" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="32"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="32"/>
+      <c r="K13" s="32"/>
+      <c r="L13" s="28"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="28"/>
+      <c r="R13" s="30"/>
+      <c r="S13" s="32"/>
+      <c r="T13" s="32"/>
+      <c r="U13" s="32"/>
+      <c r="V13" s="28"/>
+      <c r="W13" s="30"/>
+      <c r="X13" s="32"/>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="32"/>
+      <c r="AA13" s="28"/>
+      <c r="AB13" s="33"/>
+      <c r="AC13" s="34"/>
+      <c r="AD13" s="35"/>
+    </row>
+    <row r="14" spans="1:30" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="D14" s="126" t="s">
+        <v>227</v>
+      </c>
+      <c r="E14" s="42" t="s">
+        <v>228</v>
+      </c>
+      <c r="F14" s="32"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="31"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="28"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="32"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="28"/>
+      <c r="R14" s="30"/>
+      <c r="S14" s="32"/>
+      <c r="T14" s="32"/>
+      <c r="U14" s="32"/>
+      <c r="V14" s="28"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="32"/>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="32"/>
+      <c r="AA14" s="28"/>
+      <c r="AB14" s="33"/>
+      <c r="AC14" s="34"/>
+      <c r="AD14" s="35"/>
+    </row>
+    <row r="15" spans="1:30" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+      <c r="C15" s="47" t="s">
+        <v>229</v>
+      </c>
+      <c r="D15" s="126" t="s">
+        <v>227</v>
+      </c>
+      <c r="E15" s="42" t="s">
+        <v>230</v>
+      </c>
+      <c r="F15" s="32"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="32"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="28"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="31"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="28"/>
+      <c r="R15" s="30"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
+      <c r="U15" s="32"/>
+      <c r="V15" s="28"/>
+      <c r="W15" s="30"/>
+      <c r="X15" s="32"/>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="32"/>
+      <c r="AA15" s="28"/>
+      <c r="AB15" s="33"/>
+      <c r="AC15" s="34"/>
+      <c r="AD15" s="35"/>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+      <c r="C16" s="47" t="s">
+        <v>231</v>
+      </c>
+      <c r="D16" s="126" t="s">
+        <v>232</v>
+      </c>
+      <c r="E16" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="F16" s="42"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="31"/>
+      <c r="J16" s="32"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="28"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="28"/>
+      <c r="R16" s="30"/>
+      <c r="S16" s="32"/>
+      <c r="T16" s="32"/>
+      <c r="U16" s="32"/>
+      <c r="V16" s="28"/>
+      <c r="W16" s="30"/>
+      <c r="X16" s="32"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="28"/>
+      <c r="AB16" s="33"/>
+      <c r="AC16" s="34"/>
+      <c r="AD16" s="35"/>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+      <c r="C17" s="47"/>
+      <c r="D17" s="155"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="43" t="s">
+        <v>233</v>
+      </c>
+      <c r="I17" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="J17" s="32"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="31"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="32"/>
+      <c r="Q17" s="28"/>
+      <c r="R17" s="30"/>
+      <c r="S17" s="32"/>
+      <c r="T17" s="32"/>
+      <c r="U17" s="32"/>
+      <c r="V17" s="28"/>
+      <c r="W17" s="30"/>
+      <c r="X17" s="32"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="28"/>
+      <c r="AB17" s="33"/>
+      <c r="AC17" s="34"/>
+      <c r="AD17" s="35"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="47"/>
+      <c r="D18" s="155"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="43" t="s">
+        <v>234</v>
+      </c>
+      <c r="I18" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="J18" s="32"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="28"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="30"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
+      <c r="U18" s="32"/>
+      <c r="V18" s="28"/>
+      <c r="W18" s="30"/>
+      <c r="X18" s="32"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="33"/>
+      <c r="AC18" s="34"/>
+      <c r="AD18" s="35"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+      <c r="C19" s="47"/>
+      <c r="D19" s="155"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="43" t="s">
+        <v>235</v>
+      </c>
+      <c r="I19" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="31"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="30"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
+      <c r="U19" s="32"/>
+      <c r="V19" s="28"/>
+      <c r="W19" s="30"/>
+      <c r="X19" s="32"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="28"/>
+      <c r="AB19" s="33"/>
+      <c r="AC19" s="34"/>
+      <c r="AD19" s="35"/>
+    </row>
+    <row r="20" spans="1:30" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="155"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="43" t="s">
+        <v>236</v>
+      </c>
+      <c r="I20" s="126" t="s">
+        <v>237</v>
+      </c>
+      <c r="J20" s="32"/>
+      <c r="K20" s="32"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="31"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="32"/>
+      <c r="Q20" s="28"/>
+      <c r="R20" s="30"/>
+      <c r="S20" s="32"/>
+      <c r="T20" s="32"/>
+      <c r="U20" s="32"/>
+      <c r="V20" s="28"/>
+      <c r="W20" s="30"/>
+      <c r="X20" s="32"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="28"/>
+      <c r="AB20" s="33"/>
+      <c r="AC20" s="34"/>
+      <c r="AD20" s="35"/>
     </row>
     <row r="21" spans="1:30" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="36"/>

</xml_diff>